<commit_message>
fix: Suppression colonne obligatoire export MCCC
</commit_message>
<xml_diff>
--- a/public/modeles/Annexe_MCCC.xlsx
+++ b/public/modeles/Annexe_MCCC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1325EF0E-A657-994A-B6D8-C47A71E85B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C60273-1F8C-E542-976B-A1BA3BB84F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modele" sheetId="9" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
   <si>
     <t>ACCREDITATION 2024-2028</t>
   </si>
@@ -156,9 +156,6 @@
   </si>
   <si>
     <t>Type d'enseignement</t>
-  </si>
-  <si>
-    <t>Obligatoire / Optionnel</t>
   </si>
   <si>
     <t>Cours mutualisé
@@ -1055,6 +1052,72 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1073,72 +1136,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1147,12 +1150,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1578,10 +1575,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BA23"/>
+  <dimension ref="A1:AZ23"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1595,49 +1592,48 @@
     <col min="8" max="8" width="23" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" style="15" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" style="15" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" style="15" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" style="15" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" style="15" customWidth="1"/>
-    <col min="15" max="17" width="6.33203125" customWidth="1"/>
-    <col min="18" max="18" width="10.6640625" customWidth="1"/>
-    <col min="19" max="21" width="6.33203125" customWidth="1"/>
-    <col min="22" max="23" width="10" customWidth="1"/>
-    <col min="24" max="24" width="10.33203125" customWidth="1"/>
-    <col min="25" max="28" width="10.5" customWidth="1"/>
-    <col min="29" max="30" width="20.33203125" customWidth="1"/>
-    <col min="31" max="31" width="18" customWidth="1"/>
-    <col min="32" max="49" width="5.1640625" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" style="15" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" style="15" customWidth="1"/>
+    <col min="14" max="16" width="6.33203125" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" customWidth="1"/>
+    <col min="18" max="20" width="6.33203125" customWidth="1"/>
+    <col min="21" max="22" width="10" customWidth="1"/>
+    <col min="23" max="23" width="10.33203125" customWidth="1"/>
+    <col min="24" max="27" width="10.5" customWidth="1"/>
+    <col min="28" max="29" width="20.33203125" customWidth="1"/>
+    <col min="30" max="30" width="18" customWidth="1"/>
+    <col min="31" max="48" width="5.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:52" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="AI1" s="2"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
@@ -1655,70 +1651,67 @@
       <c r="AX1" s="2"/>
       <c r="AY1" s="2"/>
       <c r="AZ1" s="2"/>
-      <c r="BA1" s="2"/>
-    </row>
-    <row r="2" spans="1:53" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+    </row>
+    <row r="2" spans="1:52" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="79"/>
-    </row>
-    <row r="3" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="79" t="s">
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="73"/>
+      <c r="V2" s="73"/>
+      <c r="W2" s="73"/>
+      <c r="X2" s="73"/>
+    </row>
+    <row r="3" spans="1:52" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="79"/>
-      <c r="S3" s="79"/>
-      <c r="T3" s="79"/>
-      <c r="U3" s="79"/>
-      <c r="V3" s="79"/>
-      <c r="W3" s="79"/>
-      <c r="X3" s="79"/>
-      <c r="Y3" s="79"/>
-    </row>
-    <row r="4" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="73"/>
+      <c r="T3" s="73"/>
+      <c r="U3" s="73"/>
+      <c r="V3" s="73"/>
+      <c r="W3" s="73"/>
+      <c r="X3" s="73"/>
+    </row>
+    <row r="4" spans="1:52" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:52" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I5" s="27" t="s">
         <v>3</v>
       </c>
@@ -1731,12 +1724,11 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-    </row>
-    <row r="6" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:52" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="26"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -1753,11 +1745,11 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="2"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
+      <c r="U6" s="3"/>
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
@@ -1765,16 +1757,15 @@
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
-      <c r="AC6" s="3"/>
+      <c r="AE6" s="3"/>
       <c r="AF6" s="3"/>
       <c r="AG6" s="3"/>
       <c r="AH6" s="3"/>
       <c r="AI6" s="3"/>
       <c r="AJ6" s="3"/>
       <c r="AK6" s="3"/>
-      <c r="AL6" s="3"/>
-    </row>
-    <row r="7" spans="1:53" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:52" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1794,19 +1785,18 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
+      <c r="AE7" s="3"/>
       <c r="AF7" s="3"/>
       <c r="AG7" s="3"/>
       <c r="AH7" s="3"/>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="3"/>
       <c r="AK7" s="3"/>
-      <c r="AL7" s="3"/>
-    </row>
-    <row r="8" spans="1:53" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:52" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="J8" s="8"/>
@@ -1828,7 +1818,7 @@
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
+      <c r="AE8" s="3"/>
       <c r="AF8" s="3"/>
       <c r="AG8" s="3"/>
       <c r="AH8" s="3"/>
@@ -1843,9 +1833,8 @@
       <c r="AQ8" s="3"/>
       <c r="AR8" s="3"/>
       <c r="AS8" s="3"/>
-      <c r="AT8" s="3"/>
-    </row>
-    <row r="9" spans="1:53" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:52" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="C9" s="6"/>
       <c r="D9" s="7" t="s">
@@ -1863,11 +1852,11 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
+      <c r="U9" s="4"/>
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
@@ -1875,18 +1864,16 @@
       <c r="Z9" s="4"/>
       <c r="AA9" s="4"/>
       <c r="AB9" s="4"/>
-      <c r="AC9" s="4"/>
-    </row>
-    <row r="10" spans="1:53" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:52" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="N10" s="17"/>
-    </row>
-    <row r="11" spans="1:53" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M10" s="17"/>
+    </row>
+    <row r="11" spans="1:52" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="6"/>
       <c r="D11" s="7" t="s">
         <v>14</v>
@@ -1898,19 +1885,17 @@
         <v>16</v>
       </c>
       <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="N11" s="16"/>
-    </row>
-    <row r="12" spans="1:53" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M11" s="16"/>
+    </row>
+    <row r="12" spans="1:52" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="I12" s="28"/>
       <c r="J12" s="10"/>
       <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="N12" s="16"/>
-    </row>
-    <row r="13" spans="1:53" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M12" s="16"/>
+    </row>
+    <row r="13" spans="1:52" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="6"/>
       <c r="D13" s="7" t="s">
         <v>17</v>
@@ -1922,115 +1907,111 @@
         <v>19</v>
       </c>
       <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="N13" s="16"/>
-    </row>
-    <row r="14" spans="1:53" ht="11" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
+      <c r="M13" s="16"/>
+    </row>
+    <row r="14" spans="1:52" ht="11" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="18"/>
-    </row>
-    <row r="15" spans="1:53" s="1" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="67" t="s">
+      <c r="L14" s="5"/>
+      <c r="M14" s="18"/>
+    </row>
+    <row r="15" spans="1:52" s="1" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="71"/>
-      <c r="D15" s="74" t="s">
+      <c r="C15" s="64"/>
+      <c r="D15" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="74"/>
-      <c r="I15" s="74"/>
-      <c r="J15" s="74"/>
-      <c r="K15" s="74"/>
-      <c r="L15" s="74"/>
-      <c r="M15" s="74"/>
-      <c r="N15" s="75"/>
-      <c r="O15" s="61" t="s">
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="68"/>
+      <c r="N15" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="P15" s="63"/>
-      <c r="Q15" s="63"/>
-      <c r="R15" s="63"/>
-      <c r="S15" s="63"/>
-      <c r="T15" s="63"/>
-      <c r="U15" s="63"/>
-      <c r="V15" s="63"/>
-      <c r="W15" s="63"/>
-      <c r="X15" s="62"/>
-      <c r="Y15" s="61" t="s">
+      <c r="O15" s="56"/>
+      <c r="P15" s="56"/>
+      <c r="Q15" s="56"/>
+      <c r="R15" s="56"/>
+      <c r="S15" s="56"/>
+      <c r="T15" s="56"/>
+      <c r="U15" s="56"/>
+      <c r="V15" s="56"/>
+      <c r="W15" s="71"/>
+      <c r="X15" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="Z15" s="63"/>
-      <c r="AA15" s="63"/>
-      <c r="AB15" s="63"/>
-      <c r="AC15" s="29"/>
-      <c r="AD15" s="64" t="s">
+      <c r="Y15" s="56"/>
+      <c r="Z15" s="56"/>
+      <c r="AA15" s="56"/>
+      <c r="AB15" s="29"/>
+      <c r="AC15" s="57" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="68"/>
-      <c r="B16" s="72"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="76"/>
-      <c r="L16" s="76"/>
-      <c r="M16" s="76"/>
-      <c r="N16" s="77"/>
-      <c r="O16" s="61" t="s">
+    <row r="16" spans="1:52" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="61"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="69"/>
+      <c r="M16" s="70"/>
+      <c r="N16" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="P16" s="63"/>
-      <c r="Q16" s="63"/>
-      <c r="R16" s="62"/>
-      <c r="S16" s="61" t="s">
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="71"/>
+      <c r="R16" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="T16" s="63"/>
-      <c r="U16" s="63"/>
-      <c r="V16" s="62"/>
-      <c r="W16" s="86" t="s">
-        <v>61</v>
-      </c>
-      <c r="X16" s="64" t="s">
+      <c r="S16" s="56"/>
+      <c r="T16" s="56"/>
+      <c r="U16" s="71"/>
+      <c r="V16" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="W16" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="Y16" s="61" t="s">
+      <c r="X16" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="Z16" s="62"/>
-      <c r="AA16" s="61" t="s">
+      <c r="Y16" s="71"/>
+      <c r="Z16" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="AB16" s="62"/>
-      <c r="AC16" s="21" t="s">
+      <c r="AA16" s="71"/>
+      <c r="AB16" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="AD16" s="65"/>
-    </row>
-    <row r="17" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="69"/>
+      <c r="AC16" s="58"/>
+    </row>
+    <row r="17" spans="1:29" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="62"/>
       <c r="B17" s="22" t="s">
         <v>32</v>
       </c>
@@ -2056,66 +2037,63 @@
       <c r="J17" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="K17" s="21" t="s">
+      <c r="K17" s="19" t="s">
         <v>40</v>
       </c>
       <c r="L17" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="M17" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="M17" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="N17" s="46" t="s">
+      <c r="N17" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="O17" s="20" t="s">
+      <c r="O17" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="P17" s="24" t="s">
+      <c r="P17" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="Q17" s="23" t="s">
+      <c r="Q17" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="R17" s="14" t="s">
+      <c r="R17" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="S17" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="T17" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U17" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="S17" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="T17" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="U17" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="V17" s="14" t="s">
+      <c r="V17" s="76"/>
+      <c r="W17" s="74"/>
+      <c r="X17" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="W17" s="87"/>
-      <c r="X17" s="82"/>
-      <c r="Y17" s="13" t="s">
+      <c r="Y17" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="Z17" s="25" t="s">
+      <c r="Z17" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA17" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="AA17" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB17" s="25" t="s">
+      <c r="AB17" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="AC17" s="30" t="s">
+      <c r="AC17" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
         <v>51</v>
-      </c>
-      <c r="AD17" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
-        <v>52</v>
       </c>
       <c r="B18" s="33">
         <v>11</v>
@@ -2130,40 +2108,40 @@
       <c r="H18" s="32"/>
       <c r="I18" s="38"/>
       <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="41"/>
-      <c r="Q18" s="34"/>
-      <c r="R18" s="39"/>
-      <c r="S18" s="40"/>
-      <c r="T18" s="41"/>
-      <c r="U18" s="34"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="39"/>
+      <c r="R18" s="40"/>
+      <c r="S18" s="41"/>
+      <c r="T18" s="34"/>
+      <c r="U18" s="37"/>
       <c r="V18" s="37"/>
       <c r="W18" s="37"/>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="40"/>
-      <c r="Z18" s="42"/>
-      <c r="AA18" s="40"/>
-      <c r="AB18" s="34"/>
-      <c r="AC18" s="47" t="s">
+      <c r="X18" s="40"/>
+      <c r="Y18" s="42"/>
+      <c r="Z18" s="40"/>
+      <c r="AA18" s="34"/>
+      <c r="AB18" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC18" s="37"/>
+    </row>
+    <row r="19" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="AD18" s="37"/>
-    </row>
-    <row r="19" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
-        <v>54</v>
       </c>
       <c r="C19"/>
       <c r="H19" s="15"/>
-      <c r="M19" s="80" t="s">
-        <v>62</v>
-      </c>
-      <c r="N19" s="81"/>
-      <c r="O19" s="43"/>
+      <c r="L19" s="83" t="s">
+        <v>61</v>
+      </c>
+      <c r="M19" s="84"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="44"/>
       <c r="P19" s="44"/>
       <c r="Q19" s="44"/>
       <c r="R19" s="44"/>
@@ -2171,102 +2149,101 @@
       <c r="T19" s="44"/>
       <c r="U19" s="44"/>
       <c r="V19" s="44"/>
-      <c r="W19" s="44"/>
-      <c r="X19" s="45"/>
-    </row>
-    <row r="20" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="W19" s="45"/>
+    </row>
+    <row r="20" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="C20"/>
       <c r="H20" s="15"/>
-      <c r="M20" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="N20" s="55"/>
-      <c r="O20" s="56"/>
-      <c r="P20" s="57"/>
-      <c r="Q20" s="57"/>
-      <c r="R20" s="57"/>
-      <c r="S20" s="57"/>
-      <c r="T20" s="57"/>
-      <c r="U20" s="57"/>
-      <c r="V20" s="58"/>
-      <c r="W20" s="50"/>
-      <c r="X20" s="51"/>
-    </row>
-    <row r="21" spans="1:30" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L20" s="77" t="s">
+        <v>62</v>
+      </c>
+      <c r="M20" s="77"/>
+      <c r="N20" s="78"/>
+      <c r="O20" s="79"/>
+      <c r="P20" s="79"/>
+      <c r="Q20" s="79"/>
+      <c r="R20" s="79"/>
+      <c r="S20" s="79"/>
+      <c r="T20" s="79"/>
+      <c r="U20" s="80"/>
+      <c r="V20" s="50"/>
+      <c r="W20" s="51"/>
+    </row>
+    <row r="21" spans="1:29" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="C21" s="52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E21" s="53"/>
       <c r="H21" s="15"/>
-      <c r="M21" s="55" t="s">
-        <v>59</v>
-      </c>
-      <c r="N21" s="55"/>
-      <c r="O21" s="83"/>
-      <c r="P21" s="84"/>
-      <c r="Q21" s="84"/>
-      <c r="R21" s="84"/>
-      <c r="S21" s="84"/>
-      <c r="T21" s="84"/>
-      <c r="U21" s="84"/>
-      <c r="V21" s="84"/>
-      <c r="W21" s="84"/>
-      <c r="X21" s="85"/>
-    </row>
-    <row r="22" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L21" s="77" t="s">
+        <v>58</v>
+      </c>
+      <c r="M21" s="77"/>
+      <c r="N21" s="85"/>
+      <c r="O21" s="86"/>
+      <c r="P21" s="86"/>
+      <c r="Q21" s="86"/>
+      <c r="R21" s="86"/>
+      <c r="S21" s="86"/>
+      <c r="T21" s="86"/>
+      <c r="U21" s="86"/>
+      <c r="V21" s="86"/>
+      <c r="W21" s="87"/>
+    </row>
+    <row r="22" spans="1:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="C22" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" s="54"/>
       <c r="H22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22"/>
-      <c r="AB22" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC22" s="59"/>
-      <c r="AD22" s="60"/>
-    </row>
-    <row r="23" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="15"/>
+      <c r="M22"/>
+      <c r="AA22" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB22" s="81"/>
+      <c r="AC22" s="82"/>
+    </row>
+    <row r="23" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="C23"/>
       <c r="H23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23"/>
-      <c r="AB23" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC23" s="48"/>
-      <c r="AD23" s="49"/>
+      <c r="L23" s="15"/>
+      <c r="M23"/>
+      <c r="AA23" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB23" s="48"/>
+      <c r="AC23" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="Y15:AB15"/>
-    <mergeCell ref="AD15:AD16"/>
-    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N20:U20"/>
+    <mergeCell ref="AB22:AC22"/>
+    <mergeCell ref="X16:Y16"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N21:W21"/>
+    <mergeCell ref="X15:AA15"/>
+    <mergeCell ref="AC15:AC16"/>
+    <mergeCell ref="A1:X1"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:C16"/>
-    <mergeCell ref="D15:N16"/>
-    <mergeCell ref="O15:X15"/>
+    <mergeCell ref="D15:M16"/>
+    <mergeCell ref="N15:W15"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="A2:Y2"/>
-    <mergeCell ref="A3:Y3"/>
-    <mergeCell ref="O16:R16"/>
-    <mergeCell ref="X16:X17"/>
-    <mergeCell ref="S16:V16"/>
+    <mergeCell ref="A2:X2"/>
+    <mergeCell ref="A3:X3"/>
+    <mergeCell ref="N16:Q16"/>
     <mergeCell ref="W16:W17"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="O20:V20"/>
-    <mergeCell ref="AC22:AD22"/>
-    <mergeCell ref="Y16:Z16"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="O21:X21"/>
+    <mergeCell ref="R16:U16"/>
+    <mergeCell ref="V16:V17"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="45" orientation="landscape" r:id="rId1"/>
@@ -2278,40 +2255,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA697C32-3881-B543-B376-9C8F58E5E06A}">
   <dimension ref="A1:BA13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:53" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
@@ -2332,62 +2309,62 @@
       <c r="BA1" s="2"/>
     </row>
     <row r="2" spans="1:53" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="79"/>
+      <c r="A2" s="73" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="73"/>
+      <c r="V2" s="73"/>
+      <c r="W2" s="73"/>
+      <c r="X2" s="73"/>
+      <c r="Y2" s="73"/>
     </row>
     <row r="3" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="79"/>
-      <c r="S3" s="79"/>
-      <c r="T3" s="79"/>
-      <c r="U3" s="79"/>
-      <c r="V3" s="79"/>
-      <c r="W3" s="79"/>
-      <c r="X3" s="79"/>
-      <c r="Y3" s="79"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="73"/>
+      <c r="T3" s="73"/>
+      <c r="U3" s="73"/>
+      <c r="V3" s="73"/>
+      <c r="W3" s="73"/>
+      <c r="X3" s="73"/>
+      <c r="Y3" s="73"/>
     </row>
     <row r="4" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
@@ -2610,26 +2587,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B7BBE98651F7A43AC7BF2F06836443C" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b51c7281b06024c9ff887df9fe3bb465">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8103b6e4-b1cc-417b-af38-f980b3f4bdef" xmlns:ns3="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c056a6abdadb071051b2c083c327215c" ns2:_="" ns3:_="">
     <xsd:import namespace="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
@@ -2846,10 +2803,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E02BC65-B354-4988-8893-F98AC7F212AA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
+    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2866,20 +2854,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E02BC65-B354-4988-8893-F98AC7F212AA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
-    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: Typo modèle MCCC
</commit_message>
<xml_diff>
--- a/public/modeles/Annexe_MCCC.xlsx
+++ b/public/modeles/Annexe_MCCC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C60273-1F8C-E542-976B-A1BA3BB84F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6326CBC6-AAB5-DB40-A42D-96EDDAB2B49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modele" sheetId="9" r:id="rId1"/>
@@ -198,9 +198,6 @@
     <t>épreuve 1 (%), épreuve 2 (%), épreuve 3 (%), etc.</t>
   </si>
   <si>
-    <t>* dans le cas du Cci, la seconde chance se traduit par la non prise en compte dans le calucl de la note finale de la moins bonne des notes de Cci obtenus dans l'enseignement concerné,</t>
-  </si>
-  <si>
     <t xml:space="preserve">Responsable de mention : </t>
   </si>
   <si>
@@ -241,6 +238,9 @@
   </si>
   <si>
     <t>RÉFÉRENTIEL DE COMPÉTENCES</t>
+  </si>
+  <si>
+    <t>* dans le cas du Cci, la seconde chance se traduit par la non prise en compte dans le calcul de la note finale de la moins bonne des notes de Cci obtenues dans l'enseignement concerné.</t>
   </si>
 </sst>
 </file>
@@ -1052,9 +1052,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1100,9 +1136,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1117,39 +1150,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1577,8 +1577,8 @@
   </sheetPr>
   <dimension ref="A1:AZ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1600,39 +1600,42 @@
     <col min="18" max="20" width="6.33203125" customWidth="1"/>
     <col min="21" max="22" width="10" customWidth="1"/>
     <col min="23" max="23" width="10.33203125" customWidth="1"/>
-    <col min="24" max="27" width="10.5" customWidth="1"/>
+    <col min="24" max="24" width="10.5" customWidth="1"/>
+    <col min="25" max="25" width="12.5" customWidth="1"/>
+    <col min="26" max="26" width="10.5" customWidth="1"/>
+    <col min="27" max="27" width="12.6640625" customWidth="1"/>
     <col min="28" max="29" width="20.33203125" customWidth="1"/>
     <col min="30" max="30" width="18" customWidth="1"/>
     <col min="31" max="48" width="5.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="71"/>
+      <c r="X1" s="71"/>
       <c r="AI1" s="2"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
@@ -1653,60 +1656,60 @@
       <c r="AZ1" s="2"/>
     </row>
     <row r="2" spans="1:52" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="73"/>
-      <c r="W2" s="73"/>
-      <c r="X2" s="73"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="84"/>
+      <c r="T2" s="84"/>
+      <c r="U2" s="84"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="84"/>
+      <c r="X2" s="84"/>
     </row>
     <row r="3" spans="1:52" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="73"/>
-      <c r="T3" s="73"/>
-      <c r="U3" s="73"/>
-      <c r="V3" s="73"/>
-      <c r="W3" s="73"/>
-      <c r="X3" s="73"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="84"/>
+      <c r="T3" s="84"/>
+      <c r="U3" s="84"/>
+      <c r="V3" s="84"/>
+      <c r="W3" s="84"/>
+      <c r="X3" s="84"/>
     </row>
     <row r="4" spans="1:52" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G4" s="2"/>
@@ -1910,10 +1913,10 @@
       <c r="M13" s="16"/>
     </row>
     <row r="14" spans="1:52" ht="11" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="83"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="18"/>
@@ -1923,95 +1926,95 @@
       <c r="M14" s="18"/>
     </row>
     <row r="15" spans="1:52" s="1" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="64"/>
-      <c r="D15" s="67" t="s">
+      <c r="C15" s="76"/>
+      <c r="D15" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="68"/>
-      <c r="N15" s="55" t="s">
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="80"/>
+      <c r="N15" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="56"/>
-      <c r="P15" s="56"/>
-      <c r="Q15" s="56"/>
-      <c r="R15" s="56"/>
-      <c r="S15" s="56"/>
-      <c r="T15" s="56"/>
-      <c r="U15" s="56"/>
-      <c r="V15" s="56"/>
-      <c r="W15" s="71"/>
-      <c r="X15" s="55" t="s">
+      <c r="O15" s="68"/>
+      <c r="P15" s="68"/>
+      <c r="Q15" s="68"/>
+      <c r="R15" s="68"/>
+      <c r="S15" s="68"/>
+      <c r="T15" s="68"/>
+      <c r="U15" s="68"/>
+      <c r="V15" s="68"/>
+      <c r="W15" s="62"/>
+      <c r="X15" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="Y15" s="56"/>
-      <c r="Z15" s="56"/>
-      <c r="AA15" s="56"/>
+      <c r="Y15" s="68"/>
+      <c r="Z15" s="68"/>
+      <c r="AA15" s="68"/>
       <c r="AB15" s="29"/>
-      <c r="AC15" s="57" t="s">
+      <c r="AC15" s="69" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:52" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="61"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="69"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="70"/>
-      <c r="N16" s="55" t="s">
+      <c r="A16" s="73"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="81"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="81"/>
+      <c r="M16" s="82"/>
+      <c r="N16" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="O16" s="56"/>
-      <c r="P16" s="56"/>
-      <c r="Q16" s="71"/>
-      <c r="R16" s="55" t="s">
+      <c r="O16" s="68"/>
+      <c r="P16" s="68"/>
+      <c r="Q16" s="62"/>
+      <c r="R16" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="S16" s="56"/>
-      <c r="T16" s="56"/>
-      <c r="U16" s="71"/>
-      <c r="V16" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="W16" s="57" t="s">
+      <c r="S16" s="68"/>
+      <c r="T16" s="68"/>
+      <c r="U16" s="62"/>
+      <c r="V16" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="W16" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="X16" s="55" t="s">
+      <c r="X16" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="Y16" s="71"/>
-      <c r="Z16" s="55" t="s">
+      <c r="Y16" s="62"/>
+      <c r="Z16" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="AA16" s="71"/>
+      <c r="AA16" s="62"/>
       <c r="AB16" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="AC16" s="58"/>
+      <c r="AC16" s="70"/>
     </row>
     <row r="17" spans="1:29" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="62"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="22" t="s">
         <v>32</v>
       </c>
@@ -2041,7 +2044,7 @@
         <v>40</v>
       </c>
       <c r="L17" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M17" s="46" t="s">
         <v>41</v>
@@ -2070,8 +2073,8 @@
       <c r="U17" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="V17" s="76"/>
-      <c r="W17" s="74"/>
+      <c r="V17" s="87"/>
+      <c r="W17" s="85"/>
       <c r="X17" s="13" t="s">
         <v>47</v>
       </c>
@@ -2132,14 +2135,14 @@
     </row>
     <row r="19" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="31" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C19"/>
       <c r="H19" s="15"/>
-      <c r="L19" s="83" t="s">
-        <v>61</v>
-      </c>
-      <c r="M19" s="84"/>
+      <c r="L19" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="M19" s="64"/>
       <c r="N19" s="43"/>
       <c r="O19" s="44"/>
       <c r="P19" s="44"/>
@@ -2155,57 +2158,57 @@
       <c r="A20" s="5"/>
       <c r="C20"/>
       <c r="H20" s="15"/>
-      <c r="L20" s="77" t="s">
-        <v>62</v>
-      </c>
-      <c r="M20" s="77"/>
-      <c r="N20" s="78"/>
-      <c r="O20" s="79"/>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="79"/>
-      <c r="R20" s="79"/>
-      <c r="S20" s="79"/>
-      <c r="T20" s="79"/>
-      <c r="U20" s="80"/>
+      <c r="L20" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="M20" s="55"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="57"/>
+      <c r="P20" s="57"/>
+      <c r="Q20" s="57"/>
+      <c r="R20" s="57"/>
+      <c r="S20" s="57"/>
+      <c r="T20" s="57"/>
+      <c r="U20" s="58"/>
       <c r="V20" s="50"/>
       <c r="W20" s="51"/>
     </row>
     <row r="21" spans="1:29" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="C21" s="52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E21" s="53"/>
       <c r="H21" s="15"/>
-      <c r="L21" s="77" t="s">
-        <v>58</v>
-      </c>
-      <c r="M21" s="77"/>
-      <c r="N21" s="85"/>
-      <c r="O21" s="86"/>
-      <c r="P21" s="86"/>
-      <c r="Q21" s="86"/>
-      <c r="R21" s="86"/>
-      <c r="S21" s="86"/>
-      <c r="T21" s="86"/>
-      <c r="U21" s="86"/>
-      <c r="V21" s="86"/>
-      <c r="W21" s="87"/>
+      <c r="L21" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="M21" s="55"/>
+      <c r="N21" s="65"/>
+      <c r="O21" s="66"/>
+      <c r="P21" s="66"/>
+      <c r="Q21" s="66"/>
+      <c r="R21" s="66"/>
+      <c r="S21" s="66"/>
+      <c r="T21" s="66"/>
+      <c r="U21" s="66"/>
+      <c r="V21" s="66"/>
+      <c r="W21" s="67"/>
     </row>
     <row r="22" spans="1:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="C22" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" s="54"/>
       <c r="H22" s="15"/>
       <c r="L22" s="15"/>
       <c r="M22"/>
       <c r="AA22" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB22" s="81"/>
-      <c r="AC22" s="82"/>
+        <v>54</v>
+      </c>
+      <c r="AB22" s="59"/>
+      <c r="AC22" s="60"/>
     </row>
     <row r="23" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
@@ -2214,21 +2217,13 @@
       <c r="L23" s="15"/>
       <c r="M23"/>
       <c r="AA23" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB23" s="48"/>
       <c r="AC23" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N20:U20"/>
-    <mergeCell ref="AB22:AC22"/>
-    <mergeCell ref="X16:Y16"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="N21:W21"/>
     <mergeCell ref="X15:AA15"/>
     <mergeCell ref="AC15:AC16"/>
     <mergeCell ref="A1:X1"/>
@@ -2244,6 +2239,14 @@
     <mergeCell ref="W16:W17"/>
     <mergeCell ref="R16:U16"/>
     <mergeCell ref="V16:V17"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N20:U20"/>
+    <mergeCell ref="AB22:AC22"/>
+    <mergeCell ref="X16:Y16"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N21:W21"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="45" orientation="landscape" r:id="rId1"/>
@@ -2262,33 +2265,33 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:53" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="59"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="71"/>
+      <c r="X1" s="71"/>
+      <c r="Y1" s="71"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
@@ -2309,62 +2312,62 @@
       <c r="BA1" s="2"/>
     </row>
     <row r="2" spans="1:53" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="73" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="73"/>
-      <c r="W2" s="73"/>
-      <c r="X2" s="73"/>
-      <c r="Y2" s="73"/>
+      <c r="A2" s="84" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="84"/>
+      <c r="T2" s="84"/>
+      <c r="U2" s="84"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="84"/>
+      <c r="X2" s="84"/>
+      <c r="Y2" s="84"/>
     </row>
     <row r="3" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="73"/>
-      <c r="T3" s="73"/>
-      <c r="U3" s="73"/>
-      <c r="V3" s="73"/>
-      <c r="W3" s="73"/>
-      <c r="X3" s="73"/>
-      <c r="Y3" s="73"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="84"/>
+      <c r="T3" s="84"/>
+      <c r="U3" s="84"/>
+      <c r="V3" s="84"/>
+      <c r="W3" s="84"/>
+      <c r="X3" s="84"/>
+      <c r="Y3" s="84"/>
     </row>
     <row r="4" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
@@ -2587,6 +2590,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B7BBE98651F7A43AC7BF2F06836443C" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b51c7281b06024c9ff887df9fe3bb465">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8103b6e4-b1cc-417b-af38-f980b3f4bdef" xmlns:ns3="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c056a6abdadb071051b2c083c327215c" ns2:_="" ns3:_="">
     <xsd:import namespace="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
@@ -2803,27 +2826,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
+    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E02BC65-B354-4988-8893-F98AC7F212AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2840,23 +2862,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
-    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: modele Excel export MCCC
</commit_message>
<xml_diff>
--- a/public/modeles/Annexe_MCCC.xlsx
+++ b/public/modeles/Annexe_MCCC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6326CBC6-AAB5-DB40-A42D-96EDDAB2B49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8794AC-A452-A341-8F5D-A0176C66A238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -367,7 +367,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -810,17 +810,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -900,13 +889,31 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -988,14 +995,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1039,47 +1040,134 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1091,65 +1179,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1240,8 +1274,8 @@
       <xdr:rowOff>17318</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>288694</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2066694</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>81900</xdr:rowOff>
     </xdr:to>
@@ -1575,10 +1609,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AZ23"/>
+  <dimension ref="A1:AK23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1587,8 +1621,9 @@
     <col min="2" max="2" width="8.6640625" style="5" customWidth="1"/>
     <col min="3" max="3" width="41.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.83203125" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="50.6640625" customWidth="1"/>
+    <col min="5" max="5" width="50.83203125" customWidth="1"/>
+    <col min="6" max="6" width="50.6640625" customWidth="1"/>
+    <col min="7" max="7" width="36.33203125" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" style="15" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" style="15" customWidth="1"/>
@@ -1605,124 +1640,115 @@
     <col min="26" max="26" width="10.5" customWidth="1"/>
     <col min="27" max="27" width="12.6640625" customWidth="1"/>
     <col min="28" max="29" width="20.33203125" customWidth="1"/>
-    <col min="30" max="30" width="18" customWidth="1"/>
-    <col min="31" max="48" width="5.1640625" customWidth="1"/>
+    <col min="30" max="33" width="5.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:37" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="S1" s="71"/>
-      <c r="T1" s="71"/>
-      <c r="U1" s="71"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="71"/>
-      <c r="X1" s="71"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
       <c r="AI1" s="2"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
-      <c r="AL1" s="2"/>
-      <c r="AM1" s="2"/>
-      <c r="AN1" s="2"/>
-      <c r="AO1" s="2"/>
-      <c r="AP1" s="2"/>
-      <c r="AQ1" s="2"/>
-      <c r="AR1" s="2"/>
-      <c r="AS1" s="2"/>
-      <c r="AT1" s="2"/>
-      <c r="AU1" s="2"/>
-      <c r="AV1" s="2"/>
-      <c r="AW1" s="2"/>
-      <c r="AX1" s="2"/>
-      <c r="AY1" s="2"/>
-      <c r="AZ1" s="2"/>
-    </row>
-    <row r="2" spans="1:52" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="84" t="s">
+    </row>
+    <row r="2" spans="1:37" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="84"/>
-      <c r="R2" s="84"/>
-      <c r="S2" s="84"/>
-      <c r="T2" s="84"/>
-      <c r="U2" s="84"/>
-      <c r="V2" s="84"/>
-      <c r="W2" s="84"/>
-      <c r="X2" s="84"/>
-    </row>
-    <row r="3" spans="1:52" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="84" t="s">
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="79"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="79"/>
+      <c r="W2" s="79"/>
+      <c r="X2" s="79"/>
+    </row>
+    <row r="3" spans="1:37" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84"/>
-      <c r="N3" s="84"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="84"/>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="84"/>
-      <c r="S3" s="84"/>
-      <c r="T3" s="84"/>
-      <c r="U3" s="84"/>
-      <c r="V3" s="84"/>
-      <c r="W3" s="84"/>
-      <c r="X3" s="84"/>
-    </row>
-    <row r="4" spans="1:52" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="79"/>
+      <c r="Q3" s="79"/>
+      <c r="R3" s="79"/>
+      <c r="S3" s="79"/>
+      <c r="T3" s="79"/>
+      <c r="U3" s="79"/>
+      <c r="V3" s="79"/>
+      <c r="W3" s="79"/>
+      <c r="X3" s="79"/>
+    </row>
+    <row r="4" spans="1:37" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:52" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I5" s="27" t="s">
+    <row r="5" spans="1:37" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G5" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="K5" s="95"/>
+      <c r="L5" s="95"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1731,19 +1757,21 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:52" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="26"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="I6" s="27" t="s">
+      <c r="G6" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="H6" s="83"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="95"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -1760,30 +1788,27 @@
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="3"/>
-      <c r="AI6" s="3"/>
-      <c r="AJ6" s="3"/>
-      <c r="AK6" s="3"/>
-    </row>
-    <row r="7" spans="1:52" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    </row>
+    <row r="7" spans="1:37" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="8"/>
+      <c r="C7" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="F7" s="95"/>
+      <c r="G7" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="H7" s="83"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="95"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1791,18 +1816,15 @@
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
-      <c r="AE7" s="3"/>
-      <c r="AF7" s="3"/>
-      <c r="AG7" s="3"/>
-      <c r="AH7" s="3"/>
-      <c r="AI7" s="3"/>
-      <c r="AJ7" s="3"/>
-      <c r="AK7" s="3"/>
-    </row>
-    <row r="8" spans="1:52" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="8"/>
+    </row>
+    <row r="8" spans="1:37" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="7"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1821,36 +1843,25 @@
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
-      <c r="AE8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
-      <c r="AI8" s="3"/>
-      <c r="AJ8" s="3"/>
-      <c r="AK8" s="3"/>
-      <c r="AL8" s="3"/>
-      <c r="AM8" s="3"/>
-      <c r="AN8" s="3"/>
-      <c r="AO8" s="3"/>
-      <c r="AP8" s="3"/>
-      <c r="AQ8" s="3"/>
-      <c r="AR8" s="3"/>
-      <c r="AS8" s="3"/>
-    </row>
-    <row r="9" spans="1:52" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD8" s="3"/>
+    </row>
+    <row r="9" spans="1:37" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6"/>
+      <c r="E9" s="96" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="F9" s="95"/>
+      <c r="G9" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="H9" s="83"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="K9" s="95"/>
+      <c r="L9" s="95"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -1868,55 +1879,71 @@
       <c r="AA9" s="4"/>
       <c r="AB9" s="4"/>
     </row>
-    <row r="10" spans="1:52" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-      <c r="K10" s="17"/>
+    <row r="10" spans="1:37" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="9"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="51"/>
       <c r="M10" s="17"/>
     </row>
-    <row r="11" spans="1:52" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="6"/>
-      <c r="D11" s="7" t="s">
+    <row r="11" spans="1:37" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="6"/>
+      <c r="E11" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="F11" s="95"/>
+      <c r="G11" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="H11" s="83"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="16"/>
+      <c r="K11" s="95"/>
+      <c r="L11" s="95"/>
       <c r="M11" s="16"/>
     </row>
-    <row r="12" spans="1:52" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="7"/>
+    <row r="12" spans="1:37" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
       <c r="I12" s="28"/>
-      <c r="J12" s="10"/>
+      <c r="J12" s="53"/>
       <c r="K12" s="16"/>
+      <c r="L12" s="51"/>
       <c r="M12" s="16"/>
     </row>
-    <row r="13" spans="1:52" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="6"/>
-      <c r="D13" s="7" t="s">
+    <row r="13" spans="1:37" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D13" s="6"/>
+      <c r="E13" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="F13" s="95"/>
+      <c r="G13" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="H13" s="83"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="16"/>
+      <c r="K13" s="95"/>
+      <c r="L13" s="95"/>
       <c r="M13" s="16"/>
     </row>
-    <row r="14" spans="1:52" ht="11" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="83"/>
-      <c r="D14" s="83"/>
-      <c r="E14" s="83"/>
-      <c r="F14" s="83"/>
+    <row r="14" spans="1:37" ht="11" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="18"/>
@@ -1925,96 +1952,96 @@
       <c r="L14" s="5"/>
       <c r="M14" s="18"/>
     </row>
-    <row r="15" spans="1:52" s="1" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="72" t="s">
+    <row r="15" spans="1:37" s="1" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="76"/>
-      <c r="D15" s="79" t="s">
+      <c r="C15" s="71"/>
+      <c r="D15" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="79"/>
-      <c r="F15" s="79"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="79"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="79"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="80"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="74"/>
+      <c r="L15" s="74"/>
+      <c r="M15" s="75"/>
       <c r="N15" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="68"/>
-      <c r="P15" s="68"/>
-      <c r="Q15" s="68"/>
-      <c r="R15" s="68"/>
-      <c r="S15" s="68"/>
-      <c r="T15" s="68"/>
-      <c r="U15" s="68"/>
-      <c r="V15" s="68"/>
-      <c r="W15" s="62"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="62"/>
+      <c r="Q15" s="62"/>
+      <c r="R15" s="62"/>
+      <c r="S15" s="62"/>
+      <c r="T15" s="62"/>
+      <c r="U15" s="62"/>
+      <c r="V15" s="62"/>
+      <c r="W15" s="63"/>
       <c r="X15" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="Y15" s="68"/>
-      <c r="Z15" s="68"/>
-      <c r="AA15" s="68"/>
-      <c r="AB15" s="29"/>
-      <c r="AC15" s="69" t="s">
+      <c r="Y15" s="62"/>
+      <c r="Z15" s="62"/>
+      <c r="AA15" s="62"/>
+      <c r="AB15" s="63"/>
+      <c r="AC15" s="64" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:52" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="73"/>
-      <c r="B16" s="77"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="81"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="81"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="81"/>
-      <c r="L16" s="81"/>
-      <c r="M16" s="82"/>
+    <row r="16" spans="1:37" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="68"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
+      <c r="M16" s="77"/>
       <c r="N16" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="O16" s="68"/>
-      <c r="P16" s="68"/>
-      <c r="Q16" s="62"/>
+      <c r="O16" s="62"/>
+      <c r="P16" s="62"/>
+      <c r="Q16" s="63"/>
       <c r="R16" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="S16" s="68"/>
-      <c r="T16" s="68"/>
-      <c r="U16" s="62"/>
-      <c r="V16" s="86" t="s">
+      <c r="S16" s="62"/>
+      <c r="T16" s="62"/>
+      <c r="U16" s="63"/>
+      <c r="V16" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="W16" s="69" t="s">
+      <c r="W16" s="64" t="s">
         <v>28</v>
       </c>
       <c r="X16" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="Y16" s="62"/>
+      <c r="Y16" s="63"/>
       <c r="Z16" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="AA16" s="62"/>
+      <c r="AA16" s="63"/>
       <c r="AB16" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="AC16" s="70"/>
+      <c r="AC16" s="65"/>
     </row>
     <row r="17" spans="1:29" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="74"/>
+      <c r="A17" s="69"/>
       <c r="B17" s="22" t="s">
         <v>32</v>
       </c>
@@ -2046,7 +2073,7 @@
       <c r="L17" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="M17" s="46" t="s">
+      <c r="M17" s="44" t="s">
         <v>41</v>
       </c>
       <c r="N17" s="20" t="s">
@@ -2073,8 +2100,8 @@
       <c r="U17" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="V17" s="87"/>
-      <c r="W17" s="85"/>
+      <c r="V17" s="82"/>
+      <c r="W17" s="80"/>
       <c r="X17" s="13" t="s">
         <v>47</v>
       </c>
@@ -2087,7 +2114,7 @@
       <c r="AA17" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="AB17" s="30" t="s">
+      <c r="AB17" s="29" t="s">
         <v>50</v>
       </c>
       <c r="AC17" s="14" t="s">
@@ -2095,120 +2122,126 @@
       </c>
     </row>
     <row r="18" spans="1:29" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="33">
+      <c r="B18" s="31">
         <v>11</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="35">
+      <c r="C18" s="32"/>
+      <c r="D18" s="33">
         <v>1</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="40"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="39"/>
-      <c r="R18" s="40"/>
-      <c r="S18" s="41"/>
-      <c r="T18" s="34"/>
-      <c r="U18" s="37"/>
-      <c r="V18" s="37"/>
-      <c r="W18" s="37"/>
-      <c r="X18" s="40"/>
-      <c r="Y18" s="42"/>
-      <c r="Z18" s="40"/>
-      <c r="AA18" s="34"/>
-      <c r="AB18" s="47" t="s">
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="39"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="39"/>
+      <c r="T18" s="32"/>
+      <c r="U18" s="35"/>
+      <c r="V18" s="35"/>
+      <c r="W18" s="35"/>
+      <c r="X18" s="38"/>
+      <c r="Y18" s="40"/>
+      <c r="Z18" s="38"/>
+      <c r="AA18" s="32"/>
+      <c r="AB18" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="AC18" s="37"/>
+      <c r="AC18" s="35"/>
     </row>
     <row r="19" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="84" t="s">
         <v>63</v>
       </c>
-      <c r="C19"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="84"/>
       <c r="H19" s="15"/>
-      <c r="L19" s="63" t="s">
+      <c r="L19" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="M19" s="64"/>
-      <c r="N19" s="43"/>
-      <c r="O19" s="44"/>
-      <c r="P19" s="44"/>
-      <c r="Q19" s="44"/>
-      <c r="R19" s="44"/>
-      <c r="S19" s="44"/>
-      <c r="T19" s="44"/>
-      <c r="U19" s="44"/>
-      <c r="V19" s="44"/>
-      <c r="W19" s="45"/>
+      <c r="M19" s="91"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="42"/>
+      <c r="S19" s="42"/>
+      <c r="T19" s="42"/>
+      <c r="U19" s="42"/>
+      <c r="V19" s="42"/>
+      <c r="W19" s="43"/>
     </row>
     <row r="20" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="C20"/>
       <c r="H20" s="15"/>
-      <c r="L20" s="55" t="s">
+      <c r="L20" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="M20" s="55"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="57"/>
-      <c r="P20" s="57"/>
-      <c r="Q20" s="57"/>
-      <c r="R20" s="57"/>
-      <c r="S20" s="57"/>
-      <c r="T20" s="57"/>
-      <c r="U20" s="58"/>
-      <c r="V20" s="50"/>
-      <c r="W20" s="51"/>
+      <c r="M20" s="85"/>
+      <c r="N20" s="86"/>
+      <c r="O20" s="87"/>
+      <c r="P20" s="87"/>
+      <c r="Q20" s="87"/>
+      <c r="R20" s="87"/>
+      <c r="S20" s="87"/>
+      <c r="T20" s="87"/>
+      <c r="U20" s="88"/>
+      <c r="V20" s="46"/>
+      <c r="W20" s="47"/>
     </row>
     <row r="21" spans="1:29" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="C21" s="52" t="s">
+      <c r="C21" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="53"/>
+      <c r="E21" s="49"/>
       <c r="H21" s="15"/>
-      <c r="L21" s="55" t="s">
+      <c r="L21" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="M21" s="55"/>
-      <c r="N21" s="65"/>
-      <c r="O21" s="66"/>
-      <c r="P21" s="66"/>
-      <c r="Q21" s="66"/>
-      <c r="R21" s="66"/>
-      <c r="S21" s="66"/>
-      <c r="T21" s="66"/>
-      <c r="U21" s="66"/>
-      <c r="V21" s="66"/>
-      <c r="W21" s="67"/>
+      <c r="M21" s="85"/>
+      <c r="N21" s="92"/>
+      <c r="O21" s="93"/>
+      <c r="P21" s="93"/>
+      <c r="Q21" s="93"/>
+      <c r="R21" s="93"/>
+      <c r="S21" s="93"/>
+      <c r="T21" s="93"/>
+      <c r="U21" s="93"/>
+      <c r="V21" s="93"/>
+      <c r="W21" s="94"/>
     </row>
     <row r="22" spans="1:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="C22" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="54"/>
+      <c r="E22" s="50"/>
       <c r="H22" s="15"/>
       <c r="L22" s="15"/>
       <c r="M22"/>
-      <c r="AA22" s="28" t="s">
+      <c r="Y22" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="AB22" s="59"/>
-      <c r="AC22" s="60"/>
+      <c r="Z22" s="57"/>
+      <c r="AA22" s="58"/>
+      <c r="AB22" s="89"/>
+      <c r="AC22" s="90"/>
     </row>
     <row r="23" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
@@ -2216,15 +2249,46 @@
       <c r="H23" s="15"/>
       <c r="L23" s="15"/>
       <c r="M23"/>
-      <c r="AA23" s="28" t="s">
+      <c r="Y23" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="AB23" s="48"/>
-      <c r="AC23" s="49"/>
+      <c r="Z23" s="57"/>
+      <c r="AA23" s="58"/>
+      <c r="AB23" s="59"/>
+      <c r="AC23" s="60"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="X15:AA15"/>
+  <mergeCells count="43">
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="AB22:AC22"/>
+    <mergeCell ref="X16:Y16"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N21:W21"/>
+    <mergeCell ref="Y22:AA22"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N20:U20"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="Y23:AA23"/>
+    <mergeCell ref="AB23:AC23"/>
+    <mergeCell ref="X15:AB15"/>
     <mergeCell ref="AC15:AC16"/>
     <mergeCell ref="A1:X1"/>
     <mergeCell ref="A15:A17"/>
@@ -2238,18 +2302,14 @@
     <mergeCell ref="N16:Q16"/>
     <mergeCell ref="W16:W17"/>
     <mergeCell ref="R16:U16"/>
-    <mergeCell ref="V16:V17"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N20:U20"/>
-    <mergeCell ref="AB22:AC22"/>
-    <mergeCell ref="X16:Y16"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="N21:W21"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="45" orientation="landscape" r:id="rId1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" scale="41" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri,Normal"&amp;K000000MCCC &amp;F&amp;R&amp;"Calibri,Normal"&amp;K000000Version du &amp;D &amp;T</oddHeader>
+    <oddFooter>&amp;L&amp;"Calibri,Normal"&amp;K000000Document généré depuis ORéOF&amp;C&amp;"Calibri,Normal"&amp;K000000Document non validé en CFVU&amp;R&amp;"Calibri,Normal"&amp;K000000Université de Reims Champagne-Ardenne</oddFooter>
+  </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -2259,39 +2319,44 @@
   <dimension ref="A1:BA13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="E5" sqref="E5:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="54" customWidth="1"/>
+    <col min="3" max="3" width="65.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="S1" s="71"/>
-      <c r="T1" s="71"/>
-      <c r="U1" s="71"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="71"/>
-      <c r="X1" s="71"/>
-      <c r="Y1" s="71"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
@@ -2312,62 +2377,62 @@
       <c r="BA1" s="2"/>
     </row>
     <row r="2" spans="1:53" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="84"/>
-      <c r="R2" s="84"/>
-      <c r="S2" s="84"/>
-      <c r="T2" s="84"/>
-      <c r="U2" s="84"/>
-      <c r="V2" s="84"/>
-      <c r="W2" s="84"/>
-      <c r="X2" s="84"/>
-      <c r="Y2" s="84"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="79"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="79"/>
+      <c r="W2" s="79"/>
+      <c r="X2" s="79"/>
+      <c r="Y2" s="79"/>
     </row>
     <row r="3" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84"/>
-      <c r="N3" s="84"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="84"/>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="84"/>
-      <c r="S3" s="84"/>
-      <c r="T3" s="84"/>
-      <c r="U3" s="84"/>
-      <c r="V3" s="84"/>
-      <c r="W3" s="84"/>
-      <c r="X3" s="84"/>
-      <c r="Y3" s="84"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="79"/>
+      <c r="Q3" s="79"/>
+      <c r="R3" s="79"/>
+      <c r="S3" s="79"/>
+      <c r="T3" s="79"/>
+      <c r="U3" s="79"/>
+      <c r="V3" s="79"/>
+      <c r="W3" s="79"/>
+      <c r="X3" s="79"/>
+      <c r="Y3" s="79"/>
     </row>
     <row r="4" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
@@ -2382,14 +2447,18 @@
     <row r="5" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
-      <c r="I5" s="27" t="s">
+      <c r="E5" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="K5" s="95"/>
+      <c r="L5" s="95"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -2403,16 +2472,18 @@
       <c r="B6" s="5"/>
       <c r="C6" s="26"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="I6" s="27" t="s">
+      <c r="E6" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="95"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -2442,14 +2513,18 @@
       <c r="A7" s="7"/>
       <c r="B7" s="5"/>
       <c r="D7" s="7"/>
-      <c r="I7" s="27" t="s">
+      <c r="E7" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="95"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -2470,8 +2545,12 @@
       <c r="B8" s="5"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="8"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="7"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -2511,6 +2590,10 @@
       <c r="A9" s="11"/>
       <c r="B9" s="5"/>
       <c r="D9" s="7"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
       <c r="I9" s="27"/>
       <c r="J9" s="7"/>
       <c r="K9" s="3"/>
@@ -2537,29 +2620,43 @@
       <c r="B10" s="5"/>
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
       <c r="N10" s="17"/>
     </row>
     <row r="11" spans="1:53" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="D11" s="7"/>
-      <c r="I11" s="27" t="s">
+      <c r="E11" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="F11" s="83"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
+      <c r="K11" s="95"/>
+      <c r="L11" s="95"/>
       <c r="N11" s="16"/>
     </row>
     <row r="12" spans="1:53" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
       <c r="I12" s="28"/>
-      <c r="J12" s="10"/>
+      <c r="J12" s="53"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
       <c r="N12" s="16"/>
@@ -2567,21 +2664,35 @@
     <row r="13" spans="1:53" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="D13" s="7"/>
-      <c r="I13" s="27" t="s">
+      <c r="E13" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="F13" s="83"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="83"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
+      <c r="K13" s="95"/>
+      <c r="L13" s="95"/>
       <c r="N13" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="13">
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="E13:I13"/>
     <mergeCell ref="A1:Y1"/>
     <mergeCell ref="A2:Y2"/>
     <mergeCell ref="A3:Y3"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2590,15 +2701,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
@@ -2607,6 +2709,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2827,20 +2938,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
     <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
fix: validation, page validation, correctifs divers sur le process
</commit_message>
<xml_diff>
--- a/public/modeles/Annexe_MCCC.xlsx
+++ b/public/modeles/Annexe_MCCC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8794AC-A452-A341-8F5D-A0176C66A238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7943D1AE-0A44-7941-A795-B749C0524FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modele" sheetId="9" r:id="rId1"/>
@@ -1065,27 +1065,75 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1136,54 +1184,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1214,14 +1214,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>696537</xdr:colOff>
+      <xdr:colOff>645737</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>17318</xdr:rowOff>
+      <xdr:rowOff>245918</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1164994</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:colOff>1114194</xdr:colOff>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>94600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1251,8 +1251,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="698442" y="21128"/>
-          <a:ext cx="1923877" cy="1187897"/>
+          <a:off x="645737" y="245918"/>
+          <a:ext cx="2068657" cy="1245682"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1611,8 +1611,8 @@
   </sheetPr>
   <dimension ref="A1:AK23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1644,32 +1644,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
+      <c r="V1" s="82"/>
+      <c r="W1" s="82"/>
+      <c r="X1" s="82"/>
+      <c r="Y1" s="82"/>
+      <c r="Z1" s="82"/>
+      <c r="AA1" s="82"/>
+      <c r="AB1" s="82"/>
+      <c r="AC1" s="82"/>
       <c r="AD1" s="2"/>
       <c r="AE1" s="2"/>
       <c r="AF1" s="2"/>
@@ -1680,75 +1685,85 @@
       <c r="AK1" s="2"/>
     </row>
     <row r="2" spans="1:37" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="95"/>
+      <c r="Q2" s="95"/>
+      <c r="R2" s="95"/>
+      <c r="S2" s="95"/>
+      <c r="T2" s="95"/>
+      <c r="U2" s="95"/>
+      <c r="V2" s="95"/>
+      <c r="W2" s="95"/>
+      <c r="X2" s="95"/>
+      <c r="Y2" s="95"/>
+      <c r="Z2" s="95"/>
+      <c r="AA2" s="95"/>
+      <c r="AB2" s="95"/>
+      <c r="AC2" s="95"/>
     </row>
     <row r="3" spans="1:37" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="79"/>
-      <c r="S3" s="79"/>
-      <c r="T3" s="79"/>
-      <c r="U3" s="79"/>
-      <c r="V3" s="79"/>
-      <c r="W3" s="79"/>
-      <c r="X3" s="79"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="95"/>
+      <c r="R3" s="95"/>
+      <c r="S3" s="95"/>
+      <c r="T3" s="95"/>
+      <c r="U3" s="95"/>
+      <c r="V3" s="95"/>
+      <c r="W3" s="95"/>
+      <c r="X3" s="95"/>
+      <c r="Y3" s="95"/>
+      <c r="Z3" s="95"/>
+      <c r="AA3" s="95"/>
+      <c r="AB3" s="95"/>
+      <c r="AC3" s="95"/>
     </row>
     <row r="4" spans="1:37" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:37" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="83" t="s">
+      <c r="G5" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="95" t="s">
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="95"/>
-      <c r="L5" s="95"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1762,16 +1777,16 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="83" t="s">
+      <c r="G6" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="95" t="s">
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="95"/>
-      <c r="L6" s="95"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -1795,20 +1810,20 @@
         <v>7</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="96" t="s">
+      <c r="E7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="95"/>
-      <c r="G7" s="83" t="s">
+      <c r="F7" s="58"/>
+      <c r="G7" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="83"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="95" t="s">
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="95"/>
-      <c r="L7" s="95"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1848,20 +1863,20 @@
     <row r="9" spans="1:37" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="96" t="s">
+      <c r="E9" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="95"/>
-      <c r="G9" s="83" t="s">
+      <c r="F9" s="58"/>
+      <c r="G9" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="95" t="s">
+      <c r="H9" s="72"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="95"/>
-      <c r="L9" s="95"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -1893,20 +1908,20 @@
     </row>
     <row r="11" spans="1:37" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D11" s="6"/>
-      <c r="E11" s="96" t="s">
+      <c r="E11" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="95"/>
-      <c r="G11" s="83" t="s">
+      <c r="F11" s="58"/>
+      <c r="G11" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="83"/>
-      <c r="I11" s="83"/>
-      <c r="J11" s="95" t="s">
+      <c r="H11" s="72"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="95"/>
-      <c r="L11" s="95"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
       <c r="M11" s="16"/>
     </row>
     <row r="12" spans="1:37" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1923,27 +1938,27 @@
     </row>
     <row r="13" spans="1:37" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D13" s="6"/>
-      <c r="E13" s="96" t="s">
+      <c r="E13" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="95"/>
-      <c r="G13" s="83" t="s">
+      <c r="F13" s="58"/>
+      <c r="G13" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="83"/>
-      <c r="I13" s="83"/>
-      <c r="J13" s="95" t="s">
+      <c r="H13" s="72"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="95"/>
-      <c r="L13" s="95"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
       <c r="M13" s="16"/>
     </row>
     <row r="14" spans="1:37" ht="11" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="94"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="18"/>
@@ -1953,95 +1968,95 @@
       <c r="M14" s="18"/>
     </row>
     <row r="15" spans="1:37" s="1" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="71"/>
-      <c r="D15" s="74" t="s">
+      <c r="C15" s="87"/>
+      <c r="D15" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="74"/>
-      <c r="I15" s="74"/>
-      <c r="J15" s="74"/>
-      <c r="K15" s="74"/>
-      <c r="L15" s="74"/>
-      <c r="M15" s="75"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="90"/>
+      <c r="I15" s="90"/>
+      <c r="J15" s="90"/>
+      <c r="K15" s="90"/>
+      <c r="L15" s="90"/>
+      <c r="M15" s="91"/>
       <c r="N15" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="62"/>
-      <c r="P15" s="62"/>
-      <c r="Q15" s="62"/>
-      <c r="R15" s="62"/>
-      <c r="S15" s="62"/>
-      <c r="T15" s="62"/>
-      <c r="U15" s="62"/>
-      <c r="V15" s="62"/>
-      <c r="W15" s="63"/>
+      <c r="O15" s="79"/>
+      <c r="P15" s="79"/>
+      <c r="Q15" s="79"/>
+      <c r="R15" s="79"/>
+      <c r="S15" s="79"/>
+      <c r="T15" s="79"/>
+      <c r="U15" s="79"/>
+      <c r="V15" s="79"/>
+      <c r="W15" s="62"/>
       <c r="X15" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="Y15" s="62"/>
-      <c r="Z15" s="62"/>
-      <c r="AA15" s="62"/>
-      <c r="AB15" s="63"/>
-      <c r="AC15" s="64" t="s">
+      <c r="Y15" s="79"/>
+      <c r="Z15" s="79"/>
+      <c r="AA15" s="79"/>
+      <c r="AB15" s="62"/>
+      <c r="AC15" s="80" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:37" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="68"/>
-      <c r="B16" s="72"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="76"/>
-      <c r="L16" s="76"/>
-      <c r="M16" s="77"/>
+      <c r="A16" s="84"/>
+      <c r="B16" s="88"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="92"/>
+      <c r="L16" s="92"/>
+      <c r="M16" s="93"/>
       <c r="N16" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="O16" s="62"/>
-      <c r="P16" s="62"/>
-      <c r="Q16" s="63"/>
+      <c r="O16" s="79"/>
+      <c r="P16" s="79"/>
+      <c r="Q16" s="62"/>
       <c r="R16" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="S16" s="62"/>
-      <c r="T16" s="62"/>
-      <c r="U16" s="63"/>
-      <c r="V16" s="81" t="s">
+      <c r="S16" s="79"/>
+      <c r="T16" s="79"/>
+      <c r="U16" s="62"/>
+      <c r="V16" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="W16" s="64" t="s">
+      <c r="W16" s="80" t="s">
         <v>28</v>
       </c>
       <c r="X16" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="Y16" s="63"/>
+      <c r="Y16" s="62"/>
       <c r="Z16" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="AA16" s="63"/>
+      <c r="AA16" s="62"/>
       <c r="AB16" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="AC16" s="65"/>
+      <c r="AC16" s="81"/>
     </row>
     <row r="17" spans="1:29" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="69"/>
+      <c r="A17" s="85"/>
       <c r="B17" s="22" t="s">
         <v>32</v>
       </c>
@@ -2100,8 +2115,8 @@
       <c r="U17" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="V17" s="82"/>
-      <c r="W17" s="80"/>
+      <c r="V17" s="71"/>
+      <c r="W17" s="96"/>
       <c r="X17" s="13" t="s">
         <v>47</v>
       </c>
@@ -2161,19 +2176,19 @@
       <c r="AC18" s="35"/>
     </row>
     <row r="19" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="84" t="s">
+      <c r="A19" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="84"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="84"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
       <c r="H19" s="15"/>
-      <c r="L19" s="91" t="s">
+      <c r="L19" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="M19" s="91"/>
+      <c r="M19" s="63"/>
       <c r="N19" s="41"/>
       <c r="O19" s="42"/>
       <c r="P19" s="42"/>
@@ -2189,18 +2204,18 @@
       <c r="A20" s="5"/>
       <c r="C20"/>
       <c r="H20" s="15"/>
-      <c r="L20" s="85" t="s">
+      <c r="L20" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="M20" s="85"/>
-      <c r="N20" s="86"/>
-      <c r="O20" s="87"/>
-      <c r="P20" s="87"/>
-      <c r="Q20" s="87"/>
-      <c r="R20" s="87"/>
-      <c r="S20" s="87"/>
-      <c r="T20" s="87"/>
-      <c r="U20" s="88"/>
+      <c r="M20" s="64"/>
+      <c r="N20" s="74"/>
+      <c r="O20" s="75"/>
+      <c r="P20" s="75"/>
+      <c r="Q20" s="75"/>
+      <c r="R20" s="75"/>
+      <c r="S20" s="75"/>
+      <c r="T20" s="75"/>
+      <c r="U20" s="76"/>
       <c r="V20" s="46"/>
       <c r="W20" s="47"/>
     </row>
@@ -2211,20 +2226,20 @@
       </c>
       <c r="E21" s="49"/>
       <c r="H21" s="15"/>
-      <c r="L21" s="85" t="s">
+      <c r="L21" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="M21" s="85"/>
-      <c r="N21" s="92"/>
-      <c r="O21" s="93"/>
-      <c r="P21" s="93"/>
-      <c r="Q21" s="93"/>
-      <c r="R21" s="93"/>
-      <c r="S21" s="93"/>
-      <c r="T21" s="93"/>
-      <c r="U21" s="93"/>
-      <c r="V21" s="93"/>
-      <c r="W21" s="94"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="65"/>
+      <c r="O21" s="66"/>
+      <c r="P21" s="66"/>
+      <c r="Q21" s="66"/>
+      <c r="R21" s="66"/>
+      <c r="S21" s="66"/>
+      <c r="T21" s="66"/>
+      <c r="U21" s="66"/>
+      <c r="V21" s="66"/>
+      <c r="W21" s="67"/>
     </row>
     <row r="22" spans="1:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
@@ -2235,13 +2250,13 @@
       <c r="H22" s="15"/>
       <c r="L22" s="15"/>
       <c r="M22"/>
-      <c r="Y22" s="57" t="s">
+      <c r="Y22" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="Z22" s="57"/>
-      <c r="AA22" s="58"/>
-      <c r="AB22" s="89"/>
-      <c r="AC22" s="90"/>
+      <c r="Z22" s="68"/>
+      <c r="AA22" s="69"/>
+      <c r="AB22" s="59"/>
+      <c r="AC22" s="60"/>
     </row>
     <row r="23" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
@@ -2249,28 +2264,32 @@
       <c r="H23" s="15"/>
       <c r="L23" s="15"/>
       <c r="M23"/>
-      <c r="Y23" s="57" t="s">
+      <c r="Y23" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="Z23" s="57"/>
-      <c r="AA23" s="58"/>
-      <c r="AB23" s="59"/>
-      <c r="AC23" s="60"/>
+      <c r="Z23" s="68"/>
+      <c r="AA23" s="69"/>
+      <c r="AB23" s="77"/>
+      <c r="AC23" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="AB22:AC22"/>
-    <mergeCell ref="X16:Y16"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="N21:W21"/>
-    <mergeCell ref="Y22:AA22"/>
-    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="A1:AC1"/>
+    <mergeCell ref="A2:AC2"/>
+    <mergeCell ref="A3:AC3"/>
+    <mergeCell ref="Y23:AA23"/>
+    <mergeCell ref="AB23:AC23"/>
+    <mergeCell ref="X15:AB15"/>
+    <mergeCell ref="AC15:AC16"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="D15:M16"/>
+    <mergeCell ref="N15:W15"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="R16:U16"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="L21:M21"/>
@@ -2286,22 +2305,18 @@
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="J13:L13"/>
-    <mergeCell ref="Y23:AA23"/>
-    <mergeCell ref="AB23:AC23"/>
-    <mergeCell ref="X15:AB15"/>
-    <mergeCell ref="AC15:AC16"/>
-    <mergeCell ref="A1:X1"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="D15:M16"/>
-    <mergeCell ref="N15:W15"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="A2:X2"/>
-    <mergeCell ref="A3:X3"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="W16:W17"/>
-    <mergeCell ref="R16:U16"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="AB22:AC22"/>
+    <mergeCell ref="X16:Y16"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N21:W21"/>
+    <mergeCell ref="Y22:AA22"/>
+    <mergeCell ref="V16:V17"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2330,33 +2345,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
+      <c r="V1" s="82"/>
+      <c r="W1" s="82"/>
+      <c r="X1" s="82"/>
+      <c r="Y1" s="82"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
@@ -2377,62 +2392,62 @@
       <c r="BA1" s="2"/>
     </row>
     <row r="2" spans="1:53" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="79"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="95"/>
+      <c r="Q2" s="95"/>
+      <c r="R2" s="95"/>
+      <c r="S2" s="95"/>
+      <c r="T2" s="95"/>
+      <c r="U2" s="95"/>
+      <c r="V2" s="95"/>
+      <c r="W2" s="95"/>
+      <c r="X2" s="95"/>
+      <c r="Y2" s="95"/>
     </row>
     <row r="3" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="79"/>
-      <c r="S3" s="79"/>
-      <c r="T3" s="79"/>
-      <c r="U3" s="79"/>
-      <c r="V3" s="79"/>
-      <c r="W3" s="79"/>
-      <c r="X3" s="79"/>
-      <c r="Y3" s="79"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="95"/>
+      <c r="R3" s="95"/>
+      <c r="S3" s="95"/>
+      <c r="T3" s="95"/>
+      <c r="U3" s="95"/>
+      <c r="V3" s="95"/>
+      <c r="W3" s="95"/>
+      <c r="X3" s="95"/>
+      <c r="Y3" s="95"/>
     </row>
     <row r="4" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
@@ -2447,18 +2462,18 @@
     <row r="5" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
-      <c r="E5" s="83" t="s">
+      <c r="E5" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="95" t="s">
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="95"/>
-      <c r="L5" s="95"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -2472,18 +2487,18 @@
       <c r="B6" s="5"/>
       <c r="C6" s="26"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="83" t="s">
+      <c r="E6" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="95" t="s">
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="95"/>
-      <c r="L6" s="95"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -2513,18 +2528,18 @@
       <c r="A7" s="7"/>
       <c r="B7" s="5"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="83" t="s">
+      <c r="E7" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="95" t="s">
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="95"/>
-      <c r="L7" s="95"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -2633,18 +2648,18 @@
     <row r="11" spans="1:53" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="83" t="s">
+      <c r="E11" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="83"/>
-      <c r="G11" s="83"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="83"/>
-      <c r="J11" s="95" t="s">
+      <c r="F11" s="72"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="95"/>
-      <c r="L11" s="95"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
       <c r="N11" s="16"/>
     </row>
     <row r="12" spans="1:53" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2664,22 +2679,27 @@
     <row r="13" spans="1:53" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="83" t="s">
+      <c r="E13" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="83"/>
-      <c r="J13" s="95" t="s">
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="95"/>
-      <c r="L13" s="95"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
       <c r="N13" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="A2:Y2"/>
+    <mergeCell ref="A3:Y3"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="J13:L13"/>
@@ -2688,11 +2708,6 @@
     <mergeCell ref="E7:I7"/>
     <mergeCell ref="E11:I11"/>
     <mergeCell ref="E13:I13"/>
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="A2:Y2"/>
-    <mergeCell ref="A3:Y3"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J6:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2701,26 +2716,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B7BBE98651F7A43AC7BF2F06836443C" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b51c7281b06024c9ff887df9fe3bb465">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8103b6e4-b1cc-417b-af38-f980b3f4bdef" xmlns:ns3="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c056a6abdadb071051b2c083c327215c" ns2:_="" ns3:_="">
     <xsd:import namespace="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
@@ -2937,26 +2932,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
-    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E02BC65-B354-4988-8893-F98AC7F212AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2973,4 +2969,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
+    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: Licence, durée des épreuves, export Excel
</commit_message>
<xml_diff>
--- a/public/modeles/Annexe_MCCC.xlsx
+++ b/public/modeles/Annexe_MCCC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7943D1AE-0A44-7941-A795-B749C0524FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C8D140-2A4B-D345-9E11-4B94D17BC705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modele" sheetId="9" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
   <si>
     <t>ACCREDITATION 2024-2028</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>* dans le cas du Cci, la seconde chance se traduit par la non prise en compte dans le calcul de la note finale de la moins bonne des notes de Cci obtenues dans l'enseignement concerné.</t>
+  </si>
+  <si>
+    <t>Durée</t>
   </si>
 </sst>
 </file>
@@ -367,7 +370,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -656,58 +659,6 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -909,11 +860,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1001,16 +997,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1022,7 +1018,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1041,12 +1037,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1065,30 +1061,102 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1098,92 +1166,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1609,10 +1632,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK23"/>
+  <dimension ref="A1:AM23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="N2" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="AJ9" sqref="AJ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1635,135 +1658,139 @@
     <col min="18" max="20" width="6.33203125" customWidth="1"/>
     <col min="21" max="22" width="10" customWidth="1"/>
     <col min="23" max="23" width="10.33203125" customWidth="1"/>
-    <col min="24" max="24" width="10.5" customWidth="1"/>
-    <col min="25" max="25" width="12.5" customWidth="1"/>
-    <col min="26" max="26" width="10.5" customWidth="1"/>
-    <col min="27" max="27" width="12.6640625" customWidth="1"/>
-    <col min="28" max="29" width="20.33203125" customWidth="1"/>
-    <col min="30" max="33" width="5.1640625" customWidth="1"/>
+    <col min="24" max="28" width="11.83203125" customWidth="1"/>
+    <col min="29" max="29" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="11.83203125" customWidth="1"/>
+    <col min="32" max="35" width="5.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+    <row r="1" spans="1:39" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="82"/>
-      <c r="AA1" s="82"/>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="82"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="59"/>
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="57"/>
       <c r="AF1" s="2"/>
       <c r="AG1" s="2"/>
       <c r="AH1" s="2"/>
       <c r="AI1" s="2"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
-    </row>
-    <row r="2" spans="1:37" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="95" t="s">
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+    </row>
+    <row r="2" spans="1:39" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
-      <c r="Q2" s="95"/>
-      <c r="R2" s="95"/>
-      <c r="S2" s="95"/>
-      <c r="T2" s="95"/>
-      <c r="U2" s="95"/>
-      <c r="V2" s="95"/>
-      <c r="W2" s="95"/>
-      <c r="X2" s="95"/>
-      <c r="Y2" s="95"/>
-      <c r="Z2" s="95"/>
-      <c r="AA2" s="95"/>
-      <c r="AB2" s="95"/>
-      <c r="AC2" s="95"/>
-    </row>
-    <row r="3" spans="1:37" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="95" t="s">
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="60"/>
+      <c r="W2" s="60"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="60"/>
+      <c r="Z2" s="60"/>
+      <c r="AA2" s="60"/>
+      <c r="AB2" s="60"/>
+      <c r="AC2" s="60"/>
+      <c r="AD2" s="60"/>
+      <c r="AE2" s="58"/>
+    </row>
+    <row r="3" spans="1:39" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95"/>
-      <c r="Q3" s="95"/>
-      <c r="R3" s="95"/>
-      <c r="S3" s="95"/>
-      <c r="T3" s="95"/>
-      <c r="U3" s="95"/>
-      <c r="V3" s="95"/>
-      <c r="W3" s="95"/>
-      <c r="X3" s="95"/>
-      <c r="Y3" s="95"/>
-      <c r="Z3" s="95"/>
-      <c r="AA3" s="95"/>
-      <c r="AB3" s="95"/>
-      <c r="AC3" s="95"/>
-    </row>
-    <row r="4" spans="1:37" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="60"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="60"/>
+      <c r="U3" s="60"/>
+      <c r="V3" s="60"/>
+      <c r="W3" s="60"/>
+      <c r="X3" s="60"/>
+      <c r="Y3" s="60"/>
+      <c r="Z3" s="60"/>
+      <c r="AA3" s="60"/>
+      <c r="AB3" s="60"/>
+      <c r="AC3" s="60"/>
+      <c r="AD3" s="60"/>
+      <c r="AE3" s="58"/>
+    </row>
+    <row r="4" spans="1:39" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:37" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="72" t="s">
+    <row r="5" spans="1:39" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G5" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="58" t="s">
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1772,21 +1799,21 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:37" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="26"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="72" t="s">
+      <c r="G6" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="58" t="s">
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -1803,27 +1830,28 @@
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
-    </row>
-    <row r="7" spans="1:37" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AC6" s="3"/>
+    </row>
+    <row r="7" spans="1:39" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="8"/>
       <c r="C7" s="56" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="58"/>
-      <c r="G7" s="72" t="s">
+      <c r="F7" s="86"/>
+      <c r="G7" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="58" t="s">
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="86"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1832,7 +1860,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:37" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="8"/>
       <c r="E8" s="7"/>
       <c r="F8" s="51"/>
@@ -1858,25 +1886,26 @@
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
-      <c r="AD8" s="3"/>
-    </row>
-    <row r="9" spans="1:37" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AC8" s="3"/>
+      <c r="AF8" s="3"/>
+    </row>
+    <row r="9" spans="1:39" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="58"/>
-      <c r="G9" s="72" t="s">
+      <c r="F9" s="86"/>
+      <c r="G9" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="58" t="s">
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -1893,8 +1922,9 @@
       <c r="Z9" s="4"/>
       <c r="AA9" s="4"/>
       <c r="AB9" s="4"/>
-    </row>
-    <row r="10" spans="1:37" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AC9" s="4"/>
+    </row>
+    <row r="10" spans="1:39" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D10" s="9"/>
       <c r="E10" s="53"/>
       <c r="F10" s="51"/>
@@ -1906,25 +1936,25 @@
       <c r="L10" s="51"/>
       <c r="M10" s="17"/>
     </row>
-    <row r="11" spans="1:37" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D11" s="6"/>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="58"/>
-      <c r="G11" s="72" t="s">
+      <c r="F11" s="86"/>
+      <c r="G11" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="72"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="58" t="s">
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="86"/>
       <c r="M11" s="16"/>
     </row>
-    <row r="12" spans="1:37" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="51"/>
@@ -1936,29 +1966,29 @@
       <c r="L12" s="51"/>
       <c r="M12" s="16"/>
     </row>
-    <row r="13" spans="1:37" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D13" s="6"/>
-      <c r="E13" s="57" t="s">
+      <c r="E13" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="58"/>
-      <c r="G13" s="72" t="s">
+      <c r="F13" s="86"/>
+      <c r="G13" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="58" t="s">
+      <c r="H13" s="80"/>
+      <c r="I13" s="80"/>
+      <c r="J13" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
       <c r="M13" s="16"/>
     </row>
-    <row r="14" spans="1:37" ht="11" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
+    <row r="14" spans="1:39" ht="11" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="18"/>
@@ -1967,96 +1997,100 @@
       <c r="L14" s="5"/>
       <c r="M14" s="18"/>
     </row>
-    <row r="15" spans="1:37" s="1" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="83" t="s">
+    <row r="15" spans="1:39" s="1" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="86" t="s">
+      <c r="B15" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="87"/>
-      <c r="D15" s="90" t="s">
+      <c r="C15" s="71"/>
+      <c r="D15" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="90"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="90"/>
-      <c r="J15" s="90"/>
-      <c r="K15" s="90"/>
-      <c r="L15" s="90"/>
-      <c r="M15" s="91"/>
-      <c r="N15" s="61" t="s">
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="74"/>
+      <c r="L15" s="74"/>
+      <c r="M15" s="75"/>
+      <c r="N15" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="79"/>
-      <c r="P15" s="79"/>
-      <c r="Q15" s="79"/>
-      <c r="R15" s="79"/>
-      <c r="S15" s="79"/>
-      <c r="T15" s="79"/>
-      <c r="U15" s="79"/>
-      <c r="V15" s="79"/>
-      <c r="W15" s="62"/>
-      <c r="X15" s="61" t="s">
+      <c r="O15" s="64"/>
+      <c r="P15" s="64"/>
+      <c r="Q15" s="64"/>
+      <c r="R15" s="64"/>
+      <c r="S15" s="64"/>
+      <c r="T15" s="64"/>
+      <c r="U15" s="64"/>
+      <c r="V15" s="64"/>
+      <c r="W15" s="65"/>
+      <c r="X15" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="Y15" s="79"/>
-      <c r="Z15" s="79"/>
-      <c r="AA15" s="79"/>
-      <c r="AB15" s="62"/>
-      <c r="AC15" s="80" t="s">
+      <c r="Y15" s="64"/>
+      <c r="Z15" s="64"/>
+      <c r="AA15" s="64"/>
+      <c r="AB15" s="64"/>
+      <c r="AC15" s="65"/>
+      <c r="AD15" s="100" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:37" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="84"/>
-      <c r="B16" s="88"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="92"/>
-      <c r="M16" s="93"/>
-      <c r="N16" s="61" t="s">
+      <c r="AE15" s="101"/>
+    </row>
+    <row r="16" spans="1:39" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="68"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
+      <c r="M16" s="77"/>
+      <c r="N16" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="O16" s="79"/>
-      <c r="P16" s="79"/>
-      <c r="Q16" s="62"/>
-      <c r="R16" s="61" t="s">
+      <c r="O16" s="64"/>
+      <c r="P16" s="64"/>
+      <c r="Q16" s="65"/>
+      <c r="R16" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="S16" s="79"/>
-      <c r="T16" s="79"/>
-      <c r="U16" s="62"/>
-      <c r="V16" s="70" t="s">
+      <c r="S16" s="64"/>
+      <c r="T16" s="64"/>
+      <c r="U16" s="65"/>
+      <c r="V16" s="92" t="s">
         <v>59</v>
       </c>
-      <c r="W16" s="80" t="s">
+      <c r="W16" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="X16" s="61" t="s">
+      <c r="X16" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="Y16" s="62"/>
-      <c r="Z16" s="61" t="s">
+      <c r="Y16" s="65"/>
+      <c r="Z16" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="AA16" s="62"/>
-      <c r="AB16" s="21" t="s">
+      <c r="AA16" s="64"/>
+      <c r="AB16" s="65"/>
+      <c r="AC16" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="AC16" s="81"/>
-    </row>
-    <row r="17" spans="1:29" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="85"/>
+      <c r="AD16" s="79"/>
+      <c r="AE16" s="102"/>
+    </row>
+    <row r="17" spans="1:31" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="69"/>
       <c r="B17" s="22" t="s">
         <v>32</v>
       </c>
@@ -2115,28 +2149,34 @@
       <c r="U17" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="V17" s="71"/>
-      <c r="W17" s="96"/>
+      <c r="V17" s="93"/>
+      <c r="W17" s="79"/>
       <c r="X17" s="13" t="s">
         <v>47</v>
       </c>
       <c r="Y17" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="Z17" s="13" t="s">
+      <c r="Z17" s="94" t="s">
         <v>47</v>
       </c>
-      <c r="AA17" s="25" t="s">
+      <c r="AA17" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="AB17" s="29" t="s">
+      <c r="AB17" s="96" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC17" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="AC17" s="14" t="s">
+      <c r="AD17" s="94" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:29" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AE17" s="96" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>51</v>
       </c>
@@ -2168,27 +2208,29 @@
       <c r="W18" s="35"/>
       <c r="X18" s="38"/>
       <c r="Y18" s="40"/>
-      <c r="Z18" s="38"/>
-      <c r="AA18" s="32"/>
-      <c r="AB18" s="45" t="s">
+      <c r="Z18" s="97"/>
+      <c r="AA18" s="98"/>
+      <c r="AB18" s="99"/>
+      <c r="AC18" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="AC18" s="35"/>
-    </row>
-    <row r="19" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="73" t="s">
+      <c r="AD18" s="97"/>
+      <c r="AE18" s="99"/>
+    </row>
+    <row r="19" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
       <c r="H19" s="15"/>
-      <c r="L19" s="63" t="s">
+      <c r="L19" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="M19" s="63"/>
+      <c r="M19" s="88"/>
       <c r="N19" s="41"/>
       <c r="O19" s="42"/>
       <c r="P19" s="42"/>
@@ -2200,48 +2242,48 @@
       <c r="V19" s="42"/>
       <c r="W19" s="43"/>
     </row>
-    <row r="20" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="C20"/>
       <c r="H20" s="15"/>
-      <c r="L20" s="64" t="s">
+      <c r="L20" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="M20" s="64"/>
-      <c r="N20" s="74"/>
-      <c r="O20" s="75"/>
-      <c r="P20" s="75"/>
-      <c r="Q20" s="75"/>
-      <c r="R20" s="75"/>
-      <c r="S20" s="75"/>
-      <c r="T20" s="75"/>
-      <c r="U20" s="76"/>
+      <c r="M20" s="82"/>
+      <c r="N20" s="83"/>
+      <c r="O20" s="84"/>
+      <c r="P20" s="84"/>
+      <c r="Q20" s="84"/>
+      <c r="R20" s="84"/>
+      <c r="S20" s="84"/>
+      <c r="T20" s="84"/>
+      <c r="U20" s="85"/>
       <c r="V20" s="46"/>
       <c r="W20" s="47"/>
     </row>
-    <row r="21" spans="1:29" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="C21" s="48" t="s">
         <v>53</v>
       </c>
       <c r="E21" s="49"/>
       <c r="H21" s="15"/>
-      <c r="L21" s="64" t="s">
+      <c r="L21" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="M21" s="64"/>
-      <c r="N21" s="65"/>
-      <c r="O21" s="66"/>
-      <c r="P21" s="66"/>
-      <c r="Q21" s="66"/>
-      <c r="R21" s="66"/>
-      <c r="S21" s="66"/>
-      <c r="T21" s="66"/>
-      <c r="U21" s="66"/>
-      <c r="V21" s="66"/>
-      <c r="W21" s="67"/>
-    </row>
-    <row r="22" spans="1:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M21" s="82"/>
+      <c r="N21" s="89"/>
+      <c r="O21" s="90"/>
+      <c r="P21" s="90"/>
+      <c r="Q21" s="90"/>
+      <c r="R21" s="90"/>
+      <c r="S21" s="90"/>
+      <c r="T21" s="90"/>
+      <c r="U21" s="90"/>
+      <c r="V21" s="90"/>
+      <c r="W21" s="91"/>
+    </row>
+    <row r="22" spans="1:31" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="C22" s="28" t="s">
         <v>55</v>
@@ -2250,46 +2292,46 @@
       <c r="H22" s="15"/>
       <c r="L22" s="15"/>
       <c r="M22"/>
-      <c r="Y22" s="68" t="s">
+      <c r="Z22" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="Z22" s="68"/>
-      <c r="AA22" s="69"/>
-      <c r="AB22" s="59"/>
-      <c r="AC22" s="60"/>
-    </row>
-    <row r="23" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AA22" s="61"/>
+      <c r="AB22" s="62"/>
+      <c r="AC22" s="103"/>
+      <c r="AD22" s="104"/>
+      <c r="AE22" s="105"/>
+    </row>
+    <row r="23" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="C23"/>
       <c r="H23" s="15"/>
       <c r="L23" s="15"/>
       <c r="M23"/>
-      <c r="Y23" s="68" t="s">
+      <c r="Z23" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="Z23" s="68"/>
-      <c r="AA23" s="69"/>
-      <c r="AB23" s="77"/>
-      <c r="AC23" s="78"/>
+      <c r="AA23" s="61"/>
+      <c r="AB23" s="62"/>
+      <c r="AC23" s="103"/>
+      <c r="AD23" s="104"/>
+      <c r="AE23" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A1:AC1"/>
-    <mergeCell ref="A2:AC2"/>
-    <mergeCell ref="A3:AC3"/>
-    <mergeCell ref="Y23:AA23"/>
-    <mergeCell ref="AB23:AC23"/>
-    <mergeCell ref="X15:AB15"/>
-    <mergeCell ref="AC15:AC16"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="D15:M16"/>
-    <mergeCell ref="N15:W15"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="W16:W17"/>
-    <mergeCell ref="R16:U16"/>
+    <mergeCell ref="AC23:AE23"/>
+    <mergeCell ref="Z22:AB22"/>
+    <mergeCell ref="Z23:AB23"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="X16:Y16"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N21:W21"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="AD15:AE16"/>
+    <mergeCell ref="Z16:AB16"/>
+    <mergeCell ref="AC22:AE22"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="L21:M21"/>
@@ -2306,17 +2348,19 @@
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="AB22:AC22"/>
-    <mergeCell ref="X16:Y16"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="N21:W21"/>
-    <mergeCell ref="Y22:AA22"/>
-    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="A1:AD1"/>
+    <mergeCell ref="A2:AD2"/>
+    <mergeCell ref="A3:AD3"/>
+    <mergeCell ref="X15:AC15"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="D15:M16"/>
+    <mergeCell ref="N15:W15"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="R16:U16"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2345,33 +2389,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
@@ -2392,62 +2436,62 @@
       <c r="BA1" s="2"/>
     </row>
     <row r="2" spans="1:53" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
-      <c r="Q2" s="95"/>
-      <c r="R2" s="95"/>
-      <c r="S2" s="95"/>
-      <c r="T2" s="95"/>
-      <c r="U2" s="95"/>
-      <c r="V2" s="95"/>
-      <c r="W2" s="95"/>
-      <c r="X2" s="95"/>
-      <c r="Y2" s="95"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="60"/>
+      <c r="W2" s="60"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="60"/>
     </row>
     <row r="3" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95"/>
-      <c r="Q3" s="95"/>
-      <c r="R3" s="95"/>
-      <c r="S3" s="95"/>
-      <c r="T3" s="95"/>
-      <c r="U3" s="95"/>
-      <c r="V3" s="95"/>
-      <c r="W3" s="95"/>
-      <c r="X3" s="95"/>
-      <c r="Y3" s="95"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="60"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="60"/>
+      <c r="U3" s="60"/>
+      <c r="V3" s="60"/>
+      <c r="W3" s="60"/>
+      <c r="X3" s="60"/>
+      <c r="Y3" s="60"/>
     </row>
     <row r="4" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
@@ -2462,18 +2506,18 @@
     <row r="5" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="58" t="s">
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -2487,18 +2531,18 @@
       <c r="B6" s="5"/>
       <c r="C6" s="26"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="72" t="s">
+      <c r="E6" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="58" t="s">
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -2528,18 +2572,18 @@
       <c r="A7" s="7"/>
       <c r="B7" s="5"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="72" t="s">
+      <c r="E7" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="58" t="s">
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="86"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -2648,18 +2692,18 @@
     <row r="11" spans="1:53" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="72" t="s">
+      <c r="E11" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="72"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="58" t="s">
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="86"/>
       <c r="N11" s="16"/>
     </row>
     <row r="12" spans="1:53" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2679,27 +2723,22 @@
     <row r="13" spans="1:53" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="72" t="s">
+      <c r="E13" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="58" t="s">
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="80"/>
+      <c r="I13" s="80"/>
+      <c r="J13" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
       <c r="N13" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="A2:Y2"/>
-    <mergeCell ref="A3:Y3"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J6:L6"/>
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="J13:L13"/>
@@ -2708,6 +2747,11 @@
     <mergeCell ref="E7:I7"/>
     <mergeCell ref="E11:I11"/>
     <mergeCell ref="E13:I13"/>
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="A2:Y2"/>
+    <mergeCell ref="A3:Y3"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2933,15 +2977,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
@@ -2950,6 +2985,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2972,14 +3016,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2988,4 +3024,12 @@
     <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: Affichage des BCC selon parcours
</commit_message>
<xml_diff>
--- a/public/modeles/Annexe_MCCC.xlsx
+++ b/public/modeles/Annexe_MCCC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C8D140-2A4B-D345-9E11-4B94D17BC705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFC421F-5B9D-0F4C-965F-F930051590BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modele" sheetId="9" r:id="rId1"/>
@@ -370,7 +370,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -499,103 +499,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -761,58 +671,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -905,11 +763,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -946,7 +830,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -967,246 +851,247 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1634,8 +1519,8 @@
   </sheetPr>
   <dimension ref="A1:AM23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N2" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="AJ9" sqref="AJ9"/>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1665,39 +1550,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="59"/>
-      <c r="Z1" s="59"/>
-      <c r="AA1" s="59"/>
-      <c r="AB1" s="59"/>
-      <c r="AC1" s="59"/>
-      <c r="AD1" s="59"/>
-      <c r="AE1" s="57"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="94"/>
+      <c r="R1" s="94"/>
+      <c r="S1" s="94"/>
+      <c r="T1" s="94"/>
+      <c r="U1" s="94"/>
+      <c r="V1" s="94"/>
+      <c r="W1" s="94"/>
+      <c r="X1" s="94"/>
+      <c r="Y1" s="94"/>
+      <c r="Z1" s="94"/>
+      <c r="AA1" s="94"/>
+      <c r="AB1" s="94"/>
+      <c r="AC1" s="94"/>
+      <c r="AD1" s="94"/>
+      <c r="AE1" s="52"/>
       <c r="AF1" s="2"/>
       <c r="AG1" s="2"/>
       <c r="AH1" s="2"/>
@@ -1708,89 +1593,89 @@
       <c r="AM1" s="2"/>
     </row>
     <row r="2" spans="1:39" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="60"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="60"/>
-      <c r="V2" s="60"/>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="60"/>
-      <c r="Z2" s="60"/>
-      <c r="AA2" s="60"/>
-      <c r="AB2" s="60"/>
-      <c r="AC2" s="60"/>
-      <c r="AD2" s="60"/>
-      <c r="AE2" s="58"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="95"/>
+      <c r="Q2" s="95"/>
+      <c r="R2" s="95"/>
+      <c r="S2" s="95"/>
+      <c r="T2" s="95"/>
+      <c r="U2" s="95"/>
+      <c r="V2" s="95"/>
+      <c r="W2" s="95"/>
+      <c r="X2" s="95"/>
+      <c r="Y2" s="95"/>
+      <c r="Z2" s="95"/>
+      <c r="AA2" s="95"/>
+      <c r="AB2" s="95"/>
+      <c r="AC2" s="95"/>
+      <c r="AD2" s="95"/>
+      <c r="AE2" s="53"/>
     </row>
     <row r="3" spans="1:39" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
-      <c r="R3" s="60"/>
-      <c r="S3" s="60"/>
-      <c r="T3" s="60"/>
-      <c r="U3" s="60"/>
-      <c r="V3" s="60"/>
-      <c r="W3" s="60"/>
-      <c r="X3" s="60"/>
-      <c r="Y3" s="60"/>
-      <c r="Z3" s="60"/>
-      <c r="AA3" s="60"/>
-      <c r="AB3" s="60"/>
-      <c r="AC3" s="60"/>
-      <c r="AD3" s="60"/>
-      <c r="AE3" s="58"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="95"/>
+      <c r="R3" s="95"/>
+      <c r="S3" s="95"/>
+      <c r="T3" s="95"/>
+      <c r="U3" s="95"/>
+      <c r="V3" s="95"/>
+      <c r="W3" s="95"/>
+      <c r="X3" s="95"/>
+      <c r="Y3" s="95"/>
+      <c r="Z3" s="95"/>
+      <c r="AA3" s="95"/>
+      <c r="AB3" s="95"/>
+      <c r="AC3" s="95"/>
+      <c r="AD3" s="95"/>
+      <c r="AE3" s="53"/>
     </row>
     <row r="4" spans="1:39" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:39" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="80" t="s">
+      <c r="G5" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="86" t="s">
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="86"/>
-      <c r="L5" s="86"/>
+      <c r="K5" s="93"/>
+      <c r="L5" s="93"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1804,16 +1689,16 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="80" t="s">
+      <c r="G6" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="86" t="s">
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="86"/>
-      <c r="L6" s="86"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="93"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -1834,24 +1719,24 @@
     </row>
     <row r="7" spans="1:39" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="8"/>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="51" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="87" t="s">
+      <c r="E7" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="86"/>
-      <c r="G7" s="80" t="s">
+      <c r="F7" s="8"/>
+      <c r="G7" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="86" t="s">
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="86"/>
-      <c r="L7" s="86"/>
+      <c r="K7" s="93"/>
+      <c r="L7" s="93"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1863,10 +1748,10 @@
     <row r="8" spans="1:39" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="8"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="51"/>
+      <c r="F8" s="46"/>
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
-      <c r="I8" s="54"/>
+      <c r="I8" s="49"/>
       <c r="J8" s="7"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -1892,20 +1777,20 @@
     <row r="9" spans="1:39" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="87" t="s">
+      <c r="E9" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="86"/>
-      <c r="G9" s="80" t="s">
+      <c r="F9" s="8"/>
+      <c r="G9" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="80"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="86" t="s">
+      <c r="H9" s="92"/>
+      <c r="I9" s="92"/>
+      <c r="J9" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
+      <c r="K9" s="93"/>
+      <c r="L9" s="93"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -1926,69 +1811,69 @@
     </row>
     <row r="10" spans="1:39" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D10" s="9"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="51"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="46"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="51"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="46"/>
       <c r="M10" s="17"/>
     </row>
     <row r="11" spans="1:39" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D11" s="6"/>
-      <c r="E11" s="87" t="s">
+      <c r="E11" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="86"/>
-      <c r="G11" s="80" t="s">
+      <c r="F11" s="8"/>
+      <c r="G11" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="80"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="86" t="s">
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="86"/>
-      <c r="L11" s="86"/>
+      <c r="K11" s="93"/>
+      <c r="L11" s="93"/>
       <c r="M11" s="16"/>
     </row>
     <row r="12" spans="1:39" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="51"/>
+      <c r="F12" s="46"/>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
-      <c r="J12" s="53"/>
+      <c r="J12" s="48"/>
       <c r="K12" s="16"/>
-      <c r="L12" s="51"/>
+      <c r="L12" s="46"/>
       <c r="M12" s="16"/>
     </row>
     <row r="13" spans="1:39" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D13" s="6"/>
-      <c r="E13" s="87" t="s">
+      <c r="E13" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="86"/>
-      <c r="G13" s="80" t="s">
+      <c r="F13" s="8"/>
+      <c r="G13" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="86" t="s">
+      <c r="H13" s="92"/>
+      <c r="I13" s="92"/>
+      <c r="J13" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="86"/>
-      <c r="L13" s="86"/>
+      <c r="K13" s="93"/>
+      <c r="L13" s="93"/>
       <c r="M13" s="16"/>
     </row>
     <row r="14" spans="1:39" ht="11" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
+      <c r="C14" s="107"/>
+      <c r="D14" s="107"/>
+      <c r="E14" s="107"/>
+      <c r="F14" s="107"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="18"/>
@@ -1998,99 +1883,99 @@
       <c r="M14" s="18"/>
     </row>
     <row r="15" spans="1:39" s="1" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="71"/>
-      <c r="D15" s="74" t="s">
+      <c r="C15" s="100"/>
+      <c r="D15" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="74"/>
-      <c r="I15" s="74"/>
-      <c r="J15" s="74"/>
-      <c r="K15" s="74"/>
-      <c r="L15" s="74"/>
-      <c r="M15" s="75"/>
-      <c r="N15" s="63" t="s">
+      <c r="E15" s="103"/>
+      <c r="F15" s="103"/>
+      <c r="G15" s="103"/>
+      <c r="H15" s="103"/>
+      <c r="I15" s="103"/>
+      <c r="J15" s="103"/>
+      <c r="K15" s="103"/>
+      <c r="L15" s="103"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="64"/>
-      <c r="P15" s="64"/>
-      <c r="Q15" s="64"/>
-      <c r="R15" s="64"/>
-      <c r="S15" s="64"/>
-      <c r="T15" s="64"/>
-      <c r="U15" s="64"/>
-      <c r="V15" s="64"/>
-      <c r="W15" s="65"/>
-      <c r="X15" s="63" t="s">
+      <c r="O15" s="80"/>
+      <c r="P15" s="80"/>
+      <c r="Q15" s="80"/>
+      <c r="R15" s="80"/>
+      <c r="S15" s="80"/>
+      <c r="T15" s="80"/>
+      <c r="U15" s="80"/>
+      <c r="V15" s="80"/>
+      <c r="W15" s="81"/>
+      <c r="X15" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="Y15" s="64"/>
-      <c r="Z15" s="64"/>
-      <c r="AA15" s="64"/>
-      <c r="AB15" s="64"/>
-      <c r="AC15" s="65"/>
-      <c r="AD15" s="100" t="s">
+      <c r="Y15" s="80"/>
+      <c r="Z15" s="80"/>
+      <c r="AA15" s="80"/>
+      <c r="AB15" s="80"/>
+      <c r="AC15" s="81"/>
+      <c r="AD15" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="AE15" s="101"/>
+      <c r="AE15" s="76"/>
     </row>
     <row r="16" spans="1:39" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="68"/>
-      <c r="B16" s="72"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="76"/>
-      <c r="L16" s="76"/>
-      <c r="M16" s="77"/>
-      <c r="N16" s="63" t="s">
+      <c r="A16" s="97"/>
+      <c r="B16" s="101"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="105"/>
+      <c r="G16" s="105"/>
+      <c r="H16" s="105"/>
+      <c r="I16" s="105"/>
+      <c r="J16" s="105"/>
+      <c r="K16" s="105"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="106"/>
+      <c r="N16" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="O16" s="64"/>
-      <c r="P16" s="64"/>
-      <c r="Q16" s="65"/>
-      <c r="R16" s="63" t="s">
+      <c r="O16" s="80"/>
+      <c r="P16" s="80"/>
+      <c r="Q16" s="81"/>
+      <c r="R16" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="S16" s="64"/>
-      <c r="T16" s="64"/>
-      <c r="U16" s="65"/>
-      <c r="V16" s="92" t="s">
+      <c r="S16" s="80"/>
+      <c r="T16" s="80"/>
+      <c r="U16" s="81"/>
+      <c r="V16" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="W16" s="66" t="s">
+      <c r="W16" s="108" t="s">
         <v>28</v>
       </c>
-      <c r="X16" s="63" t="s">
+      <c r="X16" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="Y16" s="65"/>
-      <c r="Z16" s="63" t="s">
+      <c r="Y16" s="81"/>
+      <c r="Z16" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="AA16" s="64"/>
-      <c r="AB16" s="65"/>
+      <c r="AA16" s="80"/>
+      <c r="AB16" s="81"/>
       <c r="AC16" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="AD16" s="79"/>
-      <c r="AE16" s="102"/>
+      <c r="AD16" s="77"/>
+      <c r="AE16" s="78"/>
     </row>
     <row r="17" spans="1:31" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="69"/>
+      <c r="A17" s="98"/>
       <c r="B17" s="22" t="s">
         <v>32</v>
       </c>
@@ -2122,7 +2007,7 @@
       <c r="L17" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="M17" s="44" t="s">
+      <c r="M17" s="41" t="s">
         <v>41</v>
       </c>
       <c r="N17" s="20" t="s">
@@ -2149,30 +2034,30 @@
       <c r="U17" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="V17" s="93"/>
-      <c r="W17" s="79"/>
+      <c r="V17" s="88"/>
+      <c r="W17" s="77"/>
       <c r="X17" s="13" t="s">
         <v>47</v>
       </c>
       <c r="Y17" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="Z17" s="94" t="s">
+      <c r="Z17" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="AA17" s="95" t="s">
+      <c r="AA17" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="AB17" s="96" t="s">
+      <c r="AB17" s="56" t="s">
         <v>64</v>
       </c>
       <c r="AC17" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="AD17" s="94" t="s">
+      <c r="AD17" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="AE17" s="96" t="s">
+      <c r="AE17" s="56" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2193,7 +2078,7 @@
       <c r="H18" s="30"/>
       <c r="I18" s="36"/>
       <c r="J18" s="30"/>
-      <c r="K18" s="55"/>
+      <c r="K18" s="50"/>
       <c r="L18" s="30"/>
       <c r="M18" s="40"/>
       <c r="N18" s="38"/>
@@ -2208,146 +2093,115 @@
       <c r="W18" s="35"/>
       <c r="X18" s="38"/>
       <c r="Y18" s="40"/>
-      <c r="Z18" s="97"/>
-      <c r="AA18" s="98"/>
-      <c r="AB18" s="99"/>
-      <c r="AC18" s="45" t="s">
+      <c r="Z18" s="57"/>
+      <c r="AA18" s="58"/>
+      <c r="AB18" s="59"/>
+      <c r="AC18" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="AD18" s="97"/>
-      <c r="AE18" s="99"/>
-    </row>
-    <row r="19" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="81" t="s">
+      <c r="AD18" s="57"/>
+      <c r="AE18" s="59"/>
+    </row>
+    <row r="19" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="81"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
-      <c r="F19" s="81"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
+      <c r="E19" s="89"/>
+      <c r="F19" s="60"/>
       <c r="H19" s="15"/>
-      <c r="L19" s="88" t="s">
+      <c r="L19" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="M19" s="88"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="42"/>
-      <c r="S19" s="42"/>
-      <c r="T19" s="42"/>
-      <c r="U19" s="42"/>
-      <c r="V19" s="42"/>
-      <c r="W19" s="43"/>
+      <c r="M19" s="82"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="61"/>
+      <c r="P19" s="62"/>
+      <c r="Q19" s="67"/>
+      <c r="R19" s="63"/>
+      <c r="S19" s="61"/>
+      <c r="T19" s="62"/>
+      <c r="U19" s="68"/>
+      <c r="V19" s="66"/>
+      <c r="W19" s="64"/>
     </row>
     <row r="20" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="C20"/>
       <c r="H20" s="15"/>
-      <c r="L20" s="82" t="s">
+      <c r="L20" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="M20" s="82"/>
-      <c r="N20" s="83"/>
-      <c r="O20" s="84"/>
-      <c r="P20" s="84"/>
-      <c r="Q20" s="84"/>
-      <c r="R20" s="84"/>
-      <c r="S20" s="84"/>
-      <c r="T20" s="84"/>
-      <c r="U20" s="85"/>
-      <c r="V20" s="46"/>
-      <c r="W20" s="47"/>
+      <c r="M20" s="83"/>
+      <c r="N20" s="90"/>
+      <c r="O20" s="91"/>
+      <c r="P20" s="91"/>
+      <c r="Q20" s="91"/>
+      <c r="R20" s="91"/>
+      <c r="S20" s="91"/>
+      <c r="T20" s="91"/>
+      <c r="U20" s="91"/>
+      <c r="V20" s="67"/>
+      <c r="W20" s="65"/>
     </row>
     <row r="21" spans="1:31" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="C21" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="49"/>
       <c r="H21" s="15"/>
-      <c r="L21" s="82" t="s">
+      <c r="L21" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="M21" s="82"/>
-      <c r="N21" s="89"/>
-      <c r="O21" s="90"/>
-      <c r="P21" s="90"/>
-      <c r="Q21" s="90"/>
-      <c r="R21" s="90"/>
-      <c r="S21" s="90"/>
-      <c r="T21" s="90"/>
-      <c r="U21" s="90"/>
-      <c r="V21" s="90"/>
-      <c r="W21" s="91"/>
+      <c r="M21" s="83"/>
+      <c r="N21" s="84"/>
+      <c r="O21" s="85"/>
+      <c r="P21" s="85"/>
+      <c r="Q21" s="85"/>
+      <c r="R21" s="85"/>
+      <c r="S21" s="85"/>
+      <c r="T21" s="85"/>
+      <c r="U21" s="85"/>
+      <c r="V21" s="85"/>
+      <c r="W21" s="86"/>
     </row>
     <row r="22" spans="1:31" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="C22" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="50"/>
+      <c r="C22" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="44"/>
       <c r="H22" s="15"/>
       <c r="L22" s="15"/>
       <c r="M22"/>
-      <c r="Z22" s="61" t="s">
+      <c r="Z22" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="AA22" s="61"/>
-      <c r="AB22" s="62"/>
-      <c r="AC22" s="103"/>
-      <c r="AD22" s="104"/>
-      <c r="AE22" s="105"/>
+      <c r="AA22" s="73"/>
+      <c r="AB22" s="74"/>
+      <c r="AC22" s="70"/>
+      <c r="AD22" s="71"/>
+      <c r="AE22" s="72"/>
     </row>
     <row r="23" spans="1:31" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="C23"/>
+      <c r="C23" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="45"/>
       <c r="H23" s="15"/>
       <c r="L23" s="15"/>
       <c r="M23"/>
-      <c r="Z23" s="61" t="s">
+      <c r="Z23" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="AA23" s="61"/>
-      <c r="AB23" s="62"/>
-      <c r="AC23" s="103"/>
-      <c r="AD23" s="104"/>
-      <c r="AE23" s="105"/>
+      <c r="AA23" s="73"/>
+      <c r="AB23" s="74"/>
+      <c r="AC23" s="70"/>
+      <c r="AD23" s="71"/>
+      <c r="AE23" s="72"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="AC23:AE23"/>
-    <mergeCell ref="Z22:AB22"/>
-    <mergeCell ref="Z23:AB23"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="X16:Y16"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="N21:W21"/>
-    <mergeCell ref="V16:V17"/>
-    <mergeCell ref="AD15:AE16"/>
-    <mergeCell ref="Z16:AB16"/>
-    <mergeCell ref="AC22:AE22"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N20:U20"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="E13:F13"/>
+  <mergeCells count="39">
     <mergeCell ref="A1:AD1"/>
     <mergeCell ref="A2:AD2"/>
     <mergeCell ref="A3:AD3"/>
@@ -2361,6 +2215,32 @@
     <mergeCell ref="N16:Q16"/>
     <mergeCell ref="W16:W17"/>
     <mergeCell ref="R16:U16"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N20:U20"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="X16:Y16"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N21:W21"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="AC23:AE23"/>
+    <mergeCell ref="Z22:AB22"/>
+    <mergeCell ref="Z23:AB23"/>
+    <mergeCell ref="AD15:AE16"/>
+    <mergeCell ref="Z16:AB16"/>
+    <mergeCell ref="AC22:AE22"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2389,33 +2269,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="59"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="94"/>
+      <c r="R1" s="94"/>
+      <c r="S1" s="94"/>
+      <c r="T1" s="94"/>
+      <c r="U1" s="94"/>
+      <c r="V1" s="94"/>
+      <c r="W1" s="94"/>
+      <c r="X1" s="94"/>
+      <c r="Y1" s="94"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
@@ -2436,62 +2316,62 @@
       <c r="BA1" s="2"/>
     </row>
     <row r="2" spans="1:53" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="60"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="60"/>
-      <c r="V2" s="60"/>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="60"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="95"/>
+      <c r="Q2" s="95"/>
+      <c r="R2" s="95"/>
+      <c r="S2" s="95"/>
+      <c r="T2" s="95"/>
+      <c r="U2" s="95"/>
+      <c r="V2" s="95"/>
+      <c r="W2" s="95"/>
+      <c r="X2" s="95"/>
+      <c r="Y2" s="95"/>
     </row>
     <row r="3" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
-      <c r="R3" s="60"/>
-      <c r="S3" s="60"/>
-      <c r="T3" s="60"/>
-      <c r="U3" s="60"/>
-      <c r="V3" s="60"/>
-      <c r="W3" s="60"/>
-      <c r="X3" s="60"/>
-      <c r="Y3" s="60"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="95"/>
+      <c r="R3" s="95"/>
+      <c r="S3" s="95"/>
+      <c r="T3" s="95"/>
+      <c r="U3" s="95"/>
+      <c r="V3" s="95"/>
+      <c r="W3" s="95"/>
+      <c r="X3" s="95"/>
+      <c r="Y3" s="95"/>
     </row>
     <row r="4" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
@@ -2506,18 +2386,18 @@
     <row r="5" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
-      <c r="E5" s="80" t="s">
+      <c r="E5" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="86" t="s">
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="86"/>
-      <c r="L5" s="86"/>
+      <c r="K5" s="93"/>
+      <c r="L5" s="93"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -2531,18 +2411,18 @@
       <c r="B6" s="5"/>
       <c r="C6" s="26"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="80" t="s">
+      <c r="E6" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="86" t="s">
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="86"/>
-      <c r="L6" s="86"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="93"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -2572,18 +2452,18 @@
       <c r="A7" s="7"/>
       <c r="B7" s="5"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="80" t="s">
+      <c r="E7" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="86" t="s">
+      <c r="F7" s="92"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="86"/>
-      <c r="L7" s="86"/>
+      <c r="K7" s="93"/>
+      <c r="L7" s="93"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -2608,7 +2488,7 @@
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
-      <c r="I8" s="54"/>
+      <c r="I8" s="49"/>
       <c r="J8" s="7"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -2684,26 +2564,26 @@
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="52"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
       <c r="N10" s="17"/>
     </row>
     <row r="11" spans="1:53" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="80" t="s">
+      <c r="E11" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="86" t="s">
+      <c r="F11" s="92"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="86"/>
-      <c r="L11" s="86"/>
+      <c r="K11" s="93"/>
+      <c r="L11" s="93"/>
       <c r="N11" s="16"/>
     </row>
     <row r="12" spans="1:53" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2715,7 +2595,7 @@
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
-      <c r="J12" s="53"/>
+      <c r="J12" s="48"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
       <c r="N12" s="16"/>
@@ -2723,22 +2603,27 @@
     <row r="13" spans="1:53" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="80" t="s">
+      <c r="E13" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="86" t="s">
+      <c r="F13" s="92"/>
+      <c r="G13" s="92"/>
+      <c r="H13" s="92"/>
+      <c r="I13" s="92"/>
+      <c r="J13" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="86"/>
-      <c r="L13" s="86"/>
+      <c r="K13" s="93"/>
+      <c r="L13" s="93"/>
       <c r="N13" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="A2:Y2"/>
+    <mergeCell ref="A3:Y3"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="J13:L13"/>
@@ -2747,11 +2632,6 @@
     <mergeCell ref="E7:I7"/>
     <mergeCell ref="E11:I11"/>
     <mergeCell ref="E13:I13"/>
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="A2:Y2"/>
-    <mergeCell ref="A3:Y3"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J6:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2760,6 +2640,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B7BBE98651F7A43AC7BF2F06836443C" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b51c7281b06024c9ff887df9fe3bb465">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8103b6e4-b1cc-417b-af38-f980b3f4bdef" xmlns:ns3="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c056a6abdadb071051b2c083c327215c" ns2:_="" ns3:_="">
     <xsd:import namespace="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
@@ -2976,27 +2876,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
+    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E02BC65-B354-4988-8893-F98AC7F212AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3013,23 +2912,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
-    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: BUT : vérification sur les matières + BCC sur la fiche matière et pas l'UE
</commit_message>
<xml_diff>
--- a/public/modeles/Annexe_MCCC.xlsx
+++ b/public/modeles/Annexe_MCCC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18D877A-A4A0-474A-8536-1AAD2AEDC15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8277C6D7-43D3-6448-BB07-A118C4C83392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1064,9 +1064,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1091,12 +1145,6 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1106,9 +1154,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1135,12 +1180,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1160,50 +1199,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1632,7 +1632,7 @@
   <dimension ref="A1:AJ25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N4" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1763,16 +1763,16 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="91" t="s">
+      <c r="G5" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="92" t="s">
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1786,16 +1786,16 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="91" t="s">
+      <c r="G6" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="91"/>
-      <c r="I6" s="91"/>
-      <c r="J6" s="92" t="s">
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="92"/>
-      <c r="L6" s="92"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1821,16 +1821,16 @@
         <v>8</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="91" t="s">
+      <c r="G7" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="91"/>
-      <c r="I7" s="91"/>
-      <c r="J7" s="92" t="s">
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="92"/>
-      <c r="L7" s="92"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="76"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1872,16 +1872,16 @@
         <v>11</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="91" t="s">
+      <c r="G9" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="91"/>
-      <c r="I9" s="91"/>
-      <c r="J9" s="92" t="s">
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="92"/>
-      <c r="L9" s="92"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -1915,16 +1915,16 @@
         <v>14</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="91" t="s">
+      <c r="G11" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="91"/>
-      <c r="I11" s="91"/>
-      <c r="J11" s="92" t="s">
+      <c r="H11" s="75"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="92"/>
-      <c r="L11" s="92"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
       <c r="M11" s="13"/>
     </row>
     <row r="12" spans="1:36" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1945,16 +1945,16 @@
         <v>17</v>
       </c>
       <c r="F13" s="7"/>
-      <c r="G13" s="91" t="s">
+      <c r="G13" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="91"/>
-      <c r="I13" s="91"/>
-      <c r="J13" s="92" t="s">
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="92"/>
-      <c r="L13" s="92"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
       <c r="M13" s="13"/>
     </row>
     <row r="14" spans="1:36" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1965,103 +1965,103 @@
       <c r="M14"/>
     </row>
     <row r="15" spans="1:36" s="56" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="82" t="s">
+      <c r="A15" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="85" t="s">
+      <c r="B15" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="86"/>
-      <c r="D15" s="99" t="s">
+      <c r="C15" s="101"/>
+      <c r="D15" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="99"/>
-      <c r="F15" s="99"/>
-      <c r="G15" s="99"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="99"/>
-      <c r="J15" s="99"/>
-      <c r="K15" s="99"/>
-      <c r="L15" s="99"/>
-      <c r="M15" s="100"/>
-      <c r="N15" s="103" t="s">
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="77"/>
+      <c r="H15" s="77"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="77"/>
+      <c r="K15" s="77"/>
+      <c r="L15" s="77"/>
+      <c r="M15" s="78"/>
+      <c r="N15" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="104"/>
-      <c r="P15" s="104"/>
-      <c r="Q15" s="104"/>
-      <c r="R15" s="104"/>
-      <c r="S15" s="104"/>
-      <c r="T15" s="104"/>
-      <c r="U15" s="104"/>
-      <c r="V15" s="104"/>
-      <c r="W15" s="105"/>
-      <c r="X15" s="103" t="s">
+      <c r="O15" s="72"/>
+      <c r="P15" s="72"/>
+      <c r="Q15" s="72"/>
+      <c r="R15" s="72"/>
+      <c r="S15" s="72"/>
+      <c r="T15" s="72"/>
+      <c r="U15" s="72"/>
+      <c r="V15" s="72"/>
+      <c r="W15" s="81"/>
+      <c r="X15" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="Y15" s="104"/>
-      <c r="Z15" s="104"/>
-      <c r="AA15" s="71" t="s">
+      <c r="Y15" s="72"/>
+      <c r="Z15" s="72"/>
+      <c r="AA15" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="AB15" s="72"/>
-      <c r="AC15" s="72"/>
-      <c r="AD15" s="73"/>
+      <c r="AB15" s="90"/>
+      <c r="AC15" s="90"/>
+      <c r="AD15" s="91"/>
     </row>
     <row r="16" spans="1:36" s="56" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="83"/>
-      <c r="B16" s="87"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
-      <c r="H16" s="101"/>
-      <c r="I16" s="101"/>
-      <c r="J16" s="101"/>
-      <c r="K16" s="101"/>
-      <c r="L16" s="101"/>
-      <c r="M16" s="102"/>
-      <c r="N16" s="103" t="s">
+      <c r="A16" s="98"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="103"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="79"/>
+      <c r="J16" s="79"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="79"/>
+      <c r="M16" s="80"/>
+      <c r="N16" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="O16" s="104"/>
-      <c r="P16" s="104"/>
-      <c r="Q16" s="105"/>
-      <c r="R16" s="103" t="s">
+      <c r="O16" s="72"/>
+      <c r="P16" s="72"/>
+      <c r="Q16" s="81"/>
+      <c r="R16" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="S16" s="104"/>
-      <c r="T16" s="104"/>
-      <c r="U16" s="105"/>
-      <c r="V16" s="106" t="s">
+      <c r="S16" s="72"/>
+      <c r="T16" s="72"/>
+      <c r="U16" s="81"/>
+      <c r="V16" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="W16" s="89" t="s">
+      <c r="W16" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="X16" s="76" t="s">
+      <c r="X16" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="Y16" s="108" t="s">
+      <c r="Y16" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="Z16" s="78" t="s">
+      <c r="Z16" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="AA16" s="74" t="s">
+      <c r="AA16" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="AB16" s="75"/>
-      <c r="AC16" s="76" t="s">
+      <c r="AB16" s="93"/>
+      <c r="AC16" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="AD16" s="76" t="s">
+      <c r="AD16" s="67" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:30" s="61" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="84"/>
+      <c r="A17" s="99"/>
       <c r="B17" s="58" t="s">
         <v>28</v>
       </c>
@@ -2122,21 +2122,21 @@
       <c r="U17" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V17" s="107"/>
-      <c r="W17" s="90"/>
-      <c r="X17" s="77"/>
-      <c r="Y17" s="109"/>
-      <c r="Z17" s="79"/>
+      <c r="V17" s="83"/>
+      <c r="W17" s="105"/>
+      <c r="X17" s="68"/>
+      <c r="Y17" s="70"/>
+      <c r="Z17" s="95"/>
       <c r="AA17" s="54" t="s">
         <v>61</v>
       </c>
       <c r="AB17" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="AC17" s="77"/>
-      <c r="AD17" s="77"/>
-    </row>
-    <row r="18" spans="1:30" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AC17" s="68"/>
+      <c r="AD17" s="68"/>
+    </row>
+    <row r="18" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>43</v>
       </c>
@@ -2174,20 +2174,20 @@
       <c r="AC18" s="65"/>
       <c r="AD18" s="65"/>
     </row>
-    <row r="19" spans="1:30" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="110" t="s">
+    <row r="19" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="110"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="110"/>
-      <c r="E19" s="110"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
       <c r="F19" s="43"/>
       <c r="H19" s="12"/>
-      <c r="L19" s="80" t="s">
+      <c r="L19" s="96" t="s">
         <v>50</v>
       </c>
-      <c r="M19" s="80"/>
+      <c r="M19" s="96"/>
       <c r="N19" s="47"/>
       <c r="O19" s="48"/>
       <c r="P19" s="49"/>
@@ -2207,46 +2207,46 @@
       <c r="AD19" s="65"/>
     </row>
     <row r="20" spans="1:30" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="113" t="s">
+      <c r="A20" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="113"/>
-      <c r="C20" s="113"/>
-      <c r="D20" s="113"/>
-      <c r="E20" s="113"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
       <c r="H20" s="12"/>
-      <c r="L20" s="81" t="s">
+      <c r="L20" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="M20" s="81"/>
-      <c r="N20" s="68"/>
-      <c r="O20" s="69"/>
-      <c r="P20" s="69"/>
-      <c r="Q20" s="69"/>
-      <c r="R20" s="69"/>
-      <c r="S20" s="69"/>
-      <c r="T20" s="69"/>
-      <c r="U20" s="69"/>
-      <c r="V20" s="70"/>
+      <c r="M20" s="74"/>
+      <c r="N20" s="86"/>
+      <c r="O20" s="87"/>
+      <c r="P20" s="87"/>
+      <c r="Q20" s="87"/>
+      <c r="R20" s="87"/>
+      <c r="S20" s="87"/>
+      <c r="T20" s="87"/>
+      <c r="U20" s="87"/>
+      <c r="V20" s="88"/>
       <c r="W20" s="50"/>
     </row>
     <row r="21" spans="1:30" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="H21" s="12"/>
-      <c r="L21" s="81" t="s">
+      <c r="L21" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="M21" s="81"/>
-      <c r="N21" s="68"/>
-      <c r="O21" s="69"/>
-      <c r="P21" s="69"/>
-      <c r="Q21" s="69"/>
-      <c r="R21" s="69"/>
-      <c r="S21" s="69"/>
-      <c r="T21" s="69"/>
-      <c r="U21" s="69"/>
-      <c r="V21" s="69"/>
-      <c r="W21" s="70"/>
+      <c r="M21" s="74"/>
+      <c r="N21" s="86"/>
+      <c r="O21" s="87"/>
+      <c r="P21" s="87"/>
+      <c r="Q21" s="87"/>
+      <c r="R21" s="87"/>
+      <c r="S21" s="87"/>
+      <c r="T21" s="87"/>
+      <c r="U21" s="87"/>
+      <c r="V21" s="87"/>
+      <c r="W21" s="88"/>
     </row>
     <row r="22" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
@@ -2260,11 +2260,11 @@
       <c r="Y22" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="Z22" s="93"/>
-      <c r="AA22" s="94"/>
-      <c r="AB22" s="94"/>
-      <c r="AC22" s="94"/>
-      <c r="AD22" s="95"/>
+      <c r="Z22" s="106"/>
+      <c r="AA22" s="107"/>
+      <c r="AB22" s="107"/>
+      <c r="AC22" s="107"/>
+      <c r="AD22" s="108"/>
     </row>
     <row r="23" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
@@ -2278,26 +2278,38 @@
       <c r="Y23" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="Z23" s="96"/>
-      <c r="AA23" s="97"/>
-      <c r="AB23" s="97"/>
-      <c r="AC23" s="97"/>
-      <c r="AD23" s="98"/>
+      <c r="Z23" s="109"/>
+      <c r="AA23" s="110"/>
+      <c r="AB23" s="110"/>
+      <c r="AC23" s="110"/>
+      <c r="AD23" s="111"/>
     </row>
     <row r="25" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="67"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
+      <c r="A25" s="84"/>
+      <c r="B25" s="84"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="X16:X17"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="X15:Z15"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="Z22:AD22"/>
+    <mergeCell ref="Z23:AD23"/>
+    <mergeCell ref="AA15:AD15"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="AC16:AC17"/>
+    <mergeCell ref="AD16:AD17"/>
+    <mergeCell ref="Z16:Z17"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="N20:V20"/>
+    <mergeCell ref="N21:W21"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="W16:W17"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="D15:M16"/>
@@ -2314,23 +2326,11 @@
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="N20:V20"/>
-    <mergeCell ref="N21:W21"/>
-    <mergeCell ref="AA15:AD15"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="AC16:AC17"/>
-    <mergeCell ref="AD16:AD17"/>
-    <mergeCell ref="Z16:Z17"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="W16:W17"/>
-    <mergeCell ref="Z22:AD22"/>
-    <mergeCell ref="Z23:AD23"/>
+    <mergeCell ref="X16:X17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="X15:Z15"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="L21:M21"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2359,33 +2359,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111"/>
-      <c r="S1" s="111"/>
-      <c r="T1" s="111"/>
-      <c r="U1" s="111"/>
-      <c r="V1" s="111"/>
-      <c r="W1" s="111"/>
-      <c r="X1" s="111"/>
-      <c r="Y1" s="111"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
+      <c r="U1" s="112"/>
+      <c r="V1" s="112"/>
+      <c r="W1" s="112"/>
+      <c r="X1" s="112"/>
+      <c r="Y1" s="112"/>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
       <c r="AL1" s="1"/>
@@ -2406,62 +2406,62 @@
       <c r="BA1" s="1"/>
     </row>
     <row r="2" spans="1:53" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="113" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="112"/>
-      <c r="P2" s="112"/>
-      <c r="Q2" s="112"/>
-      <c r="R2" s="112"/>
-      <c r="S2" s="112"/>
-      <c r="T2" s="112"/>
-      <c r="U2" s="112"/>
-      <c r="V2" s="112"/>
-      <c r="W2" s="112"/>
-      <c r="X2" s="112"/>
-      <c r="Y2" s="112"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="113"/>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="113"/>
+      <c r="U2" s="113"/>
+      <c r="V2" s="113"/>
+      <c r="W2" s="113"/>
+      <c r="X2" s="113"/>
+      <c r="Y2" s="113"/>
     </row>
     <row r="3" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="112" t="s">
+      <c r="A3" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
-      <c r="J3" s="112"/>
-      <c r="K3" s="112"/>
-      <c r="L3" s="112"/>
-      <c r="M3" s="112"/>
-      <c r="N3" s="112"/>
-      <c r="O3" s="112"/>
-      <c r="P3" s="112"/>
-      <c r="Q3" s="112"/>
-      <c r="R3" s="112"/>
-      <c r="S3" s="112"/>
-      <c r="T3" s="112"/>
-      <c r="U3" s="112"/>
-      <c r="V3" s="112"/>
-      <c r="W3" s="112"/>
-      <c r="X3" s="112"/>
-      <c r="Y3" s="112"/>
+      <c r="B3" s="113"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="113"/>
+      <c r="J3" s="113"/>
+      <c r="K3" s="113"/>
+      <c r="L3" s="113"/>
+      <c r="M3" s="113"/>
+      <c r="N3" s="113"/>
+      <c r="O3" s="113"/>
+      <c r="P3" s="113"/>
+      <c r="Q3" s="113"/>
+      <c r="R3" s="113"/>
+      <c r="S3" s="113"/>
+      <c r="T3" s="113"/>
+      <c r="U3" s="113"/>
+      <c r="V3" s="113"/>
+      <c r="W3" s="113"/>
+      <c r="X3" s="113"/>
+      <c r="Y3" s="113"/>
     </row>
     <row r="4" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="4"/>
@@ -2476,18 +2476,18 @@
     <row r="5" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="E5" s="91" t="s">
+      <c r="E5" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="92" t="s">
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -2501,18 +2501,18 @@
       <c r="B6" s="4"/>
       <c r="C6" s="18"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="91" t="s">
+      <c r="E6" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="91"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="91"/>
-      <c r="I6" s="91"/>
-      <c r="J6" s="92" t="s">
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="92"/>
-      <c r="L6" s="92"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -2542,18 +2542,18 @@
       <c r="A7" s="6"/>
       <c r="B7" s="4"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="91" t="s">
+      <c r="E7" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="91"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="91"/>
-      <c r="I7" s="91"/>
-      <c r="J7" s="92" t="s">
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="92"/>
-      <c r="L7" s="92"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="76"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -2662,18 +2662,18 @@
     <row r="11" spans="1:53" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="91" t="s">
+      <c r="E11" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="91"/>
-      <c r="G11" s="91"/>
-      <c r="H11" s="91"/>
-      <c r="I11" s="91"/>
-      <c r="J11" s="92" t="s">
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="92"/>
-      <c r="L11" s="92"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
       <c r="N11" s="13"/>
     </row>
     <row r="12" spans="1:53" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2693,27 +2693,22 @@
     <row r="13" spans="1:53" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="91" t="s">
+      <c r="E13" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="91"/>
-      <c r="G13" s="91"/>
-      <c r="H13" s="91"/>
-      <c r="I13" s="91"/>
-      <c r="J13" s="92" t="s">
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="92"/>
-      <c r="L13" s="92"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
       <c r="N13" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="A2:Y2"/>
-    <mergeCell ref="A3:Y3"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J6:L6"/>
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="J13:L13"/>
@@ -2722,6 +2717,11 @@
     <mergeCell ref="E7:I7"/>
     <mergeCell ref="E11:I11"/>
     <mergeCell ref="E13:I13"/>
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="A2:Y2"/>
+    <mergeCell ref="A3:Y3"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2730,6 +2730,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B7BBE98651F7A43AC7BF2F06836443C" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b51c7281b06024c9ff887df9fe3bb465">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8103b6e4-b1cc-417b-af38-f980b3f4bdef" xmlns:ns3="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c056a6abdadb071051b2c083c327215c" ns2:_="" ns3:_="">
     <xsd:import namespace="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
@@ -2946,15 +2955,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2967,6 +2967,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E02BC65-B354-4988-8893-F98AC7F212AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2985,14 +2993,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
fix: MCCC avec CC > 10
</commit_message>
<xml_diff>
--- a/public/modeles/Annexe_MCCC.xlsx
+++ b/public/modeles/Annexe_MCCC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8277C6D7-43D3-6448-BB07-A118C4C83392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13865CAD-EC2B-BC46-AB44-15F6CCB87D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modele" sheetId="9" r:id="rId1"/>
@@ -375,7 +375,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -821,19 +821,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -847,10 +834,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -861,14 +848,99 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -876,7 +948,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -916,13 +988,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1021,16 +1087,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1052,16 +1109,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1070,139 +1151,142 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1632,7 +1716,7 @@
   <dimension ref="A1:AJ25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N4" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="X15" sqref="X15:Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1650,42 +1734,47 @@
     <col min="11" max="11" width="15.33203125" style="12" customWidth="1"/>
     <col min="12" max="12" width="17.33203125" customWidth="1"/>
     <col min="13" max="13" width="6.6640625" style="12" customWidth="1"/>
-    <col min="14" max="23" width="6.6640625" customWidth="1"/>
+    <col min="14" max="16" width="6.6640625" customWidth="1"/>
+    <col min="17" max="17" width="8" customWidth="1"/>
+    <col min="18" max="20" width="6.6640625" customWidth="1"/>
+    <col min="21" max="21" width="7.83203125" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" customWidth="1"/>
+    <col min="23" max="23" width="8.33203125" customWidth="1"/>
     <col min="24" max="30" width="14.33203125" customWidth="1"/>
     <col min="31" max="32" width="5.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="45"/>
-      <c r="AB1" s="41"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="39"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
@@ -1696,83 +1785,83 @@
       <c r="AJ1" s="1"/>
     </row>
     <row r="2" spans="1:36" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
-      <c r="V2" s="46"/>
-      <c r="W2" s="46"/>
-      <c r="X2" s="46"/>
-      <c r="Y2" s="46"/>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="42"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="44"/>
+      <c r="W2" s="44"/>
+      <c r="X2" s="44"/>
+      <c r="Y2" s="44"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="40"/>
     </row>
     <row r="3" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="46"/>
-      <c r="S3" s="46"/>
-      <c r="T3" s="46"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="46"/>
-      <c r="Y3" s="46"/>
-      <c r="Z3" s="46"/>
-      <c r="AA3" s="46"/>
-      <c r="AB3" s="42"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="44"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="44"/>
+      <c r="X3" s="44"/>
+      <c r="Y3" s="44"/>
+      <c r="Z3" s="44"/>
+      <c r="AA3" s="44"/>
+      <c r="AB3" s="40"/>
     </row>
     <row r="4" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="75" t="s">
+      <c r="G5" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="76" t="s">
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="76"/>
-      <c r="L5" s="76"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1782,20 +1871,20 @@
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="18"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="75" t="s">
+      <c r="G6" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="76" t="s">
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="76"/>
-      <c r="L6" s="76"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1813,24 +1902,24 @@
     </row>
     <row r="7" spans="1:36" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="7"/>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="38" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="42" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="75" t="s">
+      <c r="G7" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="76" t="s">
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="76"/>
-      <c r="L7" s="76"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1842,10 +1931,10 @@
     <row r="8" spans="1:36" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="7"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="38"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="36"/>
       <c r="J8" s="6"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1868,20 +1957,20 @@
     <row r="9" spans="1:36" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="75" t="s">
+      <c r="G9" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="76" t="s">
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="76"/>
-      <c r="L9" s="76"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -1899,62 +1988,62 @@
     </row>
     <row r="10" spans="1:36" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D10" s="8"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="33"/>
       <c r="M10" s="14"/>
     </row>
     <row r="11" spans="1:36" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D11" s="5"/>
-      <c r="E11" s="44" t="s">
+      <c r="E11" s="42" t="s">
         <v>14</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="75" t="s">
+      <c r="G11" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="76" t="s">
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="76"/>
-      <c r="L11" s="76"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="72"/>
       <c r="M11" s="13"/>
     </row>
     <row r="12" spans="1:36" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="37"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="35"/>
       <c r="K12" s="13"/>
-      <c r="L12" s="35"/>
+      <c r="L12" s="33"/>
       <c r="M12" s="13"/>
     </row>
     <row r="13" spans="1:36" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D13" s="5"/>
-      <c r="E13" s="44" t="s">
+      <c r="E13" s="42" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="7"/>
-      <c r="G13" s="75" t="s">
+      <c r="G13" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="75"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="76" t="s">
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="76"/>
-      <c r="L13" s="76"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="72"/>
       <c r="M13" s="13"/>
     </row>
     <row r="14" spans="1:36" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1964,352 +2053,340 @@
       <c r="K14"/>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:36" s="56" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="97" t="s">
+    <row r="15" spans="1:36" s="51" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="100" t="s">
+      <c r="B15" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="101"/>
-      <c r="D15" s="77" t="s">
+      <c r="C15" s="84"/>
+      <c r="D15" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="77"/>
-      <c r="L15" s="77"/>
-      <c r="M15" s="78"/>
-      <c r="N15" s="71" t="s">
+      <c r="E15" s="88"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="88"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="88"/>
+      <c r="L15" s="88"/>
+      <c r="M15" s="89"/>
+      <c r="N15" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="72"/>
-      <c r="P15" s="72"/>
-      <c r="Q15" s="72"/>
-      <c r="R15" s="72"/>
-      <c r="S15" s="72"/>
-      <c r="T15" s="72"/>
-      <c r="U15" s="72"/>
-      <c r="V15" s="72"/>
-      <c r="W15" s="81"/>
-      <c r="X15" s="71" t="s">
+      <c r="O15" s="93"/>
+      <c r="P15" s="93"/>
+      <c r="Q15" s="93"/>
+      <c r="R15" s="93"/>
+      <c r="S15" s="93"/>
+      <c r="T15" s="93"/>
+      <c r="U15" s="93"/>
+      <c r="V15" s="93"/>
+      <c r="W15" s="109"/>
+      <c r="X15" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="Y15" s="72"/>
-      <c r="Z15" s="72"/>
-      <c r="AA15" s="89" t="s">
+      <c r="Y15" s="93"/>
+      <c r="Z15" s="109"/>
+      <c r="AA15" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="AB15" s="90"/>
-      <c r="AC15" s="90"/>
-      <c r="AD15" s="91"/>
-    </row>
-    <row r="16" spans="1:36" s="56" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="98"/>
-      <c r="B16" s="102"/>
-      <c r="C16" s="103"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="79"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="79"/>
-      <c r="K16" s="79"/>
-      <c r="L16" s="79"/>
-      <c r="M16" s="80"/>
-      <c r="N16" s="71" t="s">
+      <c r="AB15" s="67"/>
+      <c r="AC15" s="67"/>
+      <c r="AD15" s="68"/>
+    </row>
+    <row r="16" spans="1:36" s="51" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="81"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="90"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="90"/>
+      <c r="J16" s="90"/>
+      <c r="K16" s="90"/>
+      <c r="L16" s="90"/>
+      <c r="M16" s="91"/>
+      <c r="N16" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="O16" s="72"/>
-      <c r="P16" s="72"/>
-      <c r="Q16" s="81"/>
-      <c r="R16" s="71" t="s">
+      <c r="O16" s="93"/>
+      <c r="P16" s="93"/>
+      <c r="Q16" s="94"/>
+      <c r="R16" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="S16" s="72"/>
-      <c r="T16" s="72"/>
-      <c r="U16" s="81"/>
-      <c r="V16" s="82" t="s">
+      <c r="S16" s="93"/>
+      <c r="T16" s="93"/>
+      <c r="U16" s="94"/>
+      <c r="V16" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="W16" s="104" t="s">
+      <c r="W16" s="114" t="s">
         <v>64</v>
       </c>
-      <c r="X16" s="67" t="s">
+      <c r="X16" s="110" t="s">
         <v>58</v>
       </c>
-      <c r="Y16" s="69" t="s">
+      <c r="Y16" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="Z16" s="94" t="s">
+      <c r="Z16" s="107" t="s">
         <v>55</v>
       </c>
-      <c r="AA16" s="92" t="s">
+      <c r="AA16" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="AB16" s="93"/>
-      <c r="AC16" s="67" t="s">
+      <c r="AB16" s="69"/>
+      <c r="AC16" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="AD16" s="67" t="s">
+      <c r="AD16" s="70" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="61" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="99"/>
-      <c r="B17" s="58" t="s">
+    <row r="17" spans="1:30" s="56" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="82"/>
+      <c r="B17" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="58" t="s">
+      <c r="D17" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="57" t="s">
+      <c r="E17" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="57" t="s">
+      <c r="F17" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="59" t="s">
+      <c r="G17" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="59" t="s">
+      <c r="H17" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="59" t="s">
+      <c r="I17" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="59" t="s">
+      <c r="J17" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="59" t="s">
+      <c r="K17" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="L17" s="59" t="s">
+      <c r="L17" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="M17" s="60" t="s">
+      <c r="M17" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="N17" s="15" t="s">
+      <c r="N17" s="116" t="s">
         <v>38</v>
       </c>
-      <c r="O17" s="17" t="s">
+      <c r="O17" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="P17" s="16" t="s">
+      <c r="P17" s="15" t="s">
         <v>40</v>
       </c>
       <c r="Q17" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="R17" s="15" t="s">
+      <c r="R17" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="S17" s="17" t="s">
+      <c r="S17" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="T17" s="16" t="s">
+      <c r="T17" s="15" t="s">
         <v>40</v>
       </c>
       <c r="U17" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="V17" s="83"/>
-      <c r="W17" s="105"/>
-      <c r="X17" s="68"/>
-      <c r="Y17" s="70"/>
-      <c r="Z17" s="95"/>
-      <c r="AA17" s="54" t="s">
+      <c r="V17" s="96"/>
+      <c r="W17" s="115"/>
+      <c r="X17" s="111"/>
+      <c r="Y17" s="98"/>
+      <c r="Z17" s="108"/>
+      <c r="AA17" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="AB17" s="55" t="s">
+      <c r="AB17" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="AC17" s="68"/>
-      <c r="AD17" s="68"/>
+      <c r="AC17" s="71"/>
+      <c r="AD17" s="71"/>
     </row>
     <row r="18" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="20">
         <v>11</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="24">
+      <c r="C18" s="21"/>
+      <c r="D18" s="22">
         <v>1</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="30"/>
-      <c r="T18" s="23"/>
-      <c r="U18" s="26"/>
-      <c r="V18" s="26"/>
-      <c r="W18" s="26"/>
-      <c r="X18" s="53"/>
-      <c r="Y18" s="62"/>
-      <c r="Z18" s="53"/>
-      <c r="AA18" s="63"/>
-      <c r="AB18" s="64"/>
-      <c r="AC18" s="65"/>
-      <c r="AD18" s="65"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="26"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="112"/>
+      <c r="X18" s="57"/>
+      <c r="Y18" s="57"/>
+      <c r="Z18" s="105"/>
+      <c r="AA18" s="104"/>
+      <c r="AB18" s="58"/>
+      <c r="AC18" s="59"/>
+      <c r="AD18" s="59"/>
     </row>
     <row r="19" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="73" t="s">
+      <c r="A19" s="99" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="43"/>
+      <c r="B19" s="99"/>
+      <c r="C19" s="99"/>
+      <c r="D19" s="99"/>
+      <c r="E19" s="99"/>
+      <c r="F19" s="41"/>
       <c r="H19" s="12"/>
-      <c r="L19" s="96" t="s">
+      <c r="L19" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="M19" s="96"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="48"/>
-      <c r="P19" s="49"/>
-      <c r="Q19" s="50"/>
-      <c r="R19" s="47"/>
-      <c r="S19" s="48"/>
-      <c r="T19" s="49"/>
-      <c r="U19" s="50"/>
-      <c r="V19" s="51"/>
-      <c r="W19" s="52"/>
-      <c r="X19" s="53"/>
-      <c r="Y19" s="62"/>
-      <c r="Z19" s="66"/>
-      <c r="AA19" s="63"/>
-      <c r="AB19" s="64"/>
-      <c r="AC19" s="65"/>
-      <c r="AD19" s="65"/>
+      <c r="M19" s="78"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="46"/>
+      <c r="P19" s="47"/>
+      <c r="Q19" s="48"/>
+      <c r="R19" s="45"/>
+      <c r="S19" s="46"/>
+      <c r="T19" s="47"/>
+      <c r="U19" s="48"/>
+      <c r="V19" s="49"/>
+      <c r="W19" s="113"/>
+      <c r="X19" s="57"/>
+      <c r="Y19" s="57"/>
+      <c r="Z19" s="106"/>
+      <c r="AA19" s="104"/>
+      <c r="AB19" s="58"/>
+      <c r="AC19" s="59"/>
+      <c r="AD19" s="59"/>
     </row>
     <row r="20" spans="1:30" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="85" t="s">
+      <c r="A20" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="85"/>
-      <c r="C20" s="85"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="85"/>
+      <c r="B20" s="74"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
       <c r="H20" s="12"/>
-      <c r="L20" s="74" t="s">
+      <c r="L20" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="M20" s="74"/>
-      <c r="N20" s="86"/>
-      <c r="O20" s="87"/>
-      <c r="P20" s="87"/>
-      <c r="Q20" s="87"/>
-      <c r="R20" s="87"/>
-      <c r="S20" s="87"/>
-      <c r="T20" s="87"/>
-      <c r="U20" s="87"/>
-      <c r="V20" s="88"/>
-      <c r="W20" s="50"/>
+      <c r="M20" s="79"/>
+      <c r="N20" s="75"/>
+      <c r="O20" s="76"/>
+      <c r="P20" s="76"/>
+      <c r="Q20" s="76"/>
+      <c r="R20" s="76"/>
+      <c r="S20" s="76"/>
+      <c r="T20" s="76"/>
+      <c r="U20" s="76"/>
+      <c r="V20" s="77"/>
+      <c r="W20" s="48"/>
     </row>
     <row r="21" spans="1:30" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="H21" s="12"/>
-      <c r="L21" s="74" t="s">
+      <c r="L21" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="M21" s="74"/>
-      <c r="N21" s="86"/>
-      <c r="O21" s="87"/>
-      <c r="P21" s="87"/>
-      <c r="Q21" s="87"/>
-      <c r="R21" s="87"/>
-      <c r="S21" s="87"/>
-      <c r="T21" s="87"/>
-      <c r="U21" s="87"/>
-      <c r="V21" s="87"/>
-      <c r="W21" s="88"/>
+      <c r="M21" s="79"/>
+      <c r="N21" s="75"/>
+      <c r="O21" s="76"/>
+      <c r="P21" s="76"/>
+      <c r="Q21" s="76"/>
+      <c r="R21" s="76"/>
+      <c r="S21" s="76"/>
+      <c r="T21" s="76"/>
+      <c r="U21" s="76"/>
+      <c r="V21" s="76"/>
+      <c r="W21" s="77"/>
     </row>
     <row r="22" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="33"/>
+      <c r="E22" s="31"/>
       <c r="H22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22"/>
-      <c r="Y22" s="20" t="s">
+      <c r="Y22" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="Z22" s="106"/>
-      <c r="AA22" s="107"/>
-      <c r="AB22" s="107"/>
-      <c r="AC22" s="107"/>
-      <c r="AD22" s="108"/>
+      <c r="Z22" s="61"/>
+      <c r="AA22" s="62"/>
+      <c r="AB22" s="62"/>
+      <c r="AC22" s="62"/>
+      <c r="AD22" s="63"/>
     </row>
     <row r="23" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="34"/>
+      <c r="E23" s="32"/>
       <c r="H23" s="12"/>
       <c r="L23" s="12"/>
       <c r="M23"/>
-      <c r="Y23" s="20" t="s">
+      <c r="Y23" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="Z23" s="109"/>
-      <c r="AA23" s="110"/>
-      <c r="AB23" s="110"/>
-      <c r="AC23" s="110"/>
-      <c r="AD23" s="111"/>
+      <c r="Z23" s="64"/>
+      <c r="AA23" s="65"/>
+      <c r="AB23" s="65"/>
+      <c r="AC23" s="65"/>
+      <c r="AD23" s="66"/>
     </row>
     <row r="25" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="84"/>
-      <c r="B25" s="84"/>
-      <c r="C25" s="84"/>
-      <c r="D25" s="84"/>
-      <c r="E25" s="84"/>
+      <c r="A25" s="73"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="Z22:AD22"/>
-    <mergeCell ref="Z23:AD23"/>
-    <mergeCell ref="AA15:AD15"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="AC16:AC17"/>
-    <mergeCell ref="AD16:AD17"/>
-    <mergeCell ref="Z16:Z17"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="N20:V20"/>
-    <mergeCell ref="N21:W21"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="X16:X17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="X15:Z15"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="L21:M21"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="D15:M16"/>
@@ -2326,11 +2403,23 @@
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="J9:L9"/>
-    <mergeCell ref="X16:X17"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="X15:Z15"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="N20:V20"/>
+    <mergeCell ref="N21:W21"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="Z22:AD22"/>
+    <mergeCell ref="Z23:AD23"/>
+    <mergeCell ref="AA15:AD15"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="AC16:AC17"/>
+    <mergeCell ref="AD16:AD17"/>
+    <mergeCell ref="Z16:Z17"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2359,33 +2448,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="112"/>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="112"/>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
-      <c r="U1" s="112"/>
-      <c r="V1" s="112"/>
-      <c r="W1" s="112"/>
-      <c r="X1" s="112"/>
-      <c r="Y1" s="112"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="100"/>
+      <c r="P1" s="100"/>
+      <c r="Q1" s="100"/>
+      <c r="R1" s="100"/>
+      <c r="S1" s="100"/>
+      <c r="T1" s="100"/>
+      <c r="U1" s="100"/>
+      <c r="V1" s="100"/>
+      <c r="W1" s="100"/>
+      <c r="X1" s="100"/>
+      <c r="Y1" s="100"/>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
       <c r="AL1" s="1"/>
@@ -2406,62 +2495,62 @@
       <c r="BA1" s="1"/>
     </row>
     <row r="2" spans="1:53" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="101" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="113"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
-      <c r="P2" s="113"/>
-      <c r="Q2" s="113"/>
-      <c r="R2" s="113"/>
-      <c r="S2" s="113"/>
-      <c r="T2" s="113"/>
-      <c r="U2" s="113"/>
-      <c r="V2" s="113"/>
-      <c r="W2" s="113"/>
-      <c r="X2" s="113"/>
-      <c r="Y2" s="113"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="101"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="101"/>
+      <c r="S2" s="101"/>
+      <c r="T2" s="101"/>
+      <c r="U2" s="101"/>
+      <c r="V2" s="101"/>
+      <c r="W2" s="101"/>
+      <c r="X2" s="101"/>
+      <c r="Y2" s="101"/>
     </row>
     <row r="3" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="113" t="s">
+      <c r="A3" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="113"/>
-      <c r="C3" s="113"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="113"/>
-      <c r="F3" s="113"/>
-      <c r="G3" s="113"/>
-      <c r="H3" s="113"/>
-      <c r="I3" s="113"/>
-      <c r="J3" s="113"/>
-      <c r="K3" s="113"/>
-      <c r="L3" s="113"/>
-      <c r="M3" s="113"/>
-      <c r="N3" s="113"/>
-      <c r="O3" s="113"/>
-      <c r="P3" s="113"/>
-      <c r="Q3" s="113"/>
-      <c r="R3" s="113"/>
-      <c r="S3" s="113"/>
-      <c r="T3" s="113"/>
-      <c r="U3" s="113"/>
-      <c r="V3" s="113"/>
-      <c r="W3" s="113"/>
-      <c r="X3" s="113"/>
-      <c r="Y3" s="113"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
+      <c r="O3" s="101"/>
+      <c r="P3" s="101"/>
+      <c r="Q3" s="101"/>
+      <c r="R3" s="101"/>
+      <c r="S3" s="101"/>
+      <c r="T3" s="101"/>
+      <c r="U3" s="101"/>
+      <c r="V3" s="101"/>
+      <c r="W3" s="101"/>
+      <c r="X3" s="101"/>
+      <c r="Y3" s="101"/>
     </row>
     <row r="4" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="4"/>
@@ -2476,18 +2565,18 @@
     <row r="5" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="76" t="s">
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="76"/>
-      <c r="L5" s="76"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -2499,20 +2588,20 @@
     </row>
     <row r="6" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
-      <c r="C6" s="18"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="75" t="s">
+      <c r="E6" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="76" t="s">
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="76"/>
-      <c r="L6" s="76"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -2542,18 +2631,18 @@
       <c r="A7" s="6"/>
       <c r="B7" s="4"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="75" t="s">
+      <c r="E7" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="76" t="s">
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="76"/>
-      <c r="L7" s="76"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -2574,11 +2663,11 @@
       <c r="B8" s="4"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="38"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="36"/>
       <c r="J8" s="6"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -2619,11 +2708,11 @@
       <c r="A9" s="10"/>
       <c r="B9" s="4"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="19"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="17"/>
       <c r="J9" s="6"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -2649,43 +2738,43 @@
       <c r="B10" s="4"/>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
       <c r="N10" s="14"/>
     </row>
     <row r="11" spans="1:53" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="76" t="s">
+      <c r="F11" s="87"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="76"/>
-      <c r="L11" s="76"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="72"/>
       <c r="N11" s="13"/>
     </row>
     <row r="12" spans="1:53" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="37"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="35"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="N12" s="13"/>
@@ -2693,22 +2782,27 @@
     <row r="13" spans="1:53" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="75" t="s">
+      <c r="E13" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="76" t="s">
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="76"/>
-      <c r="L13" s="76"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="72"/>
       <c r="N13" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="A2:Y2"/>
+    <mergeCell ref="A3:Y3"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="J13:L13"/>
@@ -2717,11 +2811,6 @@
     <mergeCell ref="E7:I7"/>
     <mergeCell ref="E11:I11"/>
     <mergeCell ref="E13:I13"/>
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="A2:Y2"/>
-    <mergeCell ref="A3:Y3"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J6:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2739,6 +2828,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B7BBE98651F7A43AC7BF2F06836443C" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b51c7281b06024c9ff887df9fe3bb465">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8103b6e4-b1cc-417b-af38-f980b3f4bdef" xmlns:ns3="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c056a6abdadb071051b2c083c327215c" ns2:_="" ns3:_="">
     <xsd:import namespace="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
@@ -2955,17 +3055,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
   <ds:schemaRefs>
@@ -2975,6 +3064,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
+    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E02BC65-B354-4988-8893-F98AC7F212AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2991,15 +3091,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
-    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: Inversion colonne MCCC
</commit_message>
<xml_diff>
--- a/public/modeles/Annexe_MCCC.xlsx
+++ b/public/modeles/Annexe_MCCC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9D8359-569C-B04D-B384-EEE926D6B643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E69F1B-46EE-584B-BE7B-E3048AA0311E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modele" sheetId="9" r:id="rId1"/>
@@ -142,9 +142,6 @@
 O / N</t>
   </si>
   <si>
-    <t>Type d'enseignement</t>
-  </si>
-  <si>
     <t>Cours mutualisé
 O / N</t>
   </si>
@@ -259,6 +256,10 @@
   </si>
   <si>
     <t>DO : Dossier; EM : Ecrit sur machine; ET : Ecrit terminal; ENT : Evaluation de l'entreprise; EP : Examen pratique; OET : Oral + écrit terminaux; OT : Oral terminal; ST : Soutenance; SDO : Soutenance sur dossier; TM : Travail sur machine; VMA-VCFA : Validation par le maître d'apprentissage et le formateur référent du CFA. CCr : Note globale de CC de première session conservée. TPr : Note globale de TP de première session conservée.</t>
+  </si>
+  <si>
+    <t>Type 
+d'enseignement</t>
   </si>
 </sst>
 </file>
@@ -1259,6 +1260,105 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1277,9 +1377,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1290,9 +1387,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1301,12 +1395,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1318,93 +1406,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1885,8 +1886,8 @@
   </sheetPr>
   <dimension ref="A1:AJ27"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:E27"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1900,8 +1901,8 @@
     <col min="7" max="7" width="36.33203125" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="11" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="14" style="11" customWidth="1"/>
+    <col min="11" max="11" width="17" style="11" customWidth="1"/>
     <col min="12" max="12" width="17.33203125" customWidth="1"/>
     <col min="13" max="13" width="6.6640625" style="11" customWidth="1"/>
     <col min="14" max="16" width="6.6640625" customWidth="1"/>
@@ -1915,38 +1916,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="82"/>
-      <c r="AA1" s="82"/>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="82"/>
-      <c r="AD1" s="82"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
+      <c r="AB1" s="115"/>
+      <c r="AC1" s="115"/>
+      <c r="AD1" s="115"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
@@ -1955,87 +1956,87 @@
       <c r="AJ1" s="1"/>
     </row>
     <row r="2" spans="1:36" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="83"/>
-      <c r="S2" s="83"/>
-      <c r="T2" s="83"/>
-      <c r="U2" s="83"/>
-      <c r="V2" s="83"/>
-      <c r="W2" s="83"/>
-      <c r="X2" s="83"/>
-      <c r="Y2" s="83"/>
-      <c r="Z2" s="83"/>
-      <c r="AA2" s="83"/>
-      <c r="AB2" s="83"/>
-      <c r="AC2" s="83"/>
-      <c r="AD2" s="83"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
+      <c r="M2" s="116"/>
+      <c r="N2" s="116"/>
+      <c r="O2" s="116"/>
+      <c r="P2" s="116"/>
+      <c r="Q2" s="116"/>
+      <c r="R2" s="116"/>
+      <c r="S2" s="116"/>
+      <c r="T2" s="116"/>
+      <c r="U2" s="116"/>
+      <c r="V2" s="116"/>
+      <c r="W2" s="116"/>
+      <c r="X2" s="116"/>
+      <c r="Y2" s="116"/>
+      <c r="Z2" s="116"/>
+      <c r="AA2" s="116"/>
+      <c r="AB2" s="116"/>
+      <c r="AC2" s="116"/>
+      <c r="AD2" s="116"/>
     </row>
     <row r="3" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
-      <c r="Q3" s="83"/>
-      <c r="R3" s="83"/>
-      <c r="S3" s="83"/>
-      <c r="T3" s="83"/>
-      <c r="U3" s="83"/>
-      <c r="V3" s="83"/>
-      <c r="W3" s="83"/>
-      <c r="X3" s="83"/>
-      <c r="Y3" s="83"/>
-      <c r="Z3" s="83"/>
-      <c r="AA3" s="83"/>
-      <c r="AB3" s="83"/>
-      <c r="AC3" s="83"/>
-      <c r="AD3" s="83"/>
+      <c r="B3" s="116"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="116"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="116"/>
+      <c r="I3" s="116"/>
+      <c r="J3" s="116"/>
+      <c r="K3" s="116"/>
+      <c r="L3" s="116"/>
+      <c r="M3" s="116"/>
+      <c r="N3" s="116"/>
+      <c r="O3" s="116"/>
+      <c r="P3" s="116"/>
+      <c r="Q3" s="116"/>
+      <c r="R3" s="116"/>
+      <c r="S3" s="116"/>
+      <c r="T3" s="116"/>
+      <c r="U3" s="116"/>
+      <c r="V3" s="116"/>
+      <c r="W3" s="116"/>
+      <c r="X3" s="116"/>
+      <c r="Y3" s="116"/>
+      <c r="Z3" s="116"/>
+      <c r="AA3" s="116"/>
+      <c r="AB3" s="116"/>
+      <c r="AC3" s="116"/>
+      <c r="AD3" s="116"/>
     </row>
     <row r="4" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="92" t="s">
+      <c r="G5" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="93" t="s">
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
+      <c r="K5" s="110"/>
+      <c r="L5" s="110"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -2049,16 +2050,16 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="92" t="s">
+      <c r="G6" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="93" t="s">
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
+      <c r="K6" s="110"/>
+      <c r="L6" s="110"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -2084,16 +2085,16 @@
         <v>8</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="92" t="s">
+      <c r="G7" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="93" t="s">
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="93"/>
-      <c r="L7" s="93"/>
+      <c r="K7" s="110"/>
+      <c r="L7" s="110"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -2135,16 +2136,16 @@
         <v>11</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="92" t="s">
+      <c r="G9" s="109" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="92"/>
-      <c r="I9" s="92"/>
-      <c r="J9" s="93" t="s">
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="93"/>
-      <c r="L9" s="93"/>
+      <c r="K9" s="110"/>
+      <c r="L9" s="110"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -2178,16 +2179,16 @@
         <v>14</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="92" t="s">
+      <c r="G11" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
-      <c r="J11" s="93" t="s">
+      <c r="H11" s="109"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="93"/>
-      <c r="L11" s="93"/>
+      <c r="K11" s="110"/>
+      <c r="L11" s="110"/>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:36" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2208,16 +2209,16 @@
         <v>17</v>
       </c>
       <c r="F13" s="7"/>
-      <c r="G13" s="92" t="s">
+      <c r="G13" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="92"/>
-      <c r="I13" s="92"/>
-      <c r="J13" s="93" t="s">
+      <c r="H13" s="109"/>
+      <c r="I13" s="109"/>
+      <c r="J13" s="110" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="93"/>
-      <c r="L13" s="93"/>
+      <c r="K13" s="110"/>
+      <c r="L13" s="110"/>
       <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:36" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2228,108 +2229,108 @@
       <c r="M14"/>
     </row>
     <row r="15" spans="1:36" s="39" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="103" t="s">
+      <c r="A15" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="106" t="s">
+      <c r="B15" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="107"/>
-      <c r="D15" s="94" t="s">
+      <c r="C15" s="85"/>
+      <c r="D15" s="123" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="94"/>
-      <c r="F15" s="94"/>
-      <c r="G15" s="94"/>
-      <c r="H15" s="94"/>
-      <c r="I15" s="94"/>
-      <c r="J15" s="94"/>
-      <c r="K15" s="94"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="95"/>
-      <c r="N15" s="98" t="s">
+      <c r="E15" s="123"/>
+      <c r="F15" s="123"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="123"/>
+      <c r="I15" s="123"/>
+      <c r="J15" s="123"/>
+      <c r="K15" s="123"/>
+      <c r="L15" s="123"/>
+      <c r="M15" s="124"/>
+      <c r="N15" s="106" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="89"/>
-      <c r="P15" s="89"/>
-      <c r="Q15" s="89"/>
-      <c r="R15" s="89"/>
-      <c r="S15" s="89"/>
-      <c r="T15" s="89"/>
-      <c r="U15" s="89"/>
-      <c r="V15" s="89"/>
-      <c r="W15" s="90"/>
-      <c r="X15" s="89" t="s">
+      <c r="O15" s="107"/>
+      <c r="P15" s="107"/>
+      <c r="Q15" s="107"/>
+      <c r="R15" s="107"/>
+      <c r="S15" s="107"/>
+      <c r="T15" s="107"/>
+      <c r="U15" s="107"/>
+      <c r="V15" s="107"/>
+      <c r="W15" s="121"/>
+      <c r="X15" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="Y15" s="89"/>
-      <c r="Z15" s="90"/>
-      <c r="AA15" s="112" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB15" s="112"/>
-      <c r="AC15" s="112"/>
-      <c r="AD15" s="113"/>
+      <c r="Y15" s="107"/>
+      <c r="Z15" s="121"/>
+      <c r="AA15" s="90" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB15" s="90"/>
+      <c r="AC15" s="90"/>
+      <c r="AD15" s="91"/>
     </row>
     <row r="16" spans="1:36" s="39" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="104"/>
-      <c r="B16" s="108"/>
-      <c r="C16" s="109"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="96"/>
-      <c r="I16" s="96"/>
-      <c r="J16" s="96"/>
-      <c r="K16" s="96"/>
-      <c r="L16" s="96"/>
-      <c r="M16" s="97"/>
-      <c r="N16" s="98" t="s">
+      <c r="A16" s="82"/>
+      <c r="B16" s="86"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="125"/>
+      <c r="E16" s="125"/>
+      <c r="F16" s="125"/>
+      <c r="G16" s="125"/>
+      <c r="H16" s="125"/>
+      <c r="I16" s="125"/>
+      <c r="J16" s="125"/>
+      <c r="K16" s="125"/>
+      <c r="L16" s="125"/>
+      <c r="M16" s="126"/>
+      <c r="N16" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="O16" s="89"/>
-      <c r="P16" s="89"/>
-      <c r="Q16" s="99"/>
-      <c r="R16" s="98" t="s">
+      <c r="O16" s="107"/>
+      <c r="P16" s="107"/>
+      <c r="Q16" s="108"/>
+      <c r="R16" s="106" t="s">
         <v>26</v>
       </c>
-      <c r="S16" s="89"/>
-      <c r="T16" s="89"/>
-      <c r="U16" s="99"/>
-      <c r="V16" s="125" t="s">
+      <c r="S16" s="107"/>
+      <c r="T16" s="107"/>
+      <c r="U16" s="108"/>
+      <c r="V16" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="W16" s="110" t="s">
-        <v>64</v>
-      </c>
-      <c r="X16" s="85" t="s">
+      <c r="W16" s="88" t="s">
+        <v>63</v>
+      </c>
+      <c r="X16" s="117" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y16" s="119" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z16" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA16" s="92" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB16" s="93"/>
+      <c r="AC16" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="Y16" s="87" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z16" s="118" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA16" s="114" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB16" s="115"/>
-      <c r="AC16" s="116" t="s">
+      <c r="AD16" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="AD16" s="116" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="17" spans="1:30" s="44" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="105"/>
+      <c r="A17" s="83"/>
       <c r="B17" s="41" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" s="41" t="s">
         <v>29</v>
@@ -2353,55 +2354,55 @@
         <v>35</v>
       </c>
       <c r="K17" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="L17" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="M17" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="L17" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="M17" s="43" t="s">
+      <c r="N17" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="N17" s="54" t="s">
+      <c r="O17" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="O17" s="55" t="s">
+      <c r="P17" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="P17" s="14" t="s">
+      <c r="Q17" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="Q17" s="10" t="s">
+      <c r="R17" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="S17" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="T17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="U17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="R17" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="S17" s="55" t="s">
-        <v>39</v>
-      </c>
-      <c r="T17" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="U17" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="V17" s="126"/>
-      <c r="W17" s="111"/>
-      <c r="X17" s="86"/>
-      <c r="Y17" s="88"/>
-      <c r="Z17" s="119"/>
+      <c r="V17" s="105"/>
+      <c r="W17" s="89"/>
+      <c r="X17" s="118"/>
+      <c r="Y17" s="120"/>
+      <c r="Z17" s="97"/>
       <c r="AA17" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB17" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="AB17" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC17" s="117"/>
-      <c r="AD17" s="117"/>
+      <c r="AC17" s="95"/>
+      <c r="AD17" s="95"/>
     </row>
     <row r="18" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="19">
         <v>11</v>
@@ -2438,19 +2439,19 @@
       <c r="AD18" s="47"/>
     </row>
     <row r="19" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="91" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="91"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="91"/>
-      <c r="E19" s="91"/>
+      <c r="A19" s="122" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="122"/>
+      <c r="C19" s="122"/>
+      <c r="D19" s="122"/>
+      <c r="E19" s="122"/>
       <c r="F19" s="36"/>
       <c r="H19" s="11"/>
-      <c r="L19" s="124" t="s">
-        <v>50</v>
-      </c>
-      <c r="M19" s="124"/>
+      <c r="L19" s="102" t="s">
+        <v>49</v>
+      </c>
+      <c r="M19" s="102"/>
       <c r="N19" s="64"/>
       <c r="O19" s="65"/>
       <c r="P19" s="66"/>
@@ -2470,63 +2471,63 @@
       <c r="AD19" s="47"/>
     </row>
     <row r="20" spans="1:30" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="120" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="120"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="120"/>
-      <c r="E20" s="120"/>
+      <c r="A20" s="98" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="98"/>
+      <c r="C20" s="98"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="98"/>
       <c r="H20" s="11"/>
-      <c r="L20" s="84" t="s">
-        <v>51</v>
-      </c>
-      <c r="M20" s="84"/>
-      <c r="N20" s="121"/>
-      <c r="O20" s="122"/>
-      <c r="P20" s="122"/>
-      <c r="Q20" s="122"/>
-      <c r="R20" s="122"/>
-      <c r="S20" s="122"/>
-      <c r="T20" s="122"/>
-      <c r="U20" s="122"/>
-      <c r="V20" s="123"/>
+      <c r="L20" s="103" t="s">
+        <v>50</v>
+      </c>
+      <c r="M20" s="103"/>
+      <c r="N20" s="99"/>
+      <c r="O20" s="100"/>
+      <c r="P20" s="100"/>
+      <c r="Q20" s="100"/>
+      <c r="R20" s="100"/>
+      <c r="S20" s="100"/>
+      <c r="T20" s="100"/>
+      <c r="U20" s="100"/>
+      <c r="V20" s="101"/>
       <c r="W20" s="67"/>
     </row>
     <row r="21" spans="1:30" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="H21" s="11"/>
-      <c r="L21" s="84" t="s">
-        <v>48</v>
-      </c>
-      <c r="M21" s="84"/>
-      <c r="N21" s="100"/>
-      <c r="O21" s="101"/>
-      <c r="P21" s="101"/>
-      <c r="Q21" s="101"/>
-      <c r="R21" s="101"/>
-      <c r="S21" s="101"/>
-      <c r="T21" s="101"/>
-      <c r="U21" s="101"/>
-      <c r="V21" s="101"/>
-      <c r="W21" s="102"/>
+      <c r="L21" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="M21" s="103"/>
+      <c r="N21" s="78"/>
+      <c r="O21" s="79"/>
+      <c r="P21" s="79"/>
+      <c r="Q21" s="79"/>
+      <c r="R21" s="79"/>
+      <c r="S21" s="79"/>
+      <c r="T21" s="79"/>
+      <c r="U21" s="79"/>
+      <c r="V21" s="79"/>
+      <c r="W21" s="80"/>
     </row>
     <row r="22" spans="1:30" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="H22" s="11"/>
-      <c r="L22" s="84" t="s">
-        <v>66</v>
-      </c>
-      <c r="M22" s="84"/>
-      <c r="N22" s="100"/>
-      <c r="O22" s="101"/>
-      <c r="P22" s="101"/>
-      <c r="Q22" s="101"/>
-      <c r="R22" s="101"/>
-      <c r="S22" s="101"/>
-      <c r="T22" s="101"/>
-      <c r="U22" s="101"/>
-      <c r="V22" s="102"/>
+      <c r="L22" s="103" t="s">
+        <v>65</v>
+      </c>
+      <c r="M22" s="103"/>
+      <c r="N22" s="78"/>
+      <c r="O22" s="79"/>
+      <c r="P22" s="79"/>
+      <c r="Q22" s="79"/>
+      <c r="R22" s="79"/>
+      <c r="S22" s="79"/>
+      <c r="T22" s="79"/>
+      <c r="U22" s="79"/>
+      <c r="V22" s="80"/>
       <c r="W22" s="67"/>
     </row>
     <row r="23" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2535,45 +2536,72 @@
     </row>
     <row r="24" spans="1:30" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C24" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D24" s="58"/>
       <c r="E24" s="59"/>
       <c r="Z24" s="11"/>
       <c r="AA24" s="61" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB24" s="79"/>
-      <c r="AC24" s="80"/>
-      <c r="AD24" s="81"/>
+        <v>44</v>
+      </c>
+      <c r="AB24" s="112"/>
+      <c r="AC24" s="113"/>
+      <c r="AD24" s="114"/>
     </row>
     <row r="25" spans="1:30" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25" s="57"/>
       <c r="E25" s="60"/>
       <c r="Z25" s="56"/>
       <c r="AA25" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB25" s="79"/>
-      <c r="AC25" s="80"/>
-      <c r="AD25" s="81"/>
+        <v>46</v>
+      </c>
+      <c r="AB25" s="112"/>
+      <c r="AC25" s="113"/>
+      <c r="AD25" s="114"/>
     </row>
     <row r="27" spans="1:30" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="78" t="s">
-        <v>73</v>
-      </c>
-      <c r="B27" s="78"/>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="78"/>
+      <c r="A27" s="111" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="111"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="111"/>
+      <c r="E27" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="AB25:AD25"/>
+    <mergeCell ref="A1:AD1"/>
+    <mergeCell ref="A2:AD2"/>
+    <mergeCell ref="A3:AD3"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="AB24:AD24"/>
+    <mergeCell ref="X16:X17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="X15:Z15"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="D15:M16"/>
+    <mergeCell ref="N15:W15"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G13:I13"/>
     <mergeCell ref="N22:V22"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:C16"/>
@@ -2590,33 +2618,6 @@
     <mergeCell ref="L20:M20"/>
     <mergeCell ref="V16:V17"/>
     <mergeCell ref="R16:U16"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="AB25:AD25"/>
-    <mergeCell ref="A1:AD1"/>
-    <mergeCell ref="A2:AD2"/>
-    <mergeCell ref="A3:AD3"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="AB24:AD24"/>
-    <mergeCell ref="X16:X17"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="X15:Z15"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="D15:M16"/>
-    <mergeCell ref="N15:W15"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2633,7 +2634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA697C32-3881-B543-B376-9C8F58E5E06A}">
   <dimension ref="A1:BA13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
@@ -2694,7 +2695,7 @@
     </row>
     <row r="2" spans="1:53" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="129" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="129"/>
       <c r="C2" s="129"/>
@@ -2723,7 +2724,7 @@
     </row>
     <row r="3" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="129" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="129"/>
       <c r="C3" s="129"/>
@@ -2766,7 +2767,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="127" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" s="127"/>
       <c r="F5" s="127"/>
@@ -2791,7 +2792,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="127" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" s="127"/>
       <c r="F6" s="127"/>
@@ -2833,7 +2834,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="127" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E7" s="127"/>
       <c r="F7" s="127"/>
@@ -2955,7 +2956,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="127" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11" s="127"/>
       <c r="F11" s="127"/>
@@ -2987,7 +2988,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="127" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E13" s="127"/>
       <c r="F13" s="127"/>
@@ -3026,6 +3027,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B7BBE98651F7A43AC7BF2F06836443C" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b51c7281b06024c9ff887df9fe3bb465">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8103b6e4-b1cc-417b-af38-f980b3f4bdef" xmlns:ns3="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c056a6abdadb071051b2c083c327215c" ns2:_="" ns3:_="">
     <xsd:import namespace="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
@@ -3242,17 +3254,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
   <ds:schemaRefs>
@@ -3262,6 +3263,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
+    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E02BC65-B354-4988-8893-F98AC7F212AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3278,15 +3290,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
-    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: Pieds de page, dates CFVU/Conseil sur excels générés
</commit_message>
<xml_diff>
--- a/public/modeles/Annexe_MCCC.xlsx
+++ b/public/modeles/Annexe_MCCC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E69F1B-46EE-584B-BE7B-E3048AA0311E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E45BAA5-7BEC-5D4F-B76C-253DB01375D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modele" sheetId="9" r:id="rId1"/>
@@ -1260,98 +1260,47 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1359,42 +1308,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1406,6 +1319,93 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1886,7 +1886,7 @@
   </sheetPr>
   <dimension ref="A1:AJ27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -1916,38 +1916,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="115"/>
-      <c r="U1" s="115"/>
-      <c r="V1" s="115"/>
-      <c r="W1" s="115"/>
-      <c r="X1" s="115"/>
-      <c r="Y1" s="115"/>
-      <c r="Z1" s="115"/>
-      <c r="AA1" s="115"/>
-      <c r="AB1" s="115"/>
-      <c r="AC1" s="115"/>
-      <c r="AD1" s="115"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
+      <c r="V1" s="82"/>
+      <c r="W1" s="82"/>
+      <c r="X1" s="82"/>
+      <c r="Y1" s="82"/>
+      <c r="Z1" s="82"/>
+      <c r="AA1" s="82"/>
+      <c r="AB1" s="82"/>
+      <c r="AC1" s="82"/>
+      <c r="AD1" s="82"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
@@ -1956,87 +1956,87 @@
       <c r="AJ1" s="1"/>
     </row>
     <row r="2" spans="1:36" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="116"/>
-      <c r="N2" s="116"/>
-      <c r="O2" s="116"/>
-      <c r="P2" s="116"/>
-      <c r="Q2" s="116"/>
-      <c r="R2" s="116"/>
-      <c r="S2" s="116"/>
-      <c r="T2" s="116"/>
-      <c r="U2" s="116"/>
-      <c r="V2" s="116"/>
-      <c r="W2" s="116"/>
-      <c r="X2" s="116"/>
-      <c r="Y2" s="116"/>
-      <c r="Z2" s="116"/>
-      <c r="AA2" s="116"/>
-      <c r="AB2" s="116"/>
-      <c r="AC2" s="116"/>
-      <c r="AD2" s="116"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="83"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="83"/>
+      <c r="V2" s="83"/>
+      <c r="W2" s="83"/>
+      <c r="X2" s="83"/>
+      <c r="Y2" s="83"/>
+      <c r="Z2" s="83"/>
+      <c r="AA2" s="83"/>
+      <c r="AB2" s="83"/>
+      <c r="AC2" s="83"/>
+      <c r="AD2" s="83"/>
     </row>
     <row r="3" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="116" t="s">
+      <c r="A3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="116"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="116"/>
-      <c r="I3" s="116"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="116"/>
-      <c r="L3" s="116"/>
-      <c r="M3" s="116"/>
-      <c r="N3" s="116"/>
-      <c r="O3" s="116"/>
-      <c r="P3" s="116"/>
-      <c r="Q3" s="116"/>
-      <c r="R3" s="116"/>
-      <c r="S3" s="116"/>
-      <c r="T3" s="116"/>
-      <c r="U3" s="116"/>
-      <c r="V3" s="116"/>
-      <c r="W3" s="116"/>
-      <c r="X3" s="116"/>
-      <c r="Y3" s="116"/>
-      <c r="Z3" s="116"/>
-      <c r="AA3" s="116"/>
-      <c r="AB3" s="116"/>
-      <c r="AC3" s="116"/>
-      <c r="AD3" s="116"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="83"/>
+      <c r="Q3" s="83"/>
+      <c r="R3" s="83"/>
+      <c r="S3" s="83"/>
+      <c r="T3" s="83"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="83"/>
+      <c r="W3" s="83"/>
+      <c r="X3" s="83"/>
+      <c r="Y3" s="83"/>
+      <c r="Z3" s="83"/>
+      <c r="AA3" s="83"/>
+      <c r="AB3" s="83"/>
+      <c r="AC3" s="83"/>
+      <c r="AD3" s="83"/>
     </row>
     <row r="4" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="109" t="s">
+      <c r="G5" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="109"/>
-      <c r="I5" s="109"/>
-      <c r="J5" s="110" t="s">
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="110"/>
-      <c r="L5" s="110"/>
+      <c r="K5" s="93"/>
+      <c r="L5" s="93"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -2050,16 +2050,16 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="109" t="s">
+      <c r="G6" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="109"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="110" t="s">
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="110"/>
-      <c r="L6" s="110"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="93"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -2085,16 +2085,16 @@
         <v>8</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="109" t="s">
+      <c r="G7" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="109"/>
-      <c r="I7" s="109"/>
-      <c r="J7" s="110" t="s">
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="110"/>
-      <c r="L7" s="110"/>
+      <c r="K7" s="93"/>
+      <c r="L7" s="93"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -2136,16 +2136,16 @@
         <v>11</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="109" t="s">
+      <c r="G9" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="109"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="110" t="s">
+      <c r="H9" s="92"/>
+      <c r="I9" s="92"/>
+      <c r="J9" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="110"/>
-      <c r="L9" s="110"/>
+      <c r="K9" s="93"/>
+      <c r="L9" s="93"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -2179,16 +2179,16 @@
         <v>14</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="109" t="s">
+      <c r="G11" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="109"/>
-      <c r="I11" s="109"/>
-      <c r="J11" s="110" t="s">
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="110"/>
-      <c r="L11" s="110"/>
+      <c r="K11" s="93"/>
+      <c r="L11" s="93"/>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:36" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2209,16 +2209,16 @@
         <v>17</v>
       </c>
       <c r="F13" s="7"/>
-      <c r="G13" s="109" t="s">
+      <c r="G13" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="109"/>
-      <c r="I13" s="109"/>
-      <c r="J13" s="110" t="s">
+      <c r="H13" s="92"/>
+      <c r="I13" s="92"/>
+      <c r="J13" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="110"/>
-      <c r="L13" s="110"/>
+      <c r="K13" s="93"/>
+      <c r="L13" s="93"/>
       <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:36" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2229,103 +2229,103 @@
       <c r="M14"/>
     </row>
     <row r="15" spans="1:36" s="39" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="81" t="s">
+      <c r="A15" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="85"/>
-      <c r="D15" s="123" t="s">
+      <c r="C15" s="107"/>
+      <c r="D15" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="123"/>
-      <c r="F15" s="123"/>
-      <c r="G15" s="123"/>
-      <c r="H15" s="123"/>
-      <c r="I15" s="123"/>
-      <c r="J15" s="123"/>
-      <c r="K15" s="123"/>
-      <c r="L15" s="123"/>
-      <c r="M15" s="124"/>
-      <c r="N15" s="106" t="s">
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="94"/>
+      <c r="H15" s="94"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="94"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="95"/>
+      <c r="N15" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="107"/>
-      <c r="P15" s="107"/>
-      <c r="Q15" s="107"/>
-      <c r="R15" s="107"/>
-      <c r="S15" s="107"/>
-      <c r="T15" s="107"/>
-      <c r="U15" s="107"/>
-      <c r="V15" s="107"/>
-      <c r="W15" s="121"/>
-      <c r="X15" s="107" t="s">
+      <c r="O15" s="89"/>
+      <c r="P15" s="89"/>
+      <c r="Q15" s="89"/>
+      <c r="R15" s="89"/>
+      <c r="S15" s="89"/>
+      <c r="T15" s="89"/>
+      <c r="U15" s="89"/>
+      <c r="V15" s="89"/>
+      <c r="W15" s="90"/>
+      <c r="X15" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="Y15" s="107"/>
-      <c r="Z15" s="121"/>
-      <c r="AA15" s="90" t="s">
+      <c r="Y15" s="89"/>
+      <c r="Z15" s="90"/>
+      <c r="AA15" s="112" t="s">
         <v>55</v>
       </c>
-      <c r="AB15" s="90"/>
-      <c r="AC15" s="90"/>
-      <c r="AD15" s="91"/>
+      <c r="AB15" s="112"/>
+      <c r="AC15" s="112"/>
+      <c r="AD15" s="113"/>
     </row>
     <row r="16" spans="1:36" s="39" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="82"/>
-      <c r="B16" s="86"/>
-      <c r="C16" s="87"/>
-      <c r="D16" s="125"/>
-      <c r="E16" s="125"/>
-      <c r="F16" s="125"/>
-      <c r="G16" s="125"/>
-      <c r="H16" s="125"/>
-      <c r="I16" s="125"/>
-      <c r="J16" s="125"/>
-      <c r="K16" s="125"/>
-      <c r="L16" s="125"/>
-      <c r="M16" s="126"/>
-      <c r="N16" s="106" t="s">
+      <c r="A16" s="104"/>
+      <c r="B16" s="108"/>
+      <c r="C16" s="109"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="96"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="96"/>
+      <c r="J16" s="96"/>
+      <c r="K16" s="96"/>
+      <c r="L16" s="96"/>
+      <c r="M16" s="97"/>
+      <c r="N16" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="O16" s="107"/>
-      <c r="P16" s="107"/>
-      <c r="Q16" s="108"/>
-      <c r="R16" s="106" t="s">
+      <c r="O16" s="89"/>
+      <c r="P16" s="89"/>
+      <c r="Q16" s="99"/>
+      <c r="R16" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="S16" s="107"/>
-      <c r="T16" s="107"/>
-      <c r="U16" s="108"/>
-      <c r="V16" s="104" t="s">
+      <c r="S16" s="89"/>
+      <c r="T16" s="89"/>
+      <c r="U16" s="99"/>
+      <c r="V16" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="W16" s="88" t="s">
+      <c r="W16" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="X16" s="117" t="s">
+      <c r="X16" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="Y16" s="119" t="s">
+      <c r="Y16" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="Z16" s="96" t="s">
+      <c r="Z16" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="AA16" s="92" t="s">
+      <c r="AA16" s="114" t="s">
         <v>62</v>
       </c>
-      <c r="AB16" s="93"/>
-      <c r="AC16" s="94" t="s">
+      <c r="AB16" s="115"/>
+      <c r="AC16" s="116" t="s">
         <v>58</v>
       </c>
-      <c r="AD16" s="94" t="s">
+      <c r="AD16" s="116" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:30" s="44" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="83"/>
+      <c r="A17" s="105"/>
       <c r="B17" s="41" t="s">
         <v>28</v>
       </c>
@@ -2386,19 +2386,19 @@
       <c r="U17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V17" s="105"/>
-      <c r="W17" s="89"/>
-      <c r="X17" s="118"/>
-      <c r="Y17" s="120"/>
-      <c r="Z17" s="97"/>
+      <c r="V17" s="126"/>
+      <c r="W17" s="111"/>
+      <c r="X17" s="86"/>
+      <c r="Y17" s="88"/>
+      <c r="Z17" s="119"/>
       <c r="AA17" s="49" t="s">
         <v>60</v>
       </c>
       <c r="AB17" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="AC17" s="95"/>
-      <c r="AD17" s="95"/>
+      <c r="AC17" s="117"/>
+      <c r="AD17" s="117"/>
     </row>
     <row r="18" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -2439,19 +2439,19 @@
       <c r="AD18" s="47"/>
     </row>
     <row r="19" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="122" t="s">
+      <c r="A19" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="122"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="122"/>
-      <c r="E19" s="122"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="91"/>
+      <c r="E19" s="91"/>
       <c r="F19" s="36"/>
       <c r="H19" s="11"/>
-      <c r="L19" s="102" t="s">
+      <c r="L19" s="124" t="s">
         <v>49</v>
       </c>
-      <c r="M19" s="102"/>
+      <c r="M19" s="124"/>
       <c r="N19" s="64"/>
       <c r="O19" s="65"/>
       <c r="P19" s="66"/>
@@ -2471,63 +2471,63 @@
       <c r="AD19" s="47"/>
     </row>
     <row r="20" spans="1:30" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="98" t="s">
+      <c r="A20" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="98"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="98"/>
+      <c r="B20" s="120"/>
+      <c r="C20" s="120"/>
+      <c r="D20" s="120"/>
+      <c r="E20" s="120"/>
       <c r="H20" s="11"/>
-      <c r="L20" s="103" t="s">
+      <c r="L20" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="M20" s="103"/>
-      <c r="N20" s="99"/>
-      <c r="O20" s="100"/>
-      <c r="P20" s="100"/>
-      <c r="Q20" s="100"/>
-      <c r="R20" s="100"/>
-      <c r="S20" s="100"/>
-      <c r="T20" s="100"/>
-      <c r="U20" s="100"/>
-      <c r="V20" s="101"/>
+      <c r="M20" s="84"/>
+      <c r="N20" s="121"/>
+      <c r="O20" s="122"/>
+      <c r="P20" s="122"/>
+      <c r="Q20" s="122"/>
+      <c r="R20" s="122"/>
+      <c r="S20" s="122"/>
+      <c r="T20" s="122"/>
+      <c r="U20" s="122"/>
+      <c r="V20" s="123"/>
       <c r="W20" s="67"/>
     </row>
     <row r="21" spans="1:30" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="H21" s="11"/>
-      <c r="L21" s="103" t="s">
+      <c r="L21" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="M21" s="103"/>
-      <c r="N21" s="78"/>
-      <c r="O21" s="79"/>
-      <c r="P21" s="79"/>
-      <c r="Q21" s="79"/>
-      <c r="R21" s="79"/>
-      <c r="S21" s="79"/>
-      <c r="T21" s="79"/>
-      <c r="U21" s="79"/>
-      <c r="V21" s="79"/>
-      <c r="W21" s="80"/>
+      <c r="M21" s="84"/>
+      <c r="N21" s="100"/>
+      <c r="O21" s="101"/>
+      <c r="P21" s="101"/>
+      <c r="Q21" s="101"/>
+      <c r="R21" s="101"/>
+      <c r="S21" s="101"/>
+      <c r="T21" s="101"/>
+      <c r="U21" s="101"/>
+      <c r="V21" s="101"/>
+      <c r="W21" s="102"/>
     </row>
     <row r="22" spans="1:30" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="H22" s="11"/>
-      <c r="L22" s="103" t="s">
+      <c r="L22" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="M22" s="103"/>
-      <c r="N22" s="78"/>
-      <c r="O22" s="79"/>
-      <c r="P22" s="79"/>
-      <c r="Q22" s="79"/>
-      <c r="R22" s="79"/>
-      <c r="S22" s="79"/>
-      <c r="T22" s="79"/>
-      <c r="U22" s="79"/>
-      <c r="V22" s="80"/>
+      <c r="M22" s="84"/>
+      <c r="N22" s="100"/>
+      <c r="O22" s="101"/>
+      <c r="P22" s="101"/>
+      <c r="Q22" s="101"/>
+      <c r="R22" s="101"/>
+      <c r="S22" s="101"/>
+      <c r="T22" s="101"/>
+      <c r="U22" s="101"/>
+      <c r="V22" s="102"/>
       <c r="W22" s="67"/>
     </row>
     <row r="23" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2544,9 +2544,9 @@
       <c r="AA24" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="AB24" s="112"/>
-      <c r="AC24" s="113"/>
-      <c r="AD24" s="114"/>
+      <c r="AB24" s="79"/>
+      <c r="AC24" s="80"/>
+      <c r="AD24" s="81"/>
     </row>
     <row r="25" spans="1:30" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
@@ -2560,21 +2560,48 @@
       <c r="AA25" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="AB25" s="112"/>
-      <c r="AC25" s="113"/>
-      <c r="AD25" s="114"/>
+      <c r="AB25" s="79"/>
+      <c r="AC25" s="80"/>
+      <c r="AD25" s="81"/>
     </row>
     <row r="27" spans="1:30" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="111" t="s">
+      <c r="A27" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="111"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="111"/>
-      <c r="E27" s="111"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="N22:V22"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="AA15:AD15"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="AC16:AC17"/>
+    <mergeCell ref="AD16:AD17"/>
+    <mergeCell ref="Z16:Z17"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="N20:V20"/>
+    <mergeCell ref="N21:W21"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="R16:U16"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J13:L13"/>
     <mergeCell ref="A27:E27"/>
     <mergeCell ref="AB25:AD25"/>
     <mergeCell ref="A1:AD1"/>
@@ -2591,39 +2618,12 @@
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="D15:M16"/>
     <mergeCell ref="N15:W15"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="N22:V22"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="W16:W17"/>
-    <mergeCell ref="AA15:AD15"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="AC16:AC17"/>
-    <mergeCell ref="AD16:AD17"/>
-    <mergeCell ref="Z16:Z17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="N20:V20"/>
-    <mergeCell ref="N21:W21"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="V16:V17"/>
-    <mergeCell ref="R16:U16"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="8" scale="41" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="40" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Calibri,Normal"&amp;K000000MCCC &amp;F&amp;R&amp;"Calibri,Normal"&amp;K000000Version du &amp;D &amp;T</oddHeader>
+    <oddHeader>&amp;C&amp;"Calibri,Normal"&amp;K000000&amp;F&amp;R&amp;"Calibri,Normal"&amp;K000000Version du &amp;D &amp;T</oddHeader>
     <oddFooter>&amp;L&amp;"Calibri,Normal"&amp;K000000Document généré depuis ORéOF&amp;C&amp;"Calibri,Normal"&amp;K000000Document non validé en CFVU&amp;R&amp;"Calibri,Normal"&amp;K000000Université de Reims Champagne-Ardenne</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
@@ -2634,8 +2634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA697C32-3881-B543-B376-9C8F58E5E06A}">
   <dimension ref="A1:BA13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3027,17 +3027,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B7BBE98651F7A43AC7BF2F06836443C" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b51c7281b06024c9ff887df9fe3bb465">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8103b6e4-b1cc-417b-af38-f980b3f4bdef" xmlns:ns3="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c056a6abdadb071051b2c083c327215c" ns2:_="" ns3:_="">
     <xsd:import namespace="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
@@ -3254,6 +3243,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
   <ds:schemaRefs>
@@ -3263,17 +3263,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
-    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E02BC65-B354-4988-8893-F98AC7F212AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3290,4 +3279,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
+    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: Affichage référentiel de compétences
</commit_message>
<xml_diff>
--- a/public/modeles/Annexe_MCCC.xlsx
+++ b/public/modeles/Annexe_MCCC.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E45BAA5-7BEC-5D4F-B76C-253DB01375D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07182ADD-C7CB-2F47-8E8D-EA1F7FEB1B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-1460" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modele" sheetId="9" r:id="rId1"/>
     <sheet name="ref. compétences" sheetId="10" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">modele!$1:$17</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'ref. compétences'!$1:$13</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1260,6 +1264,108 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1278,9 +1384,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1291,9 +1394,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1302,12 +1402,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1319,96 +1413,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1886,7 +1890,7 @@
   </sheetPr>
   <dimension ref="A1:AJ27"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -1916,38 +1920,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="82"/>
-      <c r="AA1" s="82"/>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="82"/>
-      <c r="AD1" s="82"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="116"/>
+      <c r="L1" s="116"/>
+      <c r="M1" s="116"/>
+      <c r="N1" s="116"/>
+      <c r="O1" s="116"/>
+      <c r="P1" s="116"/>
+      <c r="Q1" s="116"/>
+      <c r="R1" s="116"/>
+      <c r="S1" s="116"/>
+      <c r="T1" s="116"/>
+      <c r="U1" s="116"/>
+      <c r="V1" s="116"/>
+      <c r="W1" s="116"/>
+      <c r="X1" s="116"/>
+      <c r="Y1" s="116"/>
+      <c r="Z1" s="116"/>
+      <c r="AA1" s="116"/>
+      <c r="AB1" s="116"/>
+      <c r="AC1" s="116"/>
+      <c r="AD1" s="116"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
@@ -1956,87 +1960,87 @@
       <c r="AJ1" s="1"/>
     </row>
     <row r="2" spans="1:36" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="83"/>
-      <c r="S2" s="83"/>
-      <c r="T2" s="83"/>
-      <c r="U2" s="83"/>
-      <c r="V2" s="83"/>
-      <c r="W2" s="83"/>
-      <c r="X2" s="83"/>
-      <c r="Y2" s="83"/>
-      <c r="Z2" s="83"/>
-      <c r="AA2" s="83"/>
-      <c r="AB2" s="83"/>
-      <c r="AC2" s="83"/>
-      <c r="AD2" s="83"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="117"/>
+      <c r="O2" s="117"/>
+      <c r="P2" s="117"/>
+      <c r="Q2" s="117"/>
+      <c r="R2" s="117"/>
+      <c r="S2" s="117"/>
+      <c r="T2" s="117"/>
+      <c r="U2" s="117"/>
+      <c r="V2" s="117"/>
+      <c r="W2" s="117"/>
+      <c r="X2" s="117"/>
+      <c r="Y2" s="117"/>
+      <c r="Z2" s="117"/>
+      <c r="AA2" s="117"/>
+      <c r="AB2" s="117"/>
+      <c r="AC2" s="117"/>
+      <c r="AD2" s="117"/>
     </row>
     <row r="3" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
-      <c r="Q3" s="83"/>
-      <c r="R3" s="83"/>
-      <c r="S3" s="83"/>
-      <c r="T3" s="83"/>
-      <c r="U3" s="83"/>
-      <c r="V3" s="83"/>
-      <c r="W3" s="83"/>
-      <c r="X3" s="83"/>
-      <c r="Y3" s="83"/>
-      <c r="Z3" s="83"/>
-      <c r="AA3" s="83"/>
-      <c r="AB3" s="83"/>
-      <c r="AC3" s="83"/>
-      <c r="AD3" s="83"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="117"/>
+      <c r="I3" s="117"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="117"/>
+      <c r="L3" s="117"/>
+      <c r="M3" s="117"/>
+      <c r="N3" s="117"/>
+      <c r="O3" s="117"/>
+      <c r="P3" s="117"/>
+      <c r="Q3" s="117"/>
+      <c r="R3" s="117"/>
+      <c r="S3" s="117"/>
+      <c r="T3" s="117"/>
+      <c r="U3" s="117"/>
+      <c r="V3" s="117"/>
+      <c r="W3" s="117"/>
+      <c r="X3" s="117"/>
+      <c r="Y3" s="117"/>
+      <c r="Z3" s="117"/>
+      <c r="AA3" s="117"/>
+      <c r="AB3" s="117"/>
+      <c r="AC3" s="117"/>
+      <c r="AD3" s="117"/>
     </row>
     <row r="4" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="92" t="s">
+      <c r="G5" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="93" t="s">
+      <c r="H5" s="110"/>
+      <c r="I5" s="110"/>
+      <c r="J5" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
+      <c r="K5" s="111"/>
+      <c r="L5" s="111"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -2050,16 +2054,16 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="92" t="s">
+      <c r="G6" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="93" t="s">
+      <c r="H6" s="110"/>
+      <c r="I6" s="110"/>
+      <c r="J6" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
+      <c r="K6" s="111"/>
+      <c r="L6" s="111"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -2085,16 +2089,16 @@
         <v>8</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="92" t="s">
+      <c r="G7" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="93" t="s">
+      <c r="H7" s="110"/>
+      <c r="I7" s="110"/>
+      <c r="J7" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="93"/>
-      <c r="L7" s="93"/>
+      <c r="K7" s="111"/>
+      <c r="L7" s="111"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -2136,16 +2140,16 @@
         <v>11</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="92" t="s">
+      <c r="G9" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="92"/>
-      <c r="I9" s="92"/>
-      <c r="J9" s="93" t="s">
+      <c r="H9" s="110"/>
+      <c r="I9" s="110"/>
+      <c r="J9" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="93"/>
-      <c r="L9" s="93"/>
+      <c r="K9" s="111"/>
+      <c r="L9" s="111"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -2179,16 +2183,16 @@
         <v>14</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="92" t="s">
+      <c r="G11" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
-      <c r="J11" s="93" t="s">
+      <c r="H11" s="110"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="111" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="93"/>
-      <c r="L11" s="93"/>
+      <c r="K11" s="111"/>
+      <c r="L11" s="111"/>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:36" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2209,16 +2213,16 @@
         <v>17</v>
       </c>
       <c r="F13" s="7"/>
-      <c r="G13" s="92" t="s">
+      <c r="G13" s="110" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="92"/>
-      <c r="I13" s="92"/>
-      <c r="J13" s="93" t="s">
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
+      <c r="J13" s="111" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="93"/>
-      <c r="L13" s="93"/>
+      <c r="K13" s="111"/>
+      <c r="L13" s="111"/>
       <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:36" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2229,103 +2233,103 @@
       <c r="M14"/>
     </row>
     <row r="15" spans="1:36" s="39" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="103" t="s">
+      <c r="A15" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="106" t="s">
+      <c r="B15" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="107"/>
-      <c r="D15" s="94" t="s">
+      <c r="C15" s="86"/>
+      <c r="D15" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="94"/>
-      <c r="F15" s="94"/>
-      <c r="G15" s="94"/>
-      <c r="H15" s="94"/>
-      <c r="I15" s="94"/>
-      <c r="J15" s="94"/>
-      <c r="K15" s="94"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="95"/>
-      <c r="N15" s="98" t="s">
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="124"/>
+      <c r="I15" s="124"/>
+      <c r="J15" s="124"/>
+      <c r="K15" s="124"/>
+      <c r="L15" s="124"/>
+      <c r="M15" s="125"/>
+      <c r="N15" s="107" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="89"/>
-      <c r="P15" s="89"/>
-      <c r="Q15" s="89"/>
-      <c r="R15" s="89"/>
-      <c r="S15" s="89"/>
-      <c r="T15" s="89"/>
-      <c r="U15" s="89"/>
-      <c r="V15" s="89"/>
-      <c r="W15" s="90"/>
-      <c r="X15" s="89" t="s">
+      <c r="O15" s="108"/>
+      <c r="P15" s="108"/>
+      <c r="Q15" s="108"/>
+      <c r="R15" s="108"/>
+      <c r="S15" s="108"/>
+      <c r="T15" s="108"/>
+      <c r="U15" s="108"/>
+      <c r="V15" s="108"/>
+      <c r="W15" s="122"/>
+      <c r="X15" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="Y15" s="89"/>
-      <c r="Z15" s="90"/>
-      <c r="AA15" s="112" t="s">
+      <c r="Y15" s="108"/>
+      <c r="Z15" s="122"/>
+      <c r="AA15" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="AB15" s="112"/>
-      <c r="AC15" s="112"/>
-      <c r="AD15" s="113"/>
+      <c r="AB15" s="91"/>
+      <c r="AC15" s="91"/>
+      <c r="AD15" s="92"/>
     </row>
     <row r="16" spans="1:36" s="39" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="104"/>
-      <c r="B16" s="108"/>
-      <c r="C16" s="109"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="96"/>
-      <c r="I16" s="96"/>
-      <c r="J16" s="96"/>
-      <c r="K16" s="96"/>
-      <c r="L16" s="96"/>
-      <c r="M16" s="97"/>
-      <c r="N16" s="98" t="s">
+      <c r="A16" s="83"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="88"/>
+      <c r="D16" s="126"/>
+      <c r="E16" s="126"/>
+      <c r="F16" s="126"/>
+      <c r="G16" s="126"/>
+      <c r="H16" s="126"/>
+      <c r="I16" s="126"/>
+      <c r="J16" s="126"/>
+      <c r="K16" s="126"/>
+      <c r="L16" s="126"/>
+      <c r="M16" s="127"/>
+      <c r="N16" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="O16" s="89"/>
-      <c r="P16" s="89"/>
-      <c r="Q16" s="99"/>
-      <c r="R16" s="98" t="s">
+      <c r="O16" s="108"/>
+      <c r="P16" s="108"/>
+      <c r="Q16" s="109"/>
+      <c r="R16" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="S16" s="89"/>
-      <c r="T16" s="89"/>
-      <c r="U16" s="99"/>
-      <c r="V16" s="125" t="s">
+      <c r="S16" s="108"/>
+      <c r="T16" s="108"/>
+      <c r="U16" s="109"/>
+      <c r="V16" s="105" t="s">
         <v>27</v>
       </c>
-      <c r="W16" s="110" t="s">
+      <c r="W16" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="X16" s="85" t="s">
+      <c r="X16" s="118" t="s">
         <v>57</v>
       </c>
-      <c r="Y16" s="87" t="s">
+      <c r="Y16" s="120" t="s">
         <v>53</v>
       </c>
-      <c r="Z16" s="118" t="s">
+      <c r="Z16" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="AA16" s="114" t="s">
+      <c r="AA16" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="AB16" s="115"/>
-      <c r="AC16" s="116" t="s">
+      <c r="AB16" s="94"/>
+      <c r="AC16" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="AD16" s="116" t="s">
+      <c r="AD16" s="95" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:30" s="44" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="105"/>
+      <c r="A17" s="84"/>
       <c r="B17" s="41" t="s">
         <v>28</v>
       </c>
@@ -2386,19 +2390,19 @@
       <c r="U17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V17" s="126"/>
-      <c r="W17" s="111"/>
-      <c r="X17" s="86"/>
-      <c r="Y17" s="88"/>
-      <c r="Z17" s="119"/>
+      <c r="V17" s="106"/>
+      <c r="W17" s="90"/>
+      <c r="X17" s="119"/>
+      <c r="Y17" s="121"/>
+      <c r="Z17" s="98"/>
       <c r="AA17" s="49" t="s">
         <v>60</v>
       </c>
       <c r="AB17" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="AC17" s="117"/>
-      <c r="AD17" s="117"/>
+      <c r="AC17" s="96"/>
+      <c r="AD17" s="96"/>
     </row>
     <row r="18" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -2439,19 +2443,19 @@
       <c r="AD18" s="47"/>
     </row>
     <row r="19" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="91" t="s">
+      <c r="A19" s="123" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="91"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="91"/>
-      <c r="E19" s="91"/>
+      <c r="B19" s="123"/>
+      <c r="C19" s="123"/>
+      <c r="D19" s="123"/>
+      <c r="E19" s="123"/>
       <c r="F19" s="36"/>
       <c r="H19" s="11"/>
-      <c r="L19" s="124" t="s">
+      <c r="L19" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="M19" s="124"/>
+      <c r="M19" s="103"/>
       <c r="N19" s="64"/>
       <c r="O19" s="65"/>
       <c r="P19" s="66"/>
@@ -2471,63 +2475,63 @@
       <c r="AD19" s="47"/>
     </row>
     <row r="20" spans="1:30" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="120" t="s">
+      <c r="A20" s="99" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="120"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="120"/>
-      <c r="E20" s="120"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="99"/>
+      <c r="D20" s="99"/>
+      <c r="E20" s="99"/>
       <c r="H20" s="11"/>
-      <c r="L20" s="84" t="s">
+      <c r="L20" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="M20" s="84"/>
-      <c r="N20" s="121"/>
-      <c r="O20" s="122"/>
-      <c r="P20" s="122"/>
-      <c r="Q20" s="122"/>
-      <c r="R20" s="122"/>
-      <c r="S20" s="122"/>
-      <c r="T20" s="122"/>
-      <c r="U20" s="122"/>
-      <c r="V20" s="123"/>
+      <c r="M20" s="104"/>
+      <c r="N20" s="100"/>
+      <c r="O20" s="101"/>
+      <c r="P20" s="101"/>
+      <c r="Q20" s="101"/>
+      <c r="R20" s="101"/>
+      <c r="S20" s="101"/>
+      <c r="T20" s="101"/>
+      <c r="U20" s="101"/>
+      <c r="V20" s="102"/>
       <c r="W20" s="67"/>
     </row>
     <row r="21" spans="1:30" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="H21" s="11"/>
-      <c r="L21" s="84" t="s">
+      <c r="L21" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="M21" s="84"/>
-      <c r="N21" s="100"/>
-      <c r="O21" s="101"/>
-      <c r="P21" s="101"/>
-      <c r="Q21" s="101"/>
-      <c r="R21" s="101"/>
-      <c r="S21" s="101"/>
-      <c r="T21" s="101"/>
-      <c r="U21" s="101"/>
-      <c r="V21" s="101"/>
-      <c r="W21" s="102"/>
+      <c r="M21" s="104"/>
+      <c r="N21" s="79"/>
+      <c r="O21" s="80"/>
+      <c r="P21" s="80"/>
+      <c r="Q21" s="80"/>
+      <c r="R21" s="80"/>
+      <c r="S21" s="80"/>
+      <c r="T21" s="80"/>
+      <c r="U21" s="80"/>
+      <c r="V21" s="80"/>
+      <c r="W21" s="81"/>
     </row>
     <row r="22" spans="1:30" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="H22" s="11"/>
-      <c r="L22" s="84" t="s">
+      <c r="L22" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="M22" s="84"/>
-      <c r="N22" s="100"/>
-      <c r="O22" s="101"/>
-      <c r="P22" s="101"/>
-      <c r="Q22" s="101"/>
-      <c r="R22" s="101"/>
-      <c r="S22" s="101"/>
-      <c r="T22" s="101"/>
-      <c r="U22" s="101"/>
-      <c r="V22" s="102"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="79"/>
+      <c r="O22" s="80"/>
+      <c r="P22" s="80"/>
+      <c r="Q22" s="80"/>
+      <c r="R22" s="80"/>
+      <c r="S22" s="80"/>
+      <c r="T22" s="80"/>
+      <c r="U22" s="80"/>
+      <c r="V22" s="81"/>
       <c r="W22" s="67"/>
     </row>
     <row r="23" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2544,9 +2548,9 @@
       <c r="AA24" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="AB24" s="79"/>
-      <c r="AC24" s="80"/>
-      <c r="AD24" s="81"/>
+      <c r="AB24" s="113"/>
+      <c r="AC24" s="114"/>
+      <c r="AD24" s="115"/>
     </row>
     <row r="25" spans="1:30" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
@@ -2560,21 +2564,48 @@
       <c r="AA25" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="AB25" s="79"/>
-      <c r="AC25" s="80"/>
-      <c r="AD25" s="81"/>
+      <c r="AB25" s="113"/>
+      <c r="AC25" s="114"/>
+      <c r="AD25" s="115"/>
     </row>
     <row r="27" spans="1:30" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="78"/>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="78"/>
+      <c r="B27" s="112"/>
+      <c r="C27" s="112"/>
+      <c r="D27" s="112"/>
+      <c r="E27" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="AB25:AD25"/>
+    <mergeCell ref="A1:AD1"/>
+    <mergeCell ref="A2:AD2"/>
+    <mergeCell ref="A3:AD3"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="AB24:AD24"/>
+    <mergeCell ref="X16:X17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="X15:Z15"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="D15:M16"/>
+    <mergeCell ref="N15:W15"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G13:I13"/>
     <mergeCell ref="N22:V22"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:C16"/>
@@ -2591,37 +2622,10 @@
     <mergeCell ref="L20:M20"/>
     <mergeCell ref="V16:V17"/>
     <mergeCell ref="R16:U16"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="AB25:AD25"/>
-    <mergeCell ref="A1:AD1"/>
-    <mergeCell ref="A2:AD2"/>
-    <mergeCell ref="A3:AD3"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="AB24:AD24"/>
-    <mergeCell ref="X16:X17"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="X15:Z15"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="D15:M16"/>
-    <mergeCell ref="N15:W15"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="8" scale="40" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="40" fitToHeight="3" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri,Normal"&amp;K000000&amp;F&amp;R&amp;"Calibri,Normal"&amp;K000000Version du &amp;D &amp;T</oddHeader>
     <oddFooter>&amp;L&amp;"Calibri,Normal"&amp;K000000Document généré depuis ORéOF&amp;C&amp;"Calibri,Normal"&amp;K000000Document non validé en CFVU&amp;R&amp;"Calibri,Normal"&amp;K000000Université de Reims Champagne-Ardenne</oddFooter>
@@ -2632,10 +2636,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA697C32-3881-B543-B376-9C8F58E5E06A}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:BA13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2643,7 +2650,7 @@
     <col min="1" max="1" width="7.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" customWidth="1"/>
     <col min="3" max="3" width="108.6640625" customWidth="1"/>
-    <col min="4" max="4" width="43.33203125" customWidth="1"/>
+    <col min="4" max="4" width="64.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="20" x14ac:dyDescent="0.2">
@@ -2766,11 +2773,11 @@
       <c r="C5" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="127" t="s">
+      <c r="D5" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="127"/>
-      <c r="F5" s="127"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
       <c r="G5" s="70"/>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
@@ -2791,11 +2798,11 @@
       <c r="C6" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="127" t="s">
+      <c r="D6" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
       <c r="G6" s="70"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
@@ -2833,11 +2840,11 @@
       <c r="C7" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="127" t="s">
+      <c r="D7" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="127"/>
-      <c r="F7" s="127"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
       <c r="G7" s="70"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
@@ -2955,11 +2962,11 @@
       <c r="C11" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="127" t="s">
+      <c r="D11" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="127"/>
-      <c r="F11" s="127"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
       <c r="G11" s="70"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
@@ -2987,11 +2994,11 @@
       <c r="C13" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="127" t="s">
+      <c r="D13" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="127"/>
-      <c r="F13" s="127"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
       <c r="G13" s="70"/>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
@@ -3001,29 +3008,26 @@
       <c r="N13" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D13:F13"/>
+  <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" scale="80" fitToHeight="2" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3244,20 +3248,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
+    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3282,12 +3287,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
-    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: correctif textes modèle MCCC
</commit_message>
<xml_diff>
--- a/public/modeles/Annexe_MCCC.xlsx
+++ b/public/modeles/Annexe_MCCC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07182ADD-C7CB-2F47-8E8D-EA1F7FEB1B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E36C3D-AE88-F14D-B26C-D3678B703650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1460" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modele" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
   <si>
     <t>ACCREDITATION 2024-2028</t>
   </si>
@@ -196,9 +196,6 @@
   </si>
   <si>
     <t>RÉFÉRENTIEL DE COMPÉTENCES</t>
-  </si>
-  <si>
-    <t>* dans le cas du Cci, la seconde chance se traduit par la non prise en compte dans le calcul de la note finale de la moins bonne des notes de Cci obtenues dans l'enseignement concerné.</t>
   </si>
   <si>
     <t>Contrôle continu (CC)</t>
@@ -1267,98 +1264,47 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1366,42 +1312,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1413,6 +1323,93 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1890,8 +1887,8 @@
   </sheetPr>
   <dimension ref="A1:AJ27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="116" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16:X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1920,38 +1917,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="116"/>
-      <c r="M1" s="116"/>
-      <c r="N1" s="116"/>
-      <c r="O1" s="116"/>
-      <c r="P1" s="116"/>
-      <c r="Q1" s="116"/>
-      <c r="R1" s="116"/>
-      <c r="S1" s="116"/>
-      <c r="T1" s="116"/>
-      <c r="U1" s="116"/>
-      <c r="V1" s="116"/>
-      <c r="W1" s="116"/>
-      <c r="X1" s="116"/>
-      <c r="Y1" s="116"/>
-      <c r="Z1" s="116"/>
-      <c r="AA1" s="116"/>
-      <c r="AB1" s="116"/>
-      <c r="AC1" s="116"/>
-      <c r="AD1" s="116"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="83"/>
+      <c r="AA1" s="83"/>
+      <c r="AB1" s="83"/>
+      <c r="AC1" s="83"/>
+      <c r="AD1" s="83"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
@@ -1960,87 +1957,87 @@
       <c r="AJ1" s="1"/>
     </row>
     <row r="2" spans="1:36" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="117" t="s">
+      <c r="A2" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="117"/>
-      <c r="M2" s="117"/>
-      <c r="N2" s="117"/>
-      <c r="O2" s="117"/>
-      <c r="P2" s="117"/>
-      <c r="Q2" s="117"/>
-      <c r="R2" s="117"/>
-      <c r="S2" s="117"/>
-      <c r="T2" s="117"/>
-      <c r="U2" s="117"/>
-      <c r="V2" s="117"/>
-      <c r="W2" s="117"/>
-      <c r="X2" s="117"/>
-      <c r="Y2" s="117"/>
-      <c r="Z2" s="117"/>
-      <c r="AA2" s="117"/>
-      <c r="AB2" s="117"/>
-      <c r="AC2" s="117"/>
-      <c r="AD2" s="117"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="84"/>
+      <c r="T2" s="84"/>
+      <c r="U2" s="84"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="84"/>
+      <c r="X2" s="84"/>
+      <c r="Y2" s="84"/>
+      <c r="Z2" s="84"/>
+      <c r="AA2" s="84"/>
+      <c r="AB2" s="84"/>
+      <c r="AC2" s="84"/>
+      <c r="AD2" s="84"/>
     </row>
     <row r="3" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="117"/>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117"/>
-      <c r="H3" s="117"/>
-      <c r="I3" s="117"/>
-      <c r="J3" s="117"/>
-      <c r="K3" s="117"/>
-      <c r="L3" s="117"/>
-      <c r="M3" s="117"/>
-      <c r="N3" s="117"/>
-      <c r="O3" s="117"/>
-      <c r="P3" s="117"/>
-      <c r="Q3" s="117"/>
-      <c r="R3" s="117"/>
-      <c r="S3" s="117"/>
-      <c r="T3" s="117"/>
-      <c r="U3" s="117"/>
-      <c r="V3" s="117"/>
-      <c r="W3" s="117"/>
-      <c r="X3" s="117"/>
-      <c r="Y3" s="117"/>
-      <c r="Z3" s="117"/>
-      <c r="AA3" s="117"/>
-      <c r="AB3" s="117"/>
-      <c r="AC3" s="117"/>
-      <c r="AD3" s="117"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="84"/>
+      <c r="T3" s="84"/>
+      <c r="U3" s="84"/>
+      <c r="V3" s="84"/>
+      <c r="W3" s="84"/>
+      <c r="X3" s="84"/>
+      <c r="Y3" s="84"/>
+      <c r="Z3" s="84"/>
+      <c r="AA3" s="84"/>
+      <c r="AB3" s="84"/>
+      <c r="AC3" s="84"/>
+      <c r="AD3" s="84"/>
     </row>
     <row r="4" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="110" t="s">
+      <c r="G5" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="110"/>
-      <c r="I5" s="110"/>
-      <c r="J5" s="111" t="s">
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="111"/>
-      <c r="L5" s="111"/>
+      <c r="K5" s="94"/>
+      <c r="L5" s="94"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -2054,16 +2051,16 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="110" t="s">
+      <c r="G6" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="111" t="s">
+      <c r="H6" s="93"/>
+      <c r="I6" s="93"/>
+      <c r="J6" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="111"/>
-      <c r="L6" s="111"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="94"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -2089,16 +2086,16 @@
         <v>8</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="110" t="s">
+      <c r="G7" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="110"/>
-      <c r="I7" s="110"/>
-      <c r="J7" s="111" t="s">
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="111"/>
-      <c r="L7" s="111"/>
+      <c r="K7" s="94"/>
+      <c r="L7" s="94"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -2140,16 +2137,16 @@
         <v>11</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="110" t="s">
+      <c r="G9" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="110"/>
-      <c r="I9" s="110"/>
-      <c r="J9" s="111" t="s">
+      <c r="H9" s="93"/>
+      <c r="I9" s="93"/>
+      <c r="J9" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="111"/>
-      <c r="L9" s="111"/>
+      <c r="K9" s="94"/>
+      <c r="L9" s="94"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -2183,16 +2180,16 @@
         <v>14</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="110" t="s">
+      <c r="G11" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="110"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="111" t="s">
+      <c r="H11" s="93"/>
+      <c r="I11" s="93"/>
+      <c r="J11" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="111"/>
-      <c r="L11" s="111"/>
+      <c r="K11" s="94"/>
+      <c r="L11" s="94"/>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:36" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2213,16 +2210,16 @@
         <v>17</v>
       </c>
       <c r="F13" s="7"/>
-      <c r="G13" s="110" t="s">
+      <c r="G13" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="110"/>
-      <c r="I13" s="110"/>
-      <c r="J13" s="111" t="s">
+      <c r="H13" s="93"/>
+      <c r="I13" s="93"/>
+      <c r="J13" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="111"/>
-      <c r="L13" s="111"/>
+      <c r="K13" s="94"/>
+      <c r="L13" s="94"/>
       <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:36" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2233,108 +2230,108 @@
       <c r="M14"/>
     </row>
     <row r="15" spans="1:36" s="39" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="82" t="s">
+      <c r="A15" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="85" t="s">
+      <c r="B15" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="86"/>
-      <c r="D15" s="124" t="s">
+      <c r="C15" s="108"/>
+      <c r="D15" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="124"/>
-      <c r="F15" s="124"/>
-      <c r="G15" s="124"/>
-      <c r="H15" s="124"/>
-      <c r="I15" s="124"/>
-      <c r="J15" s="124"/>
-      <c r="K15" s="124"/>
-      <c r="L15" s="124"/>
-      <c r="M15" s="125"/>
-      <c r="N15" s="107" t="s">
+      <c r="E15" s="95"/>
+      <c r="F15" s="95"/>
+      <c r="G15" s="95"/>
+      <c r="H15" s="95"/>
+      <c r="I15" s="95"/>
+      <c r="J15" s="95"/>
+      <c r="K15" s="95"/>
+      <c r="L15" s="95"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="108"/>
-      <c r="P15" s="108"/>
-      <c r="Q15" s="108"/>
-      <c r="R15" s="108"/>
-      <c r="S15" s="108"/>
-      <c r="T15" s="108"/>
-      <c r="U15" s="108"/>
-      <c r="V15" s="108"/>
-      <c r="W15" s="122"/>
-      <c r="X15" s="108" t="s">
+      <c r="O15" s="90"/>
+      <c r="P15" s="90"/>
+      <c r="Q15" s="90"/>
+      <c r="R15" s="90"/>
+      <c r="S15" s="90"/>
+      <c r="T15" s="90"/>
+      <c r="U15" s="90"/>
+      <c r="V15" s="90"/>
+      <c r="W15" s="91"/>
+      <c r="X15" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="Y15" s="108"/>
-      <c r="Z15" s="122"/>
-      <c r="AA15" s="91" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB15" s="91"/>
-      <c r="AC15" s="91"/>
-      <c r="AD15" s="92"/>
+      <c r="Y15" s="90"/>
+      <c r="Z15" s="91"/>
+      <c r="AA15" s="113" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB15" s="113"/>
+      <c r="AC15" s="113"/>
+      <c r="AD15" s="114"/>
     </row>
     <row r="16" spans="1:36" s="39" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="83"/>
-      <c r="B16" s="87"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="126"/>
-      <c r="E16" s="126"/>
-      <c r="F16" s="126"/>
-      <c r="G16" s="126"/>
-      <c r="H16" s="126"/>
-      <c r="I16" s="126"/>
-      <c r="J16" s="126"/>
-      <c r="K16" s="126"/>
-      <c r="L16" s="126"/>
-      <c r="M16" s="127"/>
-      <c r="N16" s="107" t="s">
+      <c r="A16" s="105"/>
+      <c r="B16" s="109"/>
+      <c r="C16" s="110"/>
+      <c r="D16" s="97"/>
+      <c r="E16" s="97"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="97"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="97"/>
+      <c r="K16" s="97"/>
+      <c r="L16" s="97"/>
+      <c r="M16" s="98"/>
+      <c r="N16" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="O16" s="108"/>
-      <c r="P16" s="108"/>
-      <c r="Q16" s="109"/>
-      <c r="R16" s="107" t="s">
+      <c r="O16" s="90"/>
+      <c r="P16" s="90"/>
+      <c r="Q16" s="100"/>
+      <c r="R16" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="S16" s="108"/>
-      <c r="T16" s="108"/>
-      <c r="U16" s="109"/>
-      <c r="V16" s="105" t="s">
+      <c r="S16" s="90"/>
+      <c r="T16" s="90"/>
+      <c r="U16" s="100"/>
+      <c r="V16" s="126" t="s">
         <v>27</v>
       </c>
-      <c r="W16" s="89" t="s">
-        <v>63</v>
-      </c>
-      <c r="X16" s="118" t="s">
+      <c r="W16" s="111" t="s">
+        <v>62</v>
+      </c>
+      <c r="X16" s="86" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y16" s="88" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z16" s="119" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA16" s="115" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB16" s="116"/>
+      <c r="AC16" s="117" t="s">
         <v>57</v>
       </c>
-      <c r="Y16" s="120" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z16" s="97" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA16" s="93" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB16" s="94"/>
-      <c r="AC16" s="95" t="s">
+      <c r="AD16" s="117" t="s">
         <v>58</v>
       </c>
-      <c r="AD16" s="95" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="17" spans="1:30" s="44" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="84"/>
+      <c r="A17" s="106"/>
       <c r="B17" s="41" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="41" t="s">
         <v>29</v>
@@ -2358,7 +2355,7 @@
         <v>35</v>
       </c>
       <c r="K17" s="42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L17" s="42" t="s">
         <v>48</v>
@@ -2390,19 +2387,19 @@
       <c r="U17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V17" s="106"/>
-      <c r="W17" s="90"/>
-      <c r="X17" s="119"/>
-      <c r="Y17" s="121"/>
-      <c r="Z17" s="98"/>
+      <c r="V17" s="127"/>
+      <c r="W17" s="112"/>
+      <c r="X17" s="87"/>
+      <c r="Y17" s="89"/>
+      <c r="Z17" s="120"/>
       <c r="AA17" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB17" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="AB17" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC17" s="96"/>
-      <c r="AD17" s="96"/>
+      <c r="AC17" s="118"/>
+      <c r="AD17" s="118"/>
     </row>
     <row r="18" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -2443,19 +2440,17 @@
       <c r="AD18" s="47"/>
     </row>
     <row r="19" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="123" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="123"/>
-      <c r="C19" s="123"/>
-      <c r="D19" s="123"/>
-      <c r="E19" s="123"/>
+      <c r="A19" s="92"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="92"/>
       <c r="F19" s="36"/>
       <c r="H19" s="11"/>
-      <c r="L19" s="103" t="s">
+      <c r="L19" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="M19" s="103"/>
+      <c r="M19" s="125"/>
       <c r="N19" s="64"/>
       <c r="O19" s="65"/>
       <c r="P19" s="66"/>
@@ -2475,63 +2470,63 @@
       <c r="AD19" s="47"/>
     </row>
     <row r="20" spans="1:30" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="99" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="99"/>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="99"/>
+      <c r="A20" s="121" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="121"/>
+      <c r="C20" s="121"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="121"/>
       <c r="H20" s="11"/>
-      <c r="L20" s="104" t="s">
+      <c r="L20" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="M20" s="104"/>
-      <c r="N20" s="100"/>
-      <c r="O20" s="101"/>
-      <c r="P20" s="101"/>
-      <c r="Q20" s="101"/>
-      <c r="R20" s="101"/>
-      <c r="S20" s="101"/>
-      <c r="T20" s="101"/>
-      <c r="U20" s="101"/>
-      <c r="V20" s="102"/>
+      <c r="M20" s="85"/>
+      <c r="N20" s="122"/>
+      <c r="O20" s="123"/>
+      <c r="P20" s="123"/>
+      <c r="Q20" s="123"/>
+      <c r="R20" s="123"/>
+      <c r="S20" s="123"/>
+      <c r="T20" s="123"/>
+      <c r="U20" s="123"/>
+      <c r="V20" s="124"/>
       <c r="W20" s="67"/>
     </row>
     <row r="21" spans="1:30" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="H21" s="11"/>
-      <c r="L21" s="104" t="s">
+      <c r="L21" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="M21" s="104"/>
-      <c r="N21" s="79"/>
-      <c r="O21" s="80"/>
-      <c r="P21" s="80"/>
-      <c r="Q21" s="80"/>
-      <c r="R21" s="80"/>
-      <c r="S21" s="80"/>
-      <c r="T21" s="80"/>
-      <c r="U21" s="80"/>
-      <c r="V21" s="80"/>
-      <c r="W21" s="81"/>
+      <c r="M21" s="85"/>
+      <c r="N21" s="101"/>
+      <c r="O21" s="102"/>
+      <c r="P21" s="102"/>
+      <c r="Q21" s="102"/>
+      <c r="R21" s="102"/>
+      <c r="S21" s="102"/>
+      <c r="T21" s="102"/>
+      <c r="U21" s="102"/>
+      <c r="V21" s="102"/>
+      <c r="W21" s="103"/>
     </row>
     <row r="22" spans="1:30" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="H22" s="11"/>
-      <c r="L22" s="104" t="s">
-        <v>65</v>
-      </c>
-      <c r="M22" s="104"/>
-      <c r="N22" s="79"/>
-      <c r="O22" s="80"/>
-      <c r="P22" s="80"/>
-      <c r="Q22" s="80"/>
-      <c r="R22" s="80"/>
-      <c r="S22" s="80"/>
-      <c r="T22" s="80"/>
-      <c r="U22" s="80"/>
-      <c r="V22" s="81"/>
+      <c r="L22" s="85" t="s">
+        <v>64</v>
+      </c>
+      <c r="M22" s="85"/>
+      <c r="N22" s="101"/>
+      <c r="O22" s="102"/>
+      <c r="P22" s="102"/>
+      <c r="Q22" s="102"/>
+      <c r="R22" s="102"/>
+      <c r="S22" s="102"/>
+      <c r="T22" s="102"/>
+      <c r="U22" s="102"/>
+      <c r="V22" s="103"/>
       <c r="W22" s="67"/>
     </row>
     <row r="23" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2548,9 +2543,9 @@
       <c r="AA24" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="AB24" s="113"/>
-      <c r="AC24" s="114"/>
-      <c r="AD24" s="115"/>
+      <c r="AB24" s="80"/>
+      <c r="AC24" s="81"/>
+      <c r="AD24" s="82"/>
     </row>
     <row r="25" spans="1:30" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
@@ -2564,21 +2559,48 @@
       <c r="AA25" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="AB25" s="113"/>
-      <c r="AC25" s="114"/>
-      <c r="AD25" s="115"/>
+      <c r="AB25" s="80"/>
+      <c r="AC25" s="81"/>
+      <c r="AD25" s="82"/>
     </row>
     <row r="27" spans="1:30" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" s="112"/>
-      <c r="C27" s="112"/>
-      <c r="D27" s="112"/>
-      <c r="E27" s="112"/>
+      <c r="A27" s="79" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="79"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="N22:V22"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="AA15:AD15"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="AC16:AC17"/>
+    <mergeCell ref="AD16:AD17"/>
+    <mergeCell ref="Z16:Z17"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="N20:V20"/>
+    <mergeCell ref="N21:W21"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="R16:U16"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J13:L13"/>
     <mergeCell ref="A27:E27"/>
     <mergeCell ref="AB25:AD25"/>
     <mergeCell ref="A1:AD1"/>
@@ -2595,33 +2617,6 @@
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="D15:M16"/>
     <mergeCell ref="N15:W15"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="N22:V22"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="W16:W17"/>
-    <mergeCell ref="AA15:AD15"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="AC16:AC17"/>
-    <mergeCell ref="AD16:AD17"/>
-    <mergeCell ref="Z16:Z17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="N20:V20"/>
-    <mergeCell ref="N21:W21"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="V16:V17"/>
-    <mergeCell ref="R16:U16"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2731,7 +2726,7 @@
     </row>
     <row r="3" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="129" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="129"/>
       <c r="C3" s="129"/>
@@ -2774,7 +2769,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="78" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E5" s="78"/>
       <c r="F5" s="78"/>
@@ -2799,7 +2794,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="78" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" s="78"/>
       <c r="F6" s="78"/>
@@ -2841,7 +2836,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="78" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" s="78"/>
       <c r="F7" s="78"/>
@@ -2963,7 +2958,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="78" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11" s="78"/>
       <c r="F11" s="78"/>
@@ -2995,7 +2990,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="78" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E13" s="78"/>
       <c r="F13" s="78"/>
@@ -3031,6 +3026,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B7BBE98651F7A43AC7BF2F06836443C" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b51c7281b06024c9ff887df9fe3bb465">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8103b6e4-b1cc-417b-af38-f980b3f4bdef" xmlns:ns3="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c056a6abdadb071051b2c083c327215c" ns2:_="" ns3:_="">
     <xsd:import namespace="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
@@ -3247,15 +3251,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
   <ds:schemaRefs>
@@ -3268,6 +3263,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E02BC65-B354-4988-8893-F98AC7F212AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3284,12 +3287,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: ajout d'une phrase sur CCI dans modèle export MCCC Excel
</commit_message>
<xml_diff>
--- a/public/modeles/Annexe_MCCC.xlsx
+++ b/public/modeles/Annexe_MCCC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E36C3D-AE88-F14D-B26C-D3678B703650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273EE88D-F1C5-8A4E-98CB-B5590E2493B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
   <si>
     <t>ACCREDITATION 2024-2028</t>
   </si>
@@ -261,6 +261,9 @@
   <si>
     <t>Type 
 d'enseignement</t>
+  </si>
+  <si>
+    <t>* dans le cas du Cci, la seconde chance se traduit par la non prise en compte dans le calcul de la note finale de la moins bonne des notes de Cci obtenues dans l'enseignement concerné.</t>
   </si>
 </sst>
 </file>
@@ -1264,6 +1267,105 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1282,9 +1384,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1295,9 +1394,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1306,12 +1402,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1323,93 +1413,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1887,8 +1890,8 @@
   </sheetPr>
   <dimension ref="A1:AJ27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="116" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16:X17"/>
+    <sheetView tabSelected="1" topLeftCell="N4" zoomScale="116" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="Z20" sqref="Z20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1917,38 +1920,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="83"/>
-      <c r="V1" s="83"/>
-      <c r="W1" s="83"/>
-      <c r="X1" s="83"/>
-      <c r="Y1" s="83"/>
-      <c r="Z1" s="83"/>
-      <c r="AA1" s="83"/>
-      <c r="AB1" s="83"/>
-      <c r="AC1" s="83"/>
-      <c r="AD1" s="83"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="116"/>
+      <c r="L1" s="116"/>
+      <c r="M1" s="116"/>
+      <c r="N1" s="116"/>
+      <c r="O1" s="116"/>
+      <c r="P1" s="116"/>
+      <c r="Q1" s="116"/>
+      <c r="R1" s="116"/>
+      <c r="S1" s="116"/>
+      <c r="T1" s="116"/>
+      <c r="U1" s="116"/>
+      <c r="V1" s="116"/>
+      <c r="W1" s="116"/>
+      <c r="X1" s="116"/>
+      <c r="Y1" s="116"/>
+      <c r="Z1" s="116"/>
+      <c r="AA1" s="116"/>
+      <c r="AB1" s="116"/>
+      <c r="AC1" s="116"/>
+      <c r="AD1" s="116"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
@@ -1957,87 +1960,87 @@
       <c r="AJ1" s="1"/>
     </row>
     <row r="2" spans="1:36" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="84"/>
-      <c r="R2" s="84"/>
-      <c r="S2" s="84"/>
-      <c r="T2" s="84"/>
-      <c r="U2" s="84"/>
-      <c r="V2" s="84"/>
-      <c r="W2" s="84"/>
-      <c r="X2" s="84"/>
-      <c r="Y2" s="84"/>
-      <c r="Z2" s="84"/>
-      <c r="AA2" s="84"/>
-      <c r="AB2" s="84"/>
-      <c r="AC2" s="84"/>
-      <c r="AD2" s="84"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="117"/>
+      <c r="O2" s="117"/>
+      <c r="P2" s="117"/>
+      <c r="Q2" s="117"/>
+      <c r="R2" s="117"/>
+      <c r="S2" s="117"/>
+      <c r="T2" s="117"/>
+      <c r="U2" s="117"/>
+      <c r="V2" s="117"/>
+      <c r="W2" s="117"/>
+      <c r="X2" s="117"/>
+      <c r="Y2" s="117"/>
+      <c r="Z2" s="117"/>
+      <c r="AA2" s="117"/>
+      <c r="AB2" s="117"/>
+      <c r="AC2" s="117"/>
+      <c r="AD2" s="117"/>
     </row>
     <row r="3" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84"/>
-      <c r="N3" s="84"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="84"/>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="84"/>
-      <c r="S3" s="84"/>
-      <c r="T3" s="84"/>
-      <c r="U3" s="84"/>
-      <c r="V3" s="84"/>
-      <c r="W3" s="84"/>
-      <c r="X3" s="84"/>
-      <c r="Y3" s="84"/>
-      <c r="Z3" s="84"/>
-      <c r="AA3" s="84"/>
-      <c r="AB3" s="84"/>
-      <c r="AC3" s="84"/>
-      <c r="AD3" s="84"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="117"/>
+      <c r="I3" s="117"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="117"/>
+      <c r="L3" s="117"/>
+      <c r="M3" s="117"/>
+      <c r="N3" s="117"/>
+      <c r="O3" s="117"/>
+      <c r="P3" s="117"/>
+      <c r="Q3" s="117"/>
+      <c r="R3" s="117"/>
+      <c r="S3" s="117"/>
+      <c r="T3" s="117"/>
+      <c r="U3" s="117"/>
+      <c r="V3" s="117"/>
+      <c r="W3" s="117"/>
+      <c r="X3" s="117"/>
+      <c r="Y3" s="117"/>
+      <c r="Z3" s="117"/>
+      <c r="AA3" s="117"/>
+      <c r="AB3" s="117"/>
+      <c r="AC3" s="117"/>
+      <c r="AD3" s="117"/>
     </row>
     <row r="4" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="93" t="s">
+      <c r="G5" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94" t="s">
+      <c r="H5" s="110"/>
+      <c r="I5" s="110"/>
+      <c r="J5" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="94"/>
-      <c r="L5" s="94"/>
+      <c r="K5" s="111"/>
+      <c r="L5" s="111"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -2051,16 +2054,16 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="93" t="s">
+      <c r="G6" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94" t="s">
+      <c r="H6" s="110"/>
+      <c r="I6" s="110"/>
+      <c r="J6" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="94"/>
-      <c r="L6" s="94"/>
+      <c r="K6" s="111"/>
+      <c r="L6" s="111"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -2086,16 +2089,16 @@
         <v>8</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="93" t="s">
+      <c r="G7" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="94" t="s">
+      <c r="H7" s="110"/>
+      <c r="I7" s="110"/>
+      <c r="J7" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94"/>
+      <c r="K7" s="111"/>
+      <c r="L7" s="111"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -2137,16 +2140,16 @@
         <v>11</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="93" t="s">
+      <c r="G9" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94" t="s">
+      <c r="H9" s="110"/>
+      <c r="I9" s="110"/>
+      <c r="J9" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
+      <c r="K9" s="111"/>
+      <c r="L9" s="111"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -2180,16 +2183,16 @@
         <v>14</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="93" t="s">
+      <c r="G11" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="93"/>
-      <c r="I11" s="93"/>
-      <c r="J11" s="94" t="s">
+      <c r="H11" s="110"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="111" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="94"/>
-      <c r="L11" s="94"/>
+      <c r="K11" s="111"/>
+      <c r="L11" s="111"/>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:36" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2210,16 +2213,16 @@
         <v>17</v>
       </c>
       <c r="F13" s="7"/>
-      <c r="G13" s="93" t="s">
+      <c r="G13" s="110" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
-      <c r="J13" s="94" t="s">
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
+      <c r="J13" s="111" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="94"/>
-      <c r="L13" s="94"/>
+      <c r="K13" s="111"/>
+      <c r="L13" s="111"/>
       <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:36" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2230,103 +2233,103 @@
       <c r="M14"/>
     </row>
     <row r="15" spans="1:36" s="39" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="104" t="s">
+      <c r="A15" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="107" t="s">
+      <c r="B15" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="108"/>
-      <c r="D15" s="95" t="s">
+      <c r="C15" s="86"/>
+      <c r="D15" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="95"/>
-      <c r="F15" s="95"/>
-      <c r="G15" s="95"/>
-      <c r="H15" s="95"/>
-      <c r="I15" s="95"/>
-      <c r="J15" s="95"/>
-      <c r="K15" s="95"/>
-      <c r="L15" s="95"/>
-      <c r="M15" s="96"/>
-      <c r="N15" s="99" t="s">
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="124"/>
+      <c r="I15" s="124"/>
+      <c r="J15" s="124"/>
+      <c r="K15" s="124"/>
+      <c r="L15" s="124"/>
+      <c r="M15" s="125"/>
+      <c r="N15" s="107" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="90"/>
-      <c r="P15" s="90"/>
-      <c r="Q15" s="90"/>
-      <c r="R15" s="90"/>
-      <c r="S15" s="90"/>
-      <c r="T15" s="90"/>
-      <c r="U15" s="90"/>
-      <c r="V15" s="90"/>
-      <c r="W15" s="91"/>
-      <c r="X15" s="90" t="s">
+      <c r="O15" s="108"/>
+      <c r="P15" s="108"/>
+      <c r="Q15" s="108"/>
+      <c r="R15" s="108"/>
+      <c r="S15" s="108"/>
+      <c r="T15" s="108"/>
+      <c r="U15" s="108"/>
+      <c r="V15" s="108"/>
+      <c r="W15" s="122"/>
+      <c r="X15" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="Y15" s="90"/>
-      <c r="Z15" s="91"/>
-      <c r="AA15" s="113" t="s">
+      <c r="Y15" s="108"/>
+      <c r="Z15" s="122"/>
+      <c r="AA15" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="AB15" s="113"/>
-      <c r="AC15" s="113"/>
-      <c r="AD15" s="114"/>
+      <c r="AB15" s="91"/>
+      <c r="AC15" s="91"/>
+      <c r="AD15" s="92"/>
     </row>
     <row r="16" spans="1:36" s="39" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="105"/>
-      <c r="B16" s="109"/>
-      <c r="C16" s="110"/>
-      <c r="D16" s="97"/>
-      <c r="E16" s="97"/>
-      <c r="F16" s="97"/>
-      <c r="G16" s="97"/>
-      <c r="H16" s="97"/>
-      <c r="I16" s="97"/>
-      <c r="J16" s="97"/>
-      <c r="K16" s="97"/>
-      <c r="L16" s="97"/>
-      <c r="M16" s="98"/>
-      <c r="N16" s="99" t="s">
+      <c r="A16" s="83"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="88"/>
+      <c r="D16" s="126"/>
+      <c r="E16" s="126"/>
+      <c r="F16" s="126"/>
+      <c r="G16" s="126"/>
+      <c r="H16" s="126"/>
+      <c r="I16" s="126"/>
+      <c r="J16" s="126"/>
+      <c r="K16" s="126"/>
+      <c r="L16" s="126"/>
+      <c r="M16" s="127"/>
+      <c r="N16" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="O16" s="90"/>
-      <c r="P16" s="90"/>
-      <c r="Q16" s="100"/>
-      <c r="R16" s="99" t="s">
+      <c r="O16" s="108"/>
+      <c r="P16" s="108"/>
+      <c r="Q16" s="109"/>
+      <c r="R16" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="S16" s="90"/>
-      <c r="T16" s="90"/>
-      <c r="U16" s="100"/>
-      <c r="V16" s="126" t="s">
+      <c r="S16" s="108"/>
+      <c r="T16" s="108"/>
+      <c r="U16" s="109"/>
+      <c r="V16" s="105" t="s">
         <v>27</v>
       </c>
-      <c r="W16" s="111" t="s">
+      <c r="W16" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="X16" s="86" t="s">
+      <c r="X16" s="118" t="s">
         <v>56</v>
       </c>
-      <c r="Y16" s="88" t="s">
+      <c r="Y16" s="120" t="s">
         <v>52</v>
       </c>
-      <c r="Z16" s="119" t="s">
+      <c r="Z16" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="AA16" s="115" t="s">
+      <c r="AA16" s="93" t="s">
         <v>61</v>
       </c>
-      <c r="AB16" s="116"/>
-      <c r="AC16" s="117" t="s">
+      <c r="AB16" s="94"/>
+      <c r="AC16" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="AD16" s="117" t="s">
+      <c r="AD16" s="95" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:30" s="44" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="106"/>
+      <c r="A17" s="84"/>
       <c r="B17" s="41" t="s">
         <v>28</v>
       </c>
@@ -2387,19 +2390,19 @@
       <c r="U17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V17" s="127"/>
-      <c r="W17" s="112"/>
-      <c r="X17" s="87"/>
-      <c r="Y17" s="89"/>
-      <c r="Z17" s="120"/>
+      <c r="V17" s="106"/>
+      <c r="W17" s="90"/>
+      <c r="X17" s="119"/>
+      <c r="Y17" s="121"/>
+      <c r="Z17" s="98"/>
       <c r="AA17" s="49" t="s">
         <v>59</v>
       </c>
       <c r="AB17" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="AC17" s="118"/>
-      <c r="AD17" s="118"/>
+      <c r="AC17" s="96"/>
+      <c r="AD17" s="96"/>
     </row>
     <row r="18" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -2440,17 +2443,19 @@
       <c r="AD18" s="47"/>
     </row>
     <row r="19" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="92"/>
-      <c r="B19" s="92"/>
-      <c r="C19" s="92"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
+      <c r="A19" s="123" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="123"/>
+      <c r="C19" s="123"/>
+      <c r="D19" s="123"/>
+      <c r="E19" s="123"/>
       <c r="F19" s="36"/>
       <c r="H19" s="11"/>
-      <c r="L19" s="125" t="s">
+      <c r="L19" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="M19" s="125"/>
+      <c r="M19" s="103"/>
       <c r="N19" s="64"/>
       <c r="O19" s="65"/>
       <c r="P19" s="66"/>
@@ -2470,63 +2475,63 @@
       <c r="AD19" s="47"/>
     </row>
     <row r="20" spans="1:30" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="121" t="s">
+      <c r="A20" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="121"/>
-      <c r="C20" s="121"/>
-      <c r="D20" s="121"/>
-      <c r="E20" s="121"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="99"/>
+      <c r="D20" s="99"/>
+      <c r="E20" s="99"/>
       <c r="H20" s="11"/>
-      <c r="L20" s="85" t="s">
+      <c r="L20" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="M20" s="85"/>
-      <c r="N20" s="122"/>
-      <c r="O20" s="123"/>
-      <c r="P20" s="123"/>
-      <c r="Q20" s="123"/>
-      <c r="R20" s="123"/>
-      <c r="S20" s="123"/>
-      <c r="T20" s="123"/>
-      <c r="U20" s="123"/>
-      <c r="V20" s="124"/>
+      <c r="M20" s="104"/>
+      <c r="N20" s="100"/>
+      <c r="O20" s="101"/>
+      <c r="P20" s="101"/>
+      <c r="Q20" s="101"/>
+      <c r="R20" s="101"/>
+      <c r="S20" s="101"/>
+      <c r="T20" s="101"/>
+      <c r="U20" s="101"/>
+      <c r="V20" s="102"/>
       <c r="W20" s="67"/>
     </row>
     <row r="21" spans="1:30" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="H21" s="11"/>
-      <c r="L21" s="85" t="s">
+      <c r="L21" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="M21" s="85"/>
-      <c r="N21" s="101"/>
-      <c r="O21" s="102"/>
-      <c r="P21" s="102"/>
-      <c r="Q21" s="102"/>
-      <c r="R21" s="102"/>
-      <c r="S21" s="102"/>
-      <c r="T21" s="102"/>
-      <c r="U21" s="102"/>
-      <c r="V21" s="102"/>
-      <c r="W21" s="103"/>
+      <c r="M21" s="104"/>
+      <c r="N21" s="79"/>
+      <c r="O21" s="80"/>
+      <c r="P21" s="80"/>
+      <c r="Q21" s="80"/>
+      <c r="R21" s="80"/>
+      <c r="S21" s="80"/>
+      <c r="T21" s="80"/>
+      <c r="U21" s="80"/>
+      <c r="V21" s="80"/>
+      <c r="W21" s="81"/>
     </row>
     <row r="22" spans="1:30" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="H22" s="11"/>
-      <c r="L22" s="85" t="s">
+      <c r="L22" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="M22" s="85"/>
-      <c r="N22" s="101"/>
-      <c r="O22" s="102"/>
-      <c r="P22" s="102"/>
-      <c r="Q22" s="102"/>
-      <c r="R22" s="102"/>
-      <c r="S22" s="102"/>
-      <c r="T22" s="102"/>
-      <c r="U22" s="102"/>
-      <c r="V22" s="103"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="79"/>
+      <c r="O22" s="80"/>
+      <c r="P22" s="80"/>
+      <c r="Q22" s="80"/>
+      <c r="R22" s="80"/>
+      <c r="S22" s="80"/>
+      <c r="T22" s="80"/>
+      <c r="U22" s="80"/>
+      <c r="V22" s="81"/>
       <c r="W22" s="67"/>
     </row>
     <row r="23" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2543,9 +2548,9 @@
       <c r="AA24" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="AB24" s="80"/>
-      <c r="AC24" s="81"/>
-      <c r="AD24" s="82"/>
+      <c r="AB24" s="113"/>
+      <c r="AC24" s="114"/>
+      <c r="AD24" s="115"/>
     </row>
     <row r="25" spans="1:30" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
@@ -2559,21 +2564,48 @@
       <c r="AA25" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="AB25" s="80"/>
-      <c r="AC25" s="81"/>
-      <c r="AD25" s="82"/>
+      <c r="AB25" s="113"/>
+      <c r="AC25" s="114"/>
+      <c r="AD25" s="115"/>
     </row>
     <row r="27" spans="1:30" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="79" t="s">
+      <c r="A27" s="112" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="79"/>
-      <c r="C27" s="79"/>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
+      <c r="B27" s="112"/>
+      <c r="C27" s="112"/>
+      <c r="D27" s="112"/>
+      <c r="E27" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="AB25:AD25"/>
+    <mergeCell ref="A1:AD1"/>
+    <mergeCell ref="A2:AD2"/>
+    <mergeCell ref="A3:AD3"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="AB24:AD24"/>
+    <mergeCell ref="X16:X17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="X15:Z15"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="D15:M16"/>
+    <mergeCell ref="N15:W15"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G13:I13"/>
     <mergeCell ref="N22:V22"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:C16"/>
@@ -2590,33 +2622,6 @@
     <mergeCell ref="L20:M20"/>
     <mergeCell ref="V16:V17"/>
     <mergeCell ref="R16:U16"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="AB25:AD25"/>
-    <mergeCell ref="A1:AD1"/>
-    <mergeCell ref="A2:AD2"/>
-    <mergeCell ref="A3:AD3"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="AB24:AD24"/>
-    <mergeCell ref="X16:X17"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="X15:Z15"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="D15:M16"/>
-    <mergeCell ref="N15:W15"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3015,26 +3020,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B7BBE98651F7A43AC7BF2F06836443C" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b51c7281b06024c9ff887df9fe3bb465">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8103b6e4-b1cc-417b-af38-f980b3f4bdef" xmlns:ns3="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c056a6abdadb071051b2c083c327215c" ns2:_="" ns3:_="">
     <xsd:import namespace="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
@@ -3251,26 +3236,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
-    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E02BC65-B354-4988-8893-F98AC7F212AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3287,4 +3273,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
+    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: mise ne page excel, taille des cellules du parcours
</commit_message>
<xml_diff>
--- a/public/modeles/Annexe_MCCC.xlsx
+++ b/public/modeles/Annexe_MCCC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD9C1FC-7BB5-5F4C-B1A4-51B9A39CB241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC0D846-78B1-9C42-969D-8BE886D74D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30900" yWindow="2220" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1267,6 +1267,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1419,9 +1422,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1893,8 +1893,8 @@
   </sheetPr>
   <dimension ref="A1:AJ27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I4" zoomScale="116" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="116" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1923,38 +1923,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="83"/>
-      <c r="V1" s="83"/>
-      <c r="W1" s="83"/>
-      <c r="X1" s="83"/>
-      <c r="Y1" s="83"/>
-      <c r="Z1" s="83"/>
-      <c r="AA1" s="83"/>
-      <c r="AB1" s="83"/>
-      <c r="AC1" s="83"/>
-      <c r="AD1" s="83"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
@@ -1963,87 +1963,87 @@
       <c r="AJ1" s="1"/>
     </row>
     <row r="2" spans="1:36" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="84"/>
-      <c r="R2" s="84"/>
-      <c r="S2" s="84"/>
-      <c r="T2" s="84"/>
-      <c r="U2" s="84"/>
-      <c r="V2" s="84"/>
-      <c r="W2" s="84"/>
-      <c r="X2" s="84"/>
-      <c r="Y2" s="84"/>
-      <c r="Z2" s="84"/>
-      <c r="AA2" s="84"/>
-      <c r="AB2" s="84"/>
-      <c r="AC2" s="84"/>
-      <c r="AD2" s="84"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="85"/>
+      <c r="U2" s="85"/>
+      <c r="V2" s="85"/>
+      <c r="W2" s="85"/>
+      <c r="X2" s="85"/>
+      <c r="Y2" s="85"/>
+      <c r="Z2" s="85"/>
+      <c r="AA2" s="85"/>
+      <c r="AB2" s="85"/>
+      <c r="AC2" s="85"/>
+      <c r="AD2" s="85"/>
     </row>
     <row r="3" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84"/>
-      <c r="N3" s="84"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="84"/>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="84"/>
-      <c r="S3" s="84"/>
-      <c r="T3" s="84"/>
-      <c r="U3" s="84"/>
-      <c r="V3" s="84"/>
-      <c r="W3" s="84"/>
-      <c r="X3" s="84"/>
-      <c r="Y3" s="84"/>
-      <c r="Z3" s="84"/>
-      <c r="AA3" s="84"/>
-      <c r="AB3" s="84"/>
-      <c r="AC3" s="84"/>
-      <c r="AD3" s="84"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
+      <c r="V3" s="85"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="85"/>
+      <c r="Y3" s="85"/>
+      <c r="Z3" s="85"/>
+      <c r="AA3" s="85"/>
+      <c r="AB3" s="85"/>
+      <c r="AC3" s="85"/>
+      <c r="AD3" s="85"/>
     </row>
     <row r="4" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="93" t="s">
+      <c r="G5" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94" t="s">
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="94"/>
-      <c r="L5" s="94"/>
+      <c r="K5" s="95"/>
+      <c r="L5" s="95"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -2057,26 +2057,26 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="93" t="s">
+      <c r="G6" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94" t="s">
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="94"/>
-      <c r="L6" s="94"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="95"/>
+      <c r="M6" s="95"/>
+      <c r="N6" s="95"/>
+      <c r="O6" s="95"/>
+      <c r="P6" s="95"/>
+      <c r="Q6" s="95"/>
+      <c r="R6" s="95"/>
+      <c r="S6" s="95"/>
+      <c r="T6" s="95"/>
+      <c r="U6" s="95"/>
+      <c r="V6" s="95"/>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
@@ -2092,23 +2092,26 @@
         <v>8</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="93" t="s">
+      <c r="G7" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="94" t="s">
+      <c r="H7" s="94"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="95"/>
+      <c r="M7" s="95"/>
+      <c r="N7" s="95"/>
+      <c r="O7" s="95"/>
+      <c r="P7" s="95"/>
+      <c r="Q7" s="95"/>
+      <c r="R7" s="95"/>
+      <c r="S7" s="95"/>
+      <c r="T7" s="95"/>
+      <c r="U7" s="95"/>
+      <c r="V7" s="95"/>
     </row>
     <row r="8" spans="1:36" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="7"/>
@@ -2143,16 +2146,16 @@
         <v>11</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="93" t="s">
+      <c r="G9" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94" t="s">
+      <c r="H9" s="94"/>
+      <c r="I9" s="94"/>
+      <c r="J9" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
+      <c r="K9" s="95"/>
+      <c r="L9" s="95"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -2186,16 +2189,16 @@
         <v>14</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="93" t="s">
+      <c r="G11" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="93"/>
-      <c r="I11" s="93"/>
-      <c r="J11" s="94" t="s">
+      <c r="H11" s="94"/>
+      <c r="I11" s="94"/>
+      <c r="J11" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="94"/>
-      <c r="L11" s="94"/>
+      <c r="K11" s="95"/>
+      <c r="L11" s="95"/>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:36" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2216,16 +2219,16 @@
         <v>17</v>
       </c>
       <c r="F13" s="7"/>
-      <c r="G13" s="93" t="s">
+      <c r="G13" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
-      <c r="J13" s="94" t="s">
+      <c r="H13" s="94"/>
+      <c r="I13" s="94"/>
+      <c r="J13" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="94"/>
-      <c r="L13" s="94"/>
+      <c r="K13" s="95"/>
+      <c r="L13" s="95"/>
       <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:36" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2236,103 +2239,103 @@
       <c r="M14"/>
     </row>
     <row r="15" spans="1:36" s="39" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="104" t="s">
+      <c r="A15" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="107" t="s">
+      <c r="B15" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="108"/>
-      <c r="D15" s="95" t="s">
+      <c r="C15" s="109"/>
+      <c r="D15" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="95"/>
-      <c r="F15" s="95"/>
-      <c r="G15" s="95"/>
-      <c r="H15" s="95"/>
-      <c r="I15" s="95"/>
-      <c r="J15" s="95"/>
-      <c r="K15" s="95"/>
-      <c r="L15" s="95"/>
-      <c r="M15" s="96"/>
-      <c r="N15" s="99" t="s">
+      <c r="E15" s="96"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="96"/>
+      <c r="H15" s="96"/>
+      <c r="I15" s="96"/>
+      <c r="J15" s="96"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="96"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="90"/>
-      <c r="P15" s="90"/>
-      <c r="Q15" s="90"/>
-      <c r="R15" s="90"/>
-      <c r="S15" s="90"/>
-      <c r="T15" s="90"/>
-      <c r="U15" s="90"/>
-      <c r="V15" s="90"/>
-      <c r="W15" s="91"/>
-      <c r="X15" s="90" t="s">
+      <c r="O15" s="91"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
+      <c r="R15" s="91"/>
+      <c r="S15" s="91"/>
+      <c r="T15" s="91"/>
+      <c r="U15" s="91"/>
+      <c r="V15" s="91"/>
+      <c r="W15" s="92"/>
+      <c r="X15" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="Y15" s="90"/>
-      <c r="Z15" s="91"/>
-      <c r="AA15" s="113" t="s">
+      <c r="Y15" s="91"/>
+      <c r="Z15" s="92"/>
+      <c r="AA15" s="114" t="s">
         <v>54</v>
       </c>
-      <c r="AB15" s="113"/>
-      <c r="AC15" s="113"/>
-      <c r="AD15" s="114"/>
+      <c r="AB15" s="114"/>
+      <c r="AC15" s="114"/>
+      <c r="AD15" s="115"/>
     </row>
     <row r="16" spans="1:36" s="39" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="105"/>
-      <c r="B16" s="109"/>
-      <c r="C16" s="110"/>
-      <c r="D16" s="97"/>
-      <c r="E16" s="97"/>
-      <c r="F16" s="97"/>
-      <c r="G16" s="97"/>
-      <c r="H16" s="97"/>
-      <c r="I16" s="97"/>
-      <c r="J16" s="97"/>
-      <c r="K16" s="97"/>
-      <c r="L16" s="97"/>
-      <c r="M16" s="98"/>
-      <c r="N16" s="99" t="s">
+      <c r="A16" s="106"/>
+      <c r="B16" s="110"/>
+      <c r="C16" s="111"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="98"/>
+      <c r="J16" s="98"/>
+      <c r="K16" s="98"/>
+      <c r="L16" s="98"/>
+      <c r="M16" s="99"/>
+      <c r="N16" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="O16" s="90"/>
-      <c r="P16" s="90"/>
-      <c r="Q16" s="100"/>
-      <c r="R16" s="99" t="s">
+      <c r="O16" s="91"/>
+      <c r="P16" s="91"/>
+      <c r="Q16" s="101"/>
+      <c r="R16" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="S16" s="90"/>
-      <c r="T16" s="90"/>
-      <c r="U16" s="100"/>
-      <c r="V16" s="126" t="s">
+      <c r="S16" s="91"/>
+      <c r="T16" s="91"/>
+      <c r="U16" s="101"/>
+      <c r="V16" s="127" t="s">
         <v>27</v>
       </c>
-      <c r="W16" s="111" t="s">
+      <c r="W16" s="112" t="s">
         <v>62</v>
       </c>
-      <c r="X16" s="86" t="s">
+      <c r="X16" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="Y16" s="88" t="s">
+      <c r="Y16" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="Z16" s="119" t="s">
+      <c r="Z16" s="120" t="s">
         <v>53</v>
       </c>
-      <c r="AA16" s="115" t="s">
+      <c r="AA16" s="116" t="s">
         <v>61</v>
       </c>
-      <c r="AB16" s="116"/>
-      <c r="AC16" s="117" t="s">
+      <c r="AB16" s="117"/>
+      <c r="AC16" s="118" t="s">
         <v>57</v>
       </c>
-      <c r="AD16" s="117" t="s">
+      <c r="AD16" s="118" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:30" s="44" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="106"/>
+      <c r="A17" s="107"/>
       <c r="B17" s="41" t="s">
         <v>28</v>
       </c>
@@ -2393,19 +2396,19 @@
       <c r="U17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V17" s="127"/>
-      <c r="W17" s="112"/>
-      <c r="X17" s="87"/>
-      <c r="Y17" s="89"/>
-      <c r="Z17" s="120"/>
+      <c r="V17" s="128"/>
+      <c r="W17" s="113"/>
+      <c r="X17" s="88"/>
+      <c r="Y17" s="90"/>
+      <c r="Z17" s="121"/>
       <c r="AA17" s="49" t="s">
         <v>59</v>
       </c>
       <c r="AB17" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="AC17" s="118"/>
-      <c r="AD17" s="118"/>
+      <c r="AC17" s="119"/>
+      <c r="AD17" s="119"/>
     </row>
     <row r="18" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -2425,7 +2428,7 @@
       <c r="I18" s="24"/>
       <c r="J18" s="18"/>
       <c r="K18" s="34"/>
-      <c r="L18" s="130"/>
+      <c r="L18" s="79"/>
       <c r="M18" s="28"/>
       <c r="N18" s="26"/>
       <c r="O18" s="27"/>
@@ -2446,19 +2449,19 @@
       <c r="AD18" s="47"/>
     </row>
     <row r="19" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="92" t="s">
+      <c r="A19" s="93" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="92"/>
-      <c r="C19" s="92"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
+      <c r="B19" s="93"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="93"/>
       <c r="F19" s="36"/>
       <c r="H19" s="11"/>
-      <c r="L19" s="125" t="s">
+      <c r="L19" s="126" t="s">
         <v>49</v>
       </c>
-      <c r="M19" s="125"/>
+      <c r="M19" s="126"/>
       <c r="N19" s="64"/>
       <c r="O19" s="65"/>
       <c r="P19" s="66"/>
@@ -2478,63 +2481,63 @@
       <c r="AD19" s="47"/>
     </row>
     <row r="20" spans="1:30" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="121" t="s">
+      <c r="A20" s="122" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="121"/>
-      <c r="C20" s="121"/>
-      <c r="D20" s="121"/>
-      <c r="E20" s="121"/>
+      <c r="B20" s="122"/>
+      <c r="C20" s="122"/>
+      <c r="D20" s="122"/>
+      <c r="E20" s="122"/>
       <c r="H20" s="11"/>
-      <c r="L20" s="85" t="s">
+      <c r="L20" s="86" t="s">
         <v>50</v>
       </c>
-      <c r="M20" s="85"/>
-      <c r="N20" s="122"/>
-      <c r="O20" s="123"/>
-      <c r="P20" s="123"/>
-      <c r="Q20" s="123"/>
-      <c r="R20" s="123"/>
-      <c r="S20" s="123"/>
-      <c r="T20" s="123"/>
-      <c r="U20" s="123"/>
-      <c r="V20" s="124"/>
+      <c r="M20" s="86"/>
+      <c r="N20" s="123"/>
+      <c r="O20" s="124"/>
+      <c r="P20" s="124"/>
+      <c r="Q20" s="124"/>
+      <c r="R20" s="124"/>
+      <c r="S20" s="124"/>
+      <c r="T20" s="124"/>
+      <c r="U20" s="124"/>
+      <c r="V20" s="125"/>
       <c r="W20" s="67"/>
     </row>
     <row r="21" spans="1:30" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="H21" s="11"/>
-      <c r="L21" s="85" t="s">
+      <c r="L21" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="M21" s="85"/>
-      <c r="N21" s="101"/>
-      <c r="O21" s="102"/>
-      <c r="P21" s="102"/>
-      <c r="Q21" s="102"/>
-      <c r="R21" s="102"/>
-      <c r="S21" s="102"/>
-      <c r="T21" s="102"/>
-      <c r="U21" s="102"/>
-      <c r="V21" s="102"/>
-      <c r="W21" s="103"/>
+      <c r="M21" s="86"/>
+      <c r="N21" s="102"/>
+      <c r="O21" s="103"/>
+      <c r="P21" s="103"/>
+      <c r="Q21" s="103"/>
+      <c r="R21" s="103"/>
+      <c r="S21" s="103"/>
+      <c r="T21" s="103"/>
+      <c r="U21" s="103"/>
+      <c r="V21" s="103"/>
+      <c r="W21" s="104"/>
     </row>
     <row r="22" spans="1:30" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="H22" s="11"/>
-      <c r="L22" s="85" t="s">
+      <c r="L22" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="M22" s="85"/>
-      <c r="N22" s="101"/>
-      <c r="O22" s="102"/>
-      <c r="P22" s="102"/>
-      <c r="Q22" s="102"/>
-      <c r="R22" s="102"/>
-      <c r="S22" s="102"/>
-      <c r="T22" s="102"/>
-      <c r="U22" s="102"/>
-      <c r="V22" s="103"/>
+      <c r="M22" s="86"/>
+      <c r="N22" s="102"/>
+      <c r="O22" s="103"/>
+      <c r="P22" s="103"/>
+      <c r="Q22" s="103"/>
+      <c r="R22" s="103"/>
+      <c r="S22" s="103"/>
+      <c r="T22" s="103"/>
+      <c r="U22" s="103"/>
+      <c r="V22" s="104"/>
       <c r="W22" s="67"/>
     </row>
     <row r="23" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2551,9 +2554,9 @@
       <c r="AA24" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="AB24" s="80"/>
-      <c r="AC24" s="81"/>
-      <c r="AD24" s="82"/>
+      <c r="AB24" s="81"/>
+      <c r="AC24" s="82"/>
+      <c r="AD24" s="83"/>
     </row>
     <row r="25" spans="1:30" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
@@ -2567,30 +2570,31 @@
       <c r="AA25" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="AB25" s="80"/>
-      <c r="AC25" s="81"/>
-      <c r="AD25" s="82"/>
+      <c r="AB25" s="81"/>
+      <c r="AC25" s="82"/>
+      <c r="AD25" s="83"/>
     </row>
     <row r="27" spans="1:30" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="79" t="s">
+      <c r="A27" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="79"/>
-      <c r="C27" s="79"/>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
+      <c r="B27" s="80"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="N22:V22"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="W16:W17"/>
     <mergeCell ref="AA15:AD15"/>
     <mergeCell ref="AA16:AB16"/>
     <mergeCell ref="AC16:AC17"/>
     <mergeCell ref="AD16:AD17"/>
     <mergeCell ref="Z16:Z17"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="N22:V22"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="W16:W17"/>
     <mergeCell ref="A20:E20"/>
     <mergeCell ref="N20:V20"/>
     <mergeCell ref="N21:W21"/>
@@ -2602,10 +2606,9 @@
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J6:V6"/>
+    <mergeCell ref="J7:V7"/>
     <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="J13:L13"/>
@@ -2657,15 +2660,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
       <c r="H1" s="62"/>
       <c r="I1" s="62"/>
       <c r="J1" s="62"/>
@@ -2704,15 +2707,15 @@
       <c r="BA1" s="1"/>
     </row>
     <row r="2" spans="1:53" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="130" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="129"/>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="129"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="130"/>
       <c r="H2" s="63"/>
       <c r="I2" s="63"/>
       <c r="J2" s="63"/>
@@ -2733,15 +2736,15 @@
       <c r="Y2" s="63"/>
     </row>
     <row r="3" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="129" t="s">
+      <c r="A3" s="130" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="129"/>
-      <c r="C3" s="129"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
+      <c r="B3" s="130"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
       <c r="H3" s="63"/>
       <c r="I3" s="63"/>
       <c r="J3" s="63"/>

</xml_diff>

<commit_message>
fix: EC enfant sur nouvel EC
</commit_message>
<xml_diff>
--- a/public/modeles/Annexe_MCCC.xlsx
+++ b/public/modeles/Annexe_MCCC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD60BF8-8A55-7A46-88A4-DFCB35567D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959C0692-D7ED-A242-B951-9528CE2D1749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modele" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="75">
   <si>
     <t>ACCREDITATION 2024-2028</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>* dans le cas du Cci, la seconde chance se traduit par la non prise en compte dans le calcul de la note finale de la moins bonne des notes de Cci obtenues dans l'enseignement concerné.</t>
+  </si>
+  <si>
+    <t>*** Les choix d'EC dans le cas d'EC à choix restreint ou libre doivent être différent au sein d'un même semestre</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1040,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1270,158 +1273,161 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1893,8 +1899,8 @@
   </sheetPr>
   <dimension ref="A1:AJ27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="116" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9:L9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="116" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1923,38 +1929,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="117"/>
-      <c r="U1" s="117"/>
-      <c r="V1" s="117"/>
-      <c r="W1" s="117"/>
-      <c r="X1" s="117"/>
-      <c r="Y1" s="117"/>
-      <c r="Z1" s="117"/>
-      <c r="AA1" s="117"/>
-      <c r="AB1" s="117"/>
-      <c r="AC1" s="117"/>
-      <c r="AD1" s="117"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
@@ -1963,87 +1969,87 @@
       <c r="AJ1" s="1"/>
     </row>
     <row r="2" spans="1:36" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="118"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="118"/>
-      <c r="M2" s="118"/>
-      <c r="N2" s="118"/>
-      <c r="O2" s="118"/>
-      <c r="P2" s="118"/>
-      <c r="Q2" s="118"/>
-      <c r="R2" s="118"/>
-      <c r="S2" s="118"/>
-      <c r="T2" s="118"/>
-      <c r="U2" s="118"/>
-      <c r="V2" s="118"/>
-      <c r="W2" s="118"/>
-      <c r="X2" s="118"/>
-      <c r="Y2" s="118"/>
-      <c r="Z2" s="118"/>
-      <c r="AA2" s="118"/>
-      <c r="AB2" s="118"/>
-      <c r="AC2" s="118"/>
-      <c r="AD2" s="118"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="85"/>
+      <c r="U2" s="85"/>
+      <c r="V2" s="85"/>
+      <c r="W2" s="85"/>
+      <c r="X2" s="85"/>
+      <c r="Y2" s="85"/>
+      <c r="Z2" s="85"/>
+      <c r="AA2" s="85"/>
+      <c r="AB2" s="85"/>
+      <c r="AC2" s="85"/>
+      <c r="AD2" s="85"/>
     </row>
     <row r="3" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="118"/>
-      <c r="J3" s="118"/>
-      <c r="K3" s="118"/>
-      <c r="L3" s="118"/>
-      <c r="M3" s="118"/>
-      <c r="N3" s="118"/>
-      <c r="O3" s="118"/>
-      <c r="P3" s="118"/>
-      <c r="Q3" s="118"/>
-      <c r="R3" s="118"/>
-      <c r="S3" s="118"/>
-      <c r="T3" s="118"/>
-      <c r="U3" s="118"/>
-      <c r="V3" s="118"/>
-      <c r="W3" s="118"/>
-      <c r="X3" s="118"/>
-      <c r="Y3" s="118"/>
-      <c r="Z3" s="118"/>
-      <c r="AA3" s="118"/>
-      <c r="AB3" s="118"/>
-      <c r="AC3" s="118"/>
-      <c r="AD3" s="118"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
+      <c r="V3" s="85"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="85"/>
+      <c r="Y3" s="85"/>
+      <c r="Z3" s="85"/>
+      <c r="AA3" s="85"/>
+      <c r="AB3" s="85"/>
+      <c r="AC3" s="85"/>
+      <c r="AD3" s="85"/>
     </row>
     <row r="4" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="88" t="s">
+      <c r="G5" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="112" t="s">
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="112"/>
-      <c r="L5" s="112"/>
+      <c r="K5" s="94"/>
+      <c r="L5" s="94"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -2057,26 +2063,26 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="88" t="s">
+      <c r="G6" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="88"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="112" t="s">
+      <c r="H6" s="93"/>
+      <c r="I6" s="93"/>
+      <c r="J6" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="112"/>
-      <c r="L6" s="112"/>
-      <c r="M6" s="112"/>
-      <c r="N6" s="112"/>
-      <c r="O6" s="112"/>
-      <c r="P6" s="112"/>
-      <c r="Q6" s="112"/>
-      <c r="R6" s="112"/>
-      <c r="S6" s="112"/>
-      <c r="T6" s="112"/>
-      <c r="U6" s="112"/>
-      <c r="V6" s="112"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="94"/>
+      <c r="M6" s="94"/>
+      <c r="N6" s="94"/>
+      <c r="O6" s="94"/>
+      <c r="P6" s="94"/>
+      <c r="Q6" s="94"/>
+      <c r="R6" s="94"/>
+      <c r="S6" s="94"/>
+      <c r="T6" s="94"/>
+      <c r="U6" s="94"/>
+      <c r="V6" s="94"/>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
@@ -2092,26 +2098,26 @@
         <v>8</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="88" t="s">
+      <c r="G7" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="88"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="112" t="s">
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="112"/>
-      <c r="L7" s="112"/>
-      <c r="M7" s="112"/>
-      <c r="N7" s="112"/>
-      <c r="O7" s="112"/>
-      <c r="P7" s="112"/>
-      <c r="Q7" s="112"/>
-      <c r="R7" s="112"/>
-      <c r="S7" s="112"/>
-      <c r="T7" s="112"/>
-      <c r="U7" s="112"/>
-      <c r="V7" s="112"/>
+      <c r="K7" s="94"/>
+      <c r="L7" s="94"/>
+      <c r="M7" s="94"/>
+      <c r="N7" s="94"/>
+      <c r="O7" s="94"/>
+      <c r="P7" s="94"/>
+      <c r="Q7" s="94"/>
+      <c r="R7" s="94"/>
+      <c r="S7" s="94"/>
+      <c r="T7" s="94"/>
+      <c r="U7" s="94"/>
+      <c r="V7" s="94"/>
     </row>
     <row r="8" spans="1:36" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="7"/>
@@ -2146,16 +2152,16 @@
         <v>11</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="88" t="s">
+      <c r="G9" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="88"/>
-      <c r="I9" s="88"/>
-      <c r="J9" s="112" t="s">
+      <c r="H9" s="93"/>
+      <c r="I9" s="93"/>
+      <c r="J9" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="112"/>
-      <c r="L9" s="112"/>
+      <c r="K9" s="94"/>
+      <c r="L9" s="94"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -2189,16 +2195,16 @@
         <v>14</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="88" t="s">
+      <c r="G11" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="112" t="s">
+      <c r="H11" s="93"/>
+      <c r="I11" s="93"/>
+      <c r="J11" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="112"/>
-      <c r="L11" s="112"/>
+      <c r="K11" s="94"/>
+      <c r="L11" s="94"/>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:36" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2219,16 +2225,16 @@
         <v>17</v>
       </c>
       <c r="F13" s="7"/>
-      <c r="G13" s="88" t="s">
+      <c r="G13" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="88"/>
-      <c r="I13" s="88"/>
-      <c r="J13" s="112" t="s">
+      <c r="H13" s="93"/>
+      <c r="I13" s="93"/>
+      <c r="J13" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="112"/>
-      <c r="L13" s="112"/>
+      <c r="K13" s="94"/>
+      <c r="L13" s="94"/>
       <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:36" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2239,103 +2245,103 @@
       <c r="M14"/>
     </row>
     <row r="15" spans="1:36" s="39" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="92" t="s">
+      <c r="A15" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="95" t="s">
+      <c r="B15" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="96"/>
-      <c r="D15" s="125" t="s">
+      <c r="C15" s="107"/>
+      <c r="D15" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="125"/>
-      <c r="F15" s="125"/>
-      <c r="G15" s="125"/>
-      <c r="H15" s="125"/>
-      <c r="I15" s="125"/>
-      <c r="J15" s="125"/>
-      <c r="K15" s="125"/>
-      <c r="L15" s="125"/>
-      <c r="M15" s="126"/>
-      <c r="N15" s="109" t="s">
+      <c r="E15" s="95"/>
+      <c r="F15" s="95"/>
+      <c r="G15" s="95"/>
+      <c r="H15" s="95"/>
+      <c r="I15" s="95"/>
+      <c r="J15" s="95"/>
+      <c r="K15" s="95"/>
+      <c r="L15" s="95"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="110"/>
-      <c r="P15" s="110"/>
-      <c r="Q15" s="110"/>
-      <c r="R15" s="110"/>
-      <c r="S15" s="110"/>
-      <c r="T15" s="110"/>
-      <c r="U15" s="110"/>
-      <c r="V15" s="110"/>
-      <c r="W15" s="123"/>
-      <c r="X15" s="110" t="s">
+      <c r="O15" s="91"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
+      <c r="R15" s="91"/>
+      <c r="S15" s="91"/>
+      <c r="T15" s="91"/>
+      <c r="U15" s="91"/>
+      <c r="V15" s="91"/>
+      <c r="W15" s="92"/>
+      <c r="X15" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="Y15" s="110"/>
-      <c r="Z15" s="123"/>
-      <c r="AA15" s="80" t="s">
+      <c r="Y15" s="91"/>
+      <c r="Z15" s="92"/>
+      <c r="AA15" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="AB15" s="80"/>
-      <c r="AC15" s="80"/>
-      <c r="AD15" s="81"/>
+      <c r="AB15" s="119"/>
+      <c r="AC15" s="119"/>
+      <c r="AD15" s="120"/>
     </row>
     <row r="16" spans="1:36" s="39" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="93"/>
-      <c r="B16" s="97"/>
-      <c r="C16" s="98"/>
-      <c r="D16" s="127"/>
-      <c r="E16" s="127"/>
-      <c r="F16" s="127"/>
-      <c r="G16" s="127"/>
-      <c r="H16" s="127"/>
-      <c r="I16" s="127"/>
-      <c r="J16" s="127"/>
-      <c r="K16" s="127"/>
-      <c r="L16" s="127"/>
-      <c r="M16" s="128"/>
-      <c r="N16" s="109" t="s">
+      <c r="A16" s="104"/>
+      <c r="B16" s="108"/>
+      <c r="C16" s="109"/>
+      <c r="D16" s="97"/>
+      <c r="E16" s="97"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="97"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="97"/>
+      <c r="K16" s="97"/>
+      <c r="L16" s="97"/>
+      <c r="M16" s="98"/>
+      <c r="N16" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="O16" s="110"/>
-      <c r="P16" s="110"/>
-      <c r="Q16" s="111"/>
-      <c r="R16" s="109" t="s">
+      <c r="O16" s="91"/>
+      <c r="P16" s="91"/>
+      <c r="Q16" s="118"/>
+      <c r="R16" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="S16" s="110"/>
-      <c r="T16" s="110"/>
-      <c r="U16" s="111"/>
-      <c r="V16" s="107" t="s">
+      <c r="S16" s="91"/>
+      <c r="T16" s="91"/>
+      <c r="U16" s="118"/>
+      <c r="V16" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="W16" s="99" t="s">
+      <c r="W16" s="110" t="s">
         <v>62</v>
       </c>
-      <c r="X16" s="119" t="s">
+      <c r="X16" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="Y16" s="121" t="s">
+      <c r="Y16" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="Z16" s="86" t="s">
+      <c r="Z16" s="125" t="s">
         <v>53</v>
       </c>
-      <c r="AA16" s="82" t="s">
+      <c r="AA16" s="121" t="s">
         <v>61</v>
       </c>
-      <c r="AB16" s="83"/>
-      <c r="AC16" s="84" t="s">
+      <c r="AB16" s="122"/>
+      <c r="AC16" s="123" t="s">
         <v>57</v>
       </c>
-      <c r="AD16" s="84" t="s">
+      <c r="AD16" s="123" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:30" s="44" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="94"/>
+      <c r="A17" s="105"/>
       <c r="B17" s="41" t="s">
         <v>28</v>
       </c>
@@ -2396,19 +2402,19 @@
       <c r="U17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V17" s="108"/>
-      <c r="W17" s="100"/>
-      <c r="X17" s="120"/>
-      <c r="Y17" s="122"/>
-      <c r="Z17" s="87"/>
+      <c r="V17" s="117"/>
+      <c r="W17" s="111"/>
+      <c r="X17" s="88"/>
+      <c r="Y17" s="90"/>
+      <c r="Z17" s="126"/>
       <c r="AA17" s="49" t="s">
         <v>59</v>
       </c>
       <c r="AB17" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="AC17" s="85"/>
-      <c r="AD17" s="85"/>
+      <c r="AC17" s="124"/>
+      <c r="AD17" s="124"/>
     </row>
     <row r="18" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -2449,19 +2455,19 @@
       <c r="AD18" s="47"/>
     </row>
     <row r="19" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="124" t="s">
+      <c r="A19" s="129" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="124"/>
-      <c r="C19" s="124"/>
-      <c r="D19" s="124"/>
-      <c r="E19" s="124"/>
+      <c r="B19" s="129"/>
+      <c r="C19" s="129"/>
+      <c r="D19" s="129"/>
+      <c r="E19" s="129"/>
       <c r="F19" s="36"/>
       <c r="H19" s="11"/>
-      <c r="L19" s="105" t="s">
+      <c r="L19" s="115" t="s">
         <v>49</v>
       </c>
-      <c r="M19" s="105"/>
+      <c r="M19" s="115"/>
       <c r="N19" s="64"/>
       <c r="O19" s="65"/>
       <c r="P19" s="66"/>
@@ -2481,63 +2487,69 @@
       <c r="AD19" s="47"/>
     </row>
     <row r="20" spans="1:30" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="101" t="s">
+      <c r="A20" s="130" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="101"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="101"/>
+      <c r="B20" s="130"/>
+      <c r="C20" s="130"/>
+      <c r="D20" s="130"/>
+      <c r="E20" s="130"/>
       <c r="H20" s="11"/>
-      <c r="L20" s="106" t="s">
+      <c r="L20" s="86" t="s">
         <v>50</v>
       </c>
-      <c r="M20" s="106"/>
-      <c r="N20" s="102"/>
-      <c r="O20" s="103"/>
-      <c r="P20" s="103"/>
-      <c r="Q20" s="103"/>
-      <c r="R20" s="103"/>
-      <c r="S20" s="103"/>
-      <c r="T20" s="103"/>
-      <c r="U20" s="103"/>
-      <c r="V20" s="104"/>
+      <c r="M20" s="86"/>
+      <c r="N20" s="112"/>
+      <c r="O20" s="113"/>
+      <c r="P20" s="113"/>
+      <c r="Q20" s="113"/>
+      <c r="R20" s="113"/>
+      <c r="S20" s="113"/>
+      <c r="T20" s="113"/>
+      <c r="U20" s="113"/>
+      <c r="V20" s="114"/>
       <c r="W20" s="67"/>
     </row>
     <row r="21" spans="1:30" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+      <c r="A21" s="131" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="131"/>
+      <c r="C21" s="131"/>
+      <c r="D21" s="131"/>
+      <c r="E21" s="131"/>
       <c r="H21" s="11"/>
-      <c r="L21" s="106" t="s">
+      <c r="L21" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="M21" s="106"/>
-      <c r="N21" s="89"/>
-      <c r="O21" s="90"/>
-      <c r="P21" s="90"/>
-      <c r="Q21" s="90"/>
-      <c r="R21" s="90"/>
-      <c r="S21" s="90"/>
-      <c r="T21" s="90"/>
-      <c r="U21" s="90"/>
-      <c r="V21" s="90"/>
-      <c r="W21" s="91"/>
+      <c r="M21" s="86"/>
+      <c r="N21" s="100"/>
+      <c r="O21" s="101"/>
+      <c r="P21" s="101"/>
+      <c r="Q21" s="101"/>
+      <c r="R21" s="101"/>
+      <c r="S21" s="101"/>
+      <c r="T21" s="101"/>
+      <c r="U21" s="101"/>
+      <c r="V21" s="101"/>
+      <c r="W21" s="102"/>
     </row>
     <row r="22" spans="1:30" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="H22" s="11"/>
-      <c r="L22" s="106" t="s">
+      <c r="L22" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="M22" s="106"/>
-      <c r="N22" s="89"/>
-      <c r="O22" s="90"/>
-      <c r="P22" s="90"/>
-      <c r="Q22" s="90"/>
-      <c r="R22" s="90"/>
-      <c r="S22" s="90"/>
-      <c r="T22" s="90"/>
-      <c r="U22" s="90"/>
-      <c r="V22" s="91"/>
+      <c r="M22" s="86"/>
+      <c r="N22" s="100"/>
+      <c r="O22" s="101"/>
+      <c r="P22" s="101"/>
+      <c r="Q22" s="101"/>
+      <c r="R22" s="101"/>
+      <c r="S22" s="101"/>
+      <c r="T22" s="101"/>
+      <c r="U22" s="101"/>
+      <c r="V22" s="102"/>
       <c r="W22" s="67"/>
     </row>
     <row r="23" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2554,9 +2566,9 @@
       <c r="AA24" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="AB24" s="114"/>
-      <c r="AC24" s="115"/>
-      <c r="AD24" s="116"/>
+      <c r="AB24" s="81"/>
+      <c r="AC24" s="82"/>
+      <c r="AD24" s="83"/>
     </row>
     <row r="25" spans="1:30" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
@@ -2570,21 +2582,49 @@
       <c r="AA25" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="AB25" s="114"/>
-      <c r="AC25" s="115"/>
-      <c r="AD25" s="116"/>
+      <c r="AB25" s="81"/>
+      <c r="AC25" s="82"/>
+      <c r="AD25" s="83"/>
     </row>
     <row r="27" spans="1:30" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="113" t="s">
+      <c r="A27" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="113"/>
-      <c r="C27" s="113"/>
-      <c r="D27" s="113"/>
-      <c r="E27" s="113"/>
+      <c r="B27" s="80"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="44">
+    <mergeCell ref="AA15:AD15"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="AC16:AC17"/>
+    <mergeCell ref="AD16:AD17"/>
+    <mergeCell ref="Z16:Z17"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="N22:V22"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="N20:V20"/>
+    <mergeCell ref="N21:W21"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="R16:U16"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J6:V6"/>
+    <mergeCell ref="J7:V7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J9:L9"/>
     <mergeCell ref="A27:E27"/>
     <mergeCell ref="AB25:AD25"/>
     <mergeCell ref="A1:AD1"/>
@@ -2601,33 +2641,6 @@
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="D15:M16"/>
     <mergeCell ref="N15:W15"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J6:V6"/>
-    <mergeCell ref="J7:V7"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="N22:V22"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="W16:W17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="N20:V20"/>
-    <mergeCell ref="N21:W21"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="V16:V17"/>
-    <mergeCell ref="R16:U16"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="AA15:AD15"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="AC16:AC17"/>
-    <mergeCell ref="AD16:AD17"/>
-    <mergeCell ref="Z16:Z17"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2660,15 +2673,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="127" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
       <c r="H1" s="62"/>
       <c r="I1" s="62"/>
       <c r="J1" s="62"/>
@@ -2707,15 +2720,15 @@
       <c r="BA1" s="1"/>
     </row>
     <row r="2" spans="1:53" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="128" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="130"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
-      <c r="F2" s="130"/>
-      <c r="G2" s="130"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
       <c r="H2" s="63"/>
       <c r="I2" s="63"/>
       <c r="J2" s="63"/>
@@ -2736,15 +2749,15 @@
       <c r="Y2" s="63"/>
     </row>
     <row r="3" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="128" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="130"/>
-      <c r="C3" s="130"/>
-      <c r="D3" s="130"/>
-      <c r="E3" s="130"/>
-      <c r="F3" s="130"/>
-      <c r="G3" s="130"/>
+      <c r="B3" s="128"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
       <c r="H3" s="63"/>
       <c r="I3" s="63"/>
       <c r="J3" s="63"/>
@@ -3035,17 +3048,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B7BBE98651F7A43AC7BF2F06836443C" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b51c7281b06024c9ff887df9fe3bb465">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8103b6e4-b1cc-417b-af38-f980b3f4bdef" xmlns:ns3="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c056a6abdadb071051b2c083c327215c" ns2:_="" ns3:_="">
     <xsd:import namespace="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
@@ -3262,6 +3264,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
   <ds:schemaRefs>
@@ -3271,17 +3284,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
-    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E02BC65-B354-4988-8893-F98AC7F212AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3298,4 +3300,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
+    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: typo dans modèle MCCC xlsx
</commit_message>
<xml_diff>
--- a/public/modeles/Annexe_MCCC.xlsx
+++ b/public/modeles/Annexe_MCCC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/oreof/public/modeles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959C0692-D7ED-A242-B951-9528CE2D1749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5006EE-A3F6-1B40-B7C3-2DEA36A2222D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1273,6 +1273,105 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1291,9 +1390,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1306,127 +1402,31 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1899,8 +1899,8 @@
   </sheetPr>
   <dimension ref="A1:AJ27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="116" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:E20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="116" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1929,38 +1929,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="117"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+      <c r="Q1" s="117"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
+      <c r="W1" s="117"/>
+      <c r="X1" s="117"/>
+      <c r="Y1" s="117"/>
+      <c r="Z1" s="117"/>
+      <c r="AA1" s="117"/>
+      <c r="AB1" s="117"/>
+      <c r="AC1" s="117"/>
+      <c r="AD1" s="117"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
@@ -1969,87 +1969,87 @@
       <c r="AJ1" s="1"/>
     </row>
     <row r="2" spans="1:36" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="85"/>
-      <c r="U2" s="85"/>
-      <c r="V2" s="85"/>
-      <c r="W2" s="85"/>
-      <c r="X2" s="85"/>
-      <c r="Y2" s="85"/>
-      <c r="Z2" s="85"/>
-      <c r="AA2" s="85"/>
-      <c r="AB2" s="85"/>
-      <c r="AC2" s="85"/>
-      <c r="AD2" s="85"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="118"/>
+      <c r="O2" s="118"/>
+      <c r="P2" s="118"/>
+      <c r="Q2" s="118"/>
+      <c r="R2" s="118"/>
+      <c r="S2" s="118"/>
+      <c r="T2" s="118"/>
+      <c r="U2" s="118"/>
+      <c r="V2" s="118"/>
+      <c r="W2" s="118"/>
+      <c r="X2" s="118"/>
+      <c r="Y2" s="118"/>
+      <c r="Z2" s="118"/>
+      <c r="AA2" s="118"/>
+      <c r="AB2" s="118"/>
+      <c r="AC2" s="118"/>
+      <c r="AD2" s="118"/>
     </row>
     <row r="3" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="85"/>
-      <c r="T3" s="85"/>
-      <c r="U3" s="85"/>
-      <c r="V3" s="85"/>
-      <c r="W3" s="85"/>
-      <c r="X3" s="85"/>
-      <c r="Y3" s="85"/>
-      <c r="Z3" s="85"/>
-      <c r="AA3" s="85"/>
-      <c r="AB3" s="85"/>
-      <c r="AC3" s="85"/>
-      <c r="AD3" s="85"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="118"/>
+      <c r="O3" s="118"/>
+      <c r="P3" s="118"/>
+      <c r="Q3" s="118"/>
+      <c r="R3" s="118"/>
+      <c r="S3" s="118"/>
+      <c r="T3" s="118"/>
+      <c r="U3" s="118"/>
+      <c r="V3" s="118"/>
+      <c r="W3" s="118"/>
+      <c r="X3" s="118"/>
+      <c r="Y3" s="118"/>
+      <c r="Z3" s="118"/>
+      <c r="AA3" s="118"/>
+      <c r="AB3" s="118"/>
+      <c r="AC3" s="118"/>
+      <c r="AD3" s="118"/>
     </row>
     <row r="4" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="93" t="s">
+      <c r="G5" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94" t="s">
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="94"/>
-      <c r="L5" s="94"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="112"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -2063,26 +2063,26 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="93" t="s">
+      <c r="G6" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94" t="s">
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="94"/>
-      <c r="L6" s="94"/>
-      <c r="M6" s="94"/>
-      <c r="N6" s="94"/>
-      <c r="O6" s="94"/>
-      <c r="P6" s="94"/>
-      <c r="Q6" s="94"/>
-      <c r="R6" s="94"/>
-      <c r="S6" s="94"/>
-      <c r="T6" s="94"/>
-      <c r="U6" s="94"/>
-      <c r="V6" s="94"/>
+      <c r="K6" s="112"/>
+      <c r="L6" s="112"/>
+      <c r="M6" s="112"/>
+      <c r="N6" s="112"/>
+      <c r="O6" s="112"/>
+      <c r="P6" s="112"/>
+      <c r="Q6" s="112"/>
+      <c r="R6" s="112"/>
+      <c r="S6" s="112"/>
+      <c r="T6" s="112"/>
+      <c r="U6" s="112"/>
+      <c r="V6" s="112"/>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
@@ -2098,26 +2098,26 @@
         <v>8</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="93" t="s">
+      <c r="G7" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="94" t="s">
+      <c r="H7" s="88"/>
+      <c r="I7" s="88"/>
+      <c r="J7" s="112" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="94"/>
-      <c r="N7" s="94"/>
-      <c r="O7" s="94"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="94"/>
-      <c r="R7" s="94"/>
-      <c r="S7" s="94"/>
-      <c r="T7" s="94"/>
-      <c r="U7" s="94"/>
-      <c r="V7" s="94"/>
+      <c r="K7" s="112"/>
+      <c r="L7" s="112"/>
+      <c r="M7" s="112"/>
+      <c r="N7" s="112"/>
+      <c r="O7" s="112"/>
+      <c r="P7" s="112"/>
+      <c r="Q7" s="112"/>
+      <c r="R7" s="112"/>
+      <c r="S7" s="112"/>
+      <c r="T7" s="112"/>
+      <c r="U7" s="112"/>
+      <c r="V7" s="112"/>
     </row>
     <row r="8" spans="1:36" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="7"/>
@@ -2152,16 +2152,16 @@
         <v>11</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="93" t="s">
+      <c r="G9" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94" t="s">
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
+      <c r="K9" s="112"/>
+      <c r="L9" s="112"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -2195,16 +2195,16 @@
         <v>14</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="93" t="s">
+      <c r="G11" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="93"/>
-      <c r="I11" s="93"/>
-      <c r="J11" s="94" t="s">
+      <c r="H11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="94"/>
-      <c r="L11" s="94"/>
+      <c r="K11" s="112"/>
+      <c r="L11" s="112"/>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:36" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2225,16 +2225,16 @@
         <v>17</v>
       </c>
       <c r="F13" s="7"/>
-      <c r="G13" s="93" t="s">
+      <c r="G13" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
-      <c r="J13" s="94" t="s">
+      <c r="H13" s="88"/>
+      <c r="I13" s="88"/>
+      <c r="J13" s="112" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="94"/>
-      <c r="L13" s="94"/>
+      <c r="K13" s="112"/>
+      <c r="L13" s="112"/>
       <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:36" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2245,103 +2245,103 @@
       <c r="M14"/>
     </row>
     <row r="15" spans="1:36" s="39" customFormat="1" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="103" t="s">
+      <c r="A15" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="106" t="s">
+      <c r="B15" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="107"/>
-      <c r="D15" s="95" t="s">
+      <c r="C15" s="96"/>
+      <c r="D15" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="95"/>
-      <c r="F15" s="95"/>
-      <c r="G15" s="95"/>
-      <c r="H15" s="95"/>
-      <c r="I15" s="95"/>
-      <c r="J15" s="95"/>
-      <c r="K15" s="95"/>
-      <c r="L15" s="95"/>
-      <c r="M15" s="96"/>
-      <c r="N15" s="99" t="s">
+      <c r="E15" s="125"/>
+      <c r="F15" s="125"/>
+      <c r="G15" s="125"/>
+      <c r="H15" s="125"/>
+      <c r="I15" s="125"/>
+      <c r="J15" s="125"/>
+      <c r="K15" s="125"/>
+      <c r="L15" s="125"/>
+      <c r="M15" s="126"/>
+      <c r="N15" s="109" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="91"/>
-      <c r="P15" s="91"/>
-      <c r="Q15" s="91"/>
-      <c r="R15" s="91"/>
-      <c r="S15" s="91"/>
-      <c r="T15" s="91"/>
-      <c r="U15" s="91"/>
-      <c r="V15" s="91"/>
-      <c r="W15" s="92"/>
-      <c r="X15" s="91" t="s">
+      <c r="O15" s="110"/>
+      <c r="P15" s="110"/>
+      <c r="Q15" s="110"/>
+      <c r="R15" s="110"/>
+      <c r="S15" s="110"/>
+      <c r="T15" s="110"/>
+      <c r="U15" s="110"/>
+      <c r="V15" s="110"/>
+      <c r="W15" s="123"/>
+      <c r="X15" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="Y15" s="91"/>
-      <c r="Z15" s="92"/>
-      <c r="AA15" s="119" t="s">
+      <c r="Y15" s="110"/>
+      <c r="Z15" s="123"/>
+      <c r="AA15" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="AB15" s="119"/>
-      <c r="AC15" s="119"/>
-      <c r="AD15" s="120"/>
+      <c r="AB15" s="80"/>
+      <c r="AC15" s="80"/>
+      <c r="AD15" s="81"/>
     </row>
     <row r="16" spans="1:36" s="39" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="104"/>
-      <c r="B16" s="108"/>
-      <c r="C16" s="109"/>
-      <c r="D16" s="97"/>
-      <c r="E16" s="97"/>
-      <c r="F16" s="97"/>
-      <c r="G16" s="97"/>
-      <c r="H16" s="97"/>
-      <c r="I16" s="97"/>
-      <c r="J16" s="97"/>
-      <c r="K16" s="97"/>
-      <c r="L16" s="97"/>
-      <c r="M16" s="98"/>
-      <c r="N16" s="99" t="s">
+      <c r="A16" s="93"/>
+      <c r="B16" s="97"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="127"/>
+      <c r="E16" s="127"/>
+      <c r="F16" s="127"/>
+      <c r="G16" s="127"/>
+      <c r="H16" s="127"/>
+      <c r="I16" s="127"/>
+      <c r="J16" s="127"/>
+      <c r="K16" s="127"/>
+      <c r="L16" s="127"/>
+      <c r="M16" s="128"/>
+      <c r="N16" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="O16" s="91"/>
-      <c r="P16" s="91"/>
-      <c r="Q16" s="118"/>
-      <c r="R16" s="99" t="s">
+      <c r="O16" s="110"/>
+      <c r="P16" s="110"/>
+      <c r="Q16" s="111"/>
+      <c r="R16" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="S16" s="91"/>
-      <c r="T16" s="91"/>
-      <c r="U16" s="118"/>
-      <c r="V16" s="116" t="s">
+      <c r="S16" s="110"/>
+      <c r="T16" s="110"/>
+      <c r="U16" s="111"/>
+      <c r="V16" s="107" t="s">
         <v>27</v>
       </c>
-      <c r="W16" s="110" t="s">
+      <c r="W16" s="99" t="s">
         <v>62</v>
       </c>
-      <c r="X16" s="87" t="s">
+      <c r="X16" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="Y16" s="89" t="s">
+      <c r="Y16" s="121" t="s">
         <v>52</v>
       </c>
-      <c r="Z16" s="125" t="s">
+      <c r="Z16" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="AA16" s="121" t="s">
+      <c r="AA16" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="AB16" s="122"/>
-      <c r="AC16" s="123" t="s">
+      <c r="AB16" s="83"/>
+      <c r="AC16" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="AD16" s="123" t="s">
+      <c r="AD16" s="84" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:30" s="44" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="105"/>
+      <c r="A17" s="94"/>
       <c r="B17" s="41" t="s">
         <v>28</v>
       </c>
@@ -2402,19 +2402,19 @@
       <c r="U17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V17" s="117"/>
-      <c r="W17" s="111"/>
-      <c r="X17" s="88"/>
-      <c r="Y17" s="90"/>
-      <c r="Z17" s="126"/>
+      <c r="V17" s="108"/>
+      <c r="W17" s="100"/>
+      <c r="X17" s="120"/>
+      <c r="Y17" s="122"/>
+      <c r="Z17" s="87"/>
       <c r="AA17" s="49" t="s">
         <v>59</v>
       </c>
       <c r="AB17" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="AC17" s="124"/>
-      <c r="AD17" s="124"/>
+      <c r="AC17" s="85"/>
+      <c r="AD17" s="85"/>
     </row>
     <row r="18" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -2455,19 +2455,19 @@
       <c r="AD18" s="47"/>
     </row>
     <row r="19" spans="1:30" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="129" t="s">
+      <c r="A19" s="124" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="129"/>
-      <c r="C19" s="129"/>
-      <c r="D19" s="129"/>
-      <c r="E19" s="129"/>
+      <c r="B19" s="124"/>
+      <c r="C19" s="124"/>
+      <c r="D19" s="124"/>
+      <c r="E19" s="124"/>
       <c r="F19" s="36"/>
       <c r="H19" s="11"/>
-      <c r="L19" s="115" t="s">
+      <c r="L19" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="M19" s="115"/>
+      <c r="M19" s="105"/>
       <c r="N19" s="64"/>
       <c r="O19" s="65"/>
       <c r="P19" s="66"/>
@@ -2487,27 +2487,27 @@
       <c r="AD19" s="47"/>
     </row>
     <row r="20" spans="1:30" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="130" t="s">
+      <c r="A20" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="130"/>
-      <c r="C20" s="130"/>
-      <c r="D20" s="130"/>
-      <c r="E20" s="130"/>
+      <c r="B20" s="101"/>
+      <c r="C20" s="101"/>
+      <c r="D20" s="101"/>
+      <c r="E20" s="101"/>
       <c r="H20" s="11"/>
-      <c r="L20" s="86" t="s">
+      <c r="L20" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="M20" s="86"/>
-      <c r="N20" s="112"/>
-      <c r="O20" s="113"/>
-      <c r="P20" s="113"/>
-      <c r="Q20" s="113"/>
-      <c r="R20" s="113"/>
-      <c r="S20" s="113"/>
-      <c r="T20" s="113"/>
-      <c r="U20" s="113"/>
-      <c r="V20" s="114"/>
+      <c r="M20" s="106"/>
+      <c r="N20" s="102"/>
+      <c r="O20" s="103"/>
+      <c r="P20" s="103"/>
+      <c r="Q20" s="103"/>
+      <c r="R20" s="103"/>
+      <c r="S20" s="103"/>
+      <c r="T20" s="103"/>
+      <c r="U20" s="103"/>
+      <c r="V20" s="104"/>
       <c r="W20" s="67"/>
     </row>
     <row r="21" spans="1:30" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2519,37 +2519,37 @@
       <c r="D21" s="131"/>
       <c r="E21" s="131"/>
       <c r="H21" s="11"/>
-      <c r="L21" s="86" t="s">
+      <c r="L21" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="M21" s="86"/>
-      <c r="N21" s="100"/>
-      <c r="O21" s="101"/>
-      <c r="P21" s="101"/>
-      <c r="Q21" s="101"/>
-      <c r="R21" s="101"/>
-      <c r="S21" s="101"/>
-      <c r="T21" s="101"/>
-      <c r="U21" s="101"/>
-      <c r="V21" s="101"/>
-      <c r="W21" s="102"/>
+      <c r="M21" s="106"/>
+      <c r="N21" s="89"/>
+      <c r="O21" s="90"/>
+      <c r="P21" s="90"/>
+      <c r="Q21" s="90"/>
+      <c r="R21" s="90"/>
+      <c r="S21" s="90"/>
+      <c r="T21" s="90"/>
+      <c r="U21" s="90"/>
+      <c r="V21" s="90"/>
+      <c r="W21" s="91"/>
     </row>
     <row r="22" spans="1:30" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="H22" s="11"/>
-      <c r="L22" s="86" t="s">
+      <c r="L22" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="M22" s="86"/>
-      <c r="N22" s="100"/>
-      <c r="O22" s="101"/>
-      <c r="P22" s="101"/>
-      <c r="Q22" s="101"/>
-      <c r="R22" s="101"/>
-      <c r="S22" s="101"/>
-      <c r="T22" s="101"/>
-      <c r="U22" s="101"/>
-      <c r="V22" s="102"/>
+      <c r="M22" s="106"/>
+      <c r="N22" s="89"/>
+      <c r="O22" s="90"/>
+      <c r="P22" s="90"/>
+      <c r="Q22" s="90"/>
+      <c r="R22" s="90"/>
+      <c r="S22" s="90"/>
+      <c r="T22" s="90"/>
+      <c r="U22" s="90"/>
+      <c r="V22" s="91"/>
       <c r="W22" s="67"/>
     </row>
     <row r="23" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2566,9 +2566,9 @@
       <c r="AA24" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="AB24" s="81"/>
-      <c r="AC24" s="82"/>
-      <c r="AD24" s="83"/>
+      <c r="AB24" s="114"/>
+      <c r="AC24" s="115"/>
+      <c r="AD24" s="116"/>
     </row>
     <row r="25" spans="1:30" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
@@ -2582,49 +2582,21 @@
       <c r="AA25" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="AB25" s="81"/>
-      <c r="AC25" s="82"/>
-      <c r="AD25" s="83"/>
+      <c r="AB25" s="114"/>
+      <c r="AC25" s="115"/>
+      <c r="AD25" s="116"/>
     </row>
     <row r="27" spans="1:30" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="80" t="s">
+      <c r="A27" s="113" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="80"/>
-      <c r="C27" s="80"/>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
+      <c r="B27" s="113"/>
+      <c r="C27" s="113"/>
+      <c r="D27" s="113"/>
+      <c r="E27" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="AA15:AD15"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="AC16:AC17"/>
-    <mergeCell ref="AD16:AD17"/>
-    <mergeCell ref="Z16:Z17"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="N22:V22"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="W16:W17"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="N20:V20"/>
-    <mergeCell ref="N21:W21"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="V16:V17"/>
-    <mergeCell ref="R16:U16"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J6:V6"/>
-    <mergeCell ref="J7:V7"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J9:L9"/>
     <mergeCell ref="A27:E27"/>
     <mergeCell ref="AB25:AD25"/>
     <mergeCell ref="A1:AD1"/>
@@ -2641,6 +2613,34 @@
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="D15:M16"/>
     <mergeCell ref="N15:W15"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J6:V6"/>
+    <mergeCell ref="J7:V7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="N22:V22"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="N20:V20"/>
+    <mergeCell ref="N21:W21"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="R16:U16"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="AA15:AD15"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="AC16:AC17"/>
+    <mergeCell ref="AD16:AD17"/>
+    <mergeCell ref="Z16:Z17"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2673,15 +2673,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
       <c r="H1" s="62"/>
       <c r="I1" s="62"/>
       <c r="J1" s="62"/>
@@ -2720,15 +2720,15 @@
       <c r="BA1" s="1"/>
     </row>
     <row r="2" spans="1:53" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="130" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="130"/>
       <c r="H2" s="63"/>
       <c r="I2" s="63"/>
       <c r="J2" s="63"/>
@@ -2749,15 +2749,15 @@
       <c r="Y2" s="63"/>
     </row>
     <row r="3" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="130" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="128"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
+      <c r="B3" s="130"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
       <c r="H3" s="63"/>
       <c r="I3" s="63"/>
       <c r="J3" s="63"/>
@@ -3048,6 +3048,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B7BBE98651F7A43AC7BF2F06836443C" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b51c7281b06024c9ff887df9fe3bb465">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8103b6e4-b1cc-417b-af38-f980b3f4bdef" xmlns:ns3="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c056a6abdadb071051b2c083c327215c" ns2:_="" ns3:_="">
     <xsd:import namespace="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
@@ -3264,17 +3275,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="026a8ae5-d6a9-4af7-bf98-fe61cc11d283" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8103b6e4-b1cc-417b-af38-f980b3f4bdef">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD87B94F-381C-458D-A5C9-64DD7F51B7FF}">
   <ds:schemaRefs>
@@ -3284,6 +3284,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
+    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E02BC65-B354-4988-8893-F98AC7F212AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3300,15 +3311,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9C2EEE-EA72-4039-9998-752A033046FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="026a8ae5-d6a9-4af7-bf98-fe61cc11d283"/>
-    <ds:schemaRef ds:uri="8103b6e4-b1cc-417b-af38-f980b3f4bdef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>